<commit_message>
revised algorithm, not working yet
</commit_message>
<xml_diff>
--- a/Data/Lgas_10_10/analysis.xlsx
+++ b/Data/Lgas_10_10/analysis.xlsx
@@ -9,14 +9,13 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="3100" yWindow="2140" windowWidth="25600" windowHeight="10040" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="2140" windowWidth="25600" windowHeight="10040" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="SUSWeight_function" localSheetId="0">Sheet1!#REF!</definedName>
-    <definedName name="SUSWeight_function_1" localSheetId="0">Sheet1!$B$2:$B$102</definedName>
+    <definedName name="SUSWeight_function" localSheetId="0">Sheet1!$B$2:$B$102</definedName>
     <definedName name="Weight_function_1" localSheetId="0">Sheet1!#REF!</definedName>
     <definedName name="Weight_function_2" localSheetId="0">Sheet1!#REF!</definedName>
   </definedNames>
@@ -39,7 +38,7 @@
     </textPr>
   </connection>
   <connection id="2" name="SUSWeight_function1" type="6" refreshedVersion="0" background="1" saveData="1">
-    <textPr fileType="mac" codePage="10000" sourceFile="/Users/Yuding/Dropbox/SUS_2D/Data/Lgas_10_10/SUSWeight_function.txt">
+    <textPr fileType="mac" sourceFile="/Users/Yuding/Dropbox/SUS_2D/Data/Lgas_10_10/SUSWeight_function.txt">
       <textFields>
         <textField/>
       </textFields>
@@ -227,304 +226,304 @@
                   <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.01023208135447E-5</c:v>
+                  <c:v>0.00217155351350793</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.01227382007085E-5</c:v>
+                  <c:v>0.00535988393210267</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>6.8603809569166E-6</c:v>
+                  <c:v>0.00921733448272161</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>5.21445760507996E-6</c:v>
+                  <c:v>0.013593861089636</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>4.19791489561526E-6</c:v>
+                  <c:v>0.0184090803993526</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>3.54954184289185E-6</c:v>
+                  <c:v>0.0235840766512481</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>3.07531917962026E-6</c:v>
+                  <c:v>0.0290702600847431</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>2.71671581663645E-6</c:v>
+                  <c:v>0.0348272627480584</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>2.43632957208128E-6</c:v>
+                  <c:v>0.0408271902273382</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>2.21805966363066E-6</c:v>
+                  <c:v>0.0470471155075272</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>2.0406601534878E-6</c:v>
+                  <c:v>0.0534736737050751</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>1.88806600682637E-6</c:v>
+                  <c:v>0.0600884671972965</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>1.76498672282717E-6</c:v>
+                  <c:v>0.0668789612961371</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>1.6578318047546E-6</c:v>
+                  <c:v>0.0738324944431908</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>1.56667494400268E-6</c:v>
+                  <c:v>0.0809442178935088</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>1.4861789078024E-6</c:v>
+                  <c:v>0.0882036627415398</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>1.41296722418643E-6</c:v>
+                  <c:v>0.0956066310917906</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>1.35101086006113E-6</c:v>
+                  <c:v>0.10314592280126</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>1.29655692817377E-6</c:v>
+                  <c:v>0.110815890760507</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>1.24747931201368E-6</c:v>
+                  <c:v>0.118610897794628</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>1.20116152316256E-6</c:v>
+                  <c:v>0.12652820654724</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>1.16194018447594E-6</c:v>
+                  <c:v>0.134562865531754</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>1.12668121955215E-6</c:v>
+                  <c:v>0.142709575611685</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>1.0933173709318E-6</c:v>
+                  <c:v>0.150966448181399</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>1.06311218650523E-6</c:v>
+                  <c:v>0.159332045948284</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>1.03603806622083E-6</c:v>
+                  <c:v>0.167802724364665</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>1.01038524484521E-6</c:v>
+                  <c:v>0.17637566795473</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>9.87839205464925E-7</c:v>
+                  <c:v>0.185049159531407</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>9.68961733252916E-7</c:v>
+                  <c:v>0.193820102747784</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>9.49544527161952E-7</c:v>
+                  <c:v>0.202688090944586</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>9.31079190612546E-7</c:v>
+                  <c:v>0.211650139245864</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>9.14921035391304E-7</c:v>
+                  <c:v>0.220704947623271</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>8.98368069413061E-7</c:v>
+                  <c:v>0.229850438385688</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>8.86868012335373E-7</c:v>
+                  <c:v>0.239084522725128</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>8.74553595036951E-7</c:v>
+                  <c:v>0.248407357896666</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>8.63327115942438E-7</c:v>
+                  <c:v>0.25781765535015</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>8.52087422414622E-7</c:v>
+                  <c:v>0.267313565577113</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>8.42988004691359E-7</c:v>
+                  <c:v>0.27689376796074</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>8.3459600752784E-7</c:v>
+                  <c:v>0.286558191509196</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>8.28337423307156E-7</c:v>
+                  <c:v>0.296306454923557</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>8.21464877337437E-7</c:v>
+                  <c:v>0.306137951098381</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>8.15103210465075E-7</c:v>
+                  <c:v>0.316051216765052</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>8.09773971747898E-7</c:v>
+                  <c:v>0.326046118416911</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>8.05507415199551E-7</c:v>
+                  <c:v>0.336121331677857</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>8.01000609893609E-7</c:v>
+                  <c:v>0.346277395486609</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>7.9849914108589E-7</c:v>
+                  <c:v>0.356514270641318</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>7.95960025305249E-7</c:v>
+                  <c:v>0.366830823896544</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>7.93722291753524E-7</c:v>
+                  <c:v>0.377226506726489</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>7.92483138845691E-7</c:v>
+                  <c:v>0.387701816900506</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>7.92105245428775E-7</c:v>
+                  <c:v>0.398257143077766</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>7.91787265815937E-7</c:v>
+                  <c:v>0.408892115625185</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>7.93265178658044E-7</c:v>
+                  <c:v>0.419606772622226</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>7.93886124126593E-7</c:v>
+                  <c:v>0.430401786403432</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>7.95899208890678E-7</c:v>
+                  <c:v>0.441277755456894</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>7.97960731532401E-7</c:v>
+                  <c:v>0.4522341912173</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>8.02064514004982E-7</c:v>
+                  <c:v>0.463271353516599</c:v>
                 </c:pt>
                 <c:pt idx="57">
-                  <c:v>8.05639800972941E-7</c:v>
+                  <c:v>0.474389412147293</c:v>
                 </c:pt>
                 <c:pt idx="58">
-                  <c:v>8.11139541630782E-7</c:v>
+                  <c:v>0.485588860921686</c:v>
                 </c:pt>
                 <c:pt idx="59">
-                  <c:v>8.14987622353611E-7</c:v>
+                  <c:v>0.496870146105143</c:v>
                 </c:pt>
                 <c:pt idx="60">
-                  <c:v>8.21304979596055E-7</c:v>
+                  <c:v>0.508234601746501</c:v>
                 </c:pt>
                 <c:pt idx="61">
-                  <c:v>8.2756417648131E-7</c:v>
+                  <c:v>0.519682707896085</c:v>
                 </c:pt>
                 <c:pt idx="62">
-                  <c:v>8.35732233025168E-7</c:v>
+                  <c:v>0.531215077791243</c:v>
                 </c:pt>
                 <c:pt idx="63">
-                  <c:v>8.43538390408314E-7</c:v>
+                  <c:v>0.542832118106839</c:v>
                 </c:pt>
                 <c:pt idx="64">
-                  <c:v>8.5385612098126E-7</c:v>
+                  <c:v>0.55453460294763</c:v>
                 </c:pt>
                 <c:pt idx="65">
-                  <c:v>8.62886103763274E-7</c:v>
+                  <c:v>0.566323343017697</c:v>
                 </c:pt>
                 <c:pt idx="66">
-                  <c:v>8.74464882077615E-7</c:v>
+                  <c:v>0.578199991311635</c:v>
                 </c:pt>
                 <c:pt idx="67">
-                  <c:v>8.86617178759621E-7</c:v>
+                  <c:v>0.590166089044337</c:v>
                 </c:pt>
                 <c:pt idx="68">
-                  <c:v>9.00626250355779E-7</c:v>
+                  <c:v>0.602222289043173</c:v>
                 </c:pt>
                 <c:pt idx="69">
-                  <c:v>9.14884205330471E-7</c:v>
+                  <c:v>0.614370710188383</c:v>
                 </c:pt>
                 <c:pt idx="70">
-                  <c:v>9.32406583348273E-7</c:v>
+                  <c:v>0.626611693929114</c:v>
                 </c:pt>
                 <c:pt idx="71">
-                  <c:v>9.48964229236864E-7</c:v>
+                  <c:v>0.638948568737666</c:v>
                 </c:pt>
                 <c:pt idx="72">
-                  <c:v>9.67855112197311E-7</c:v>
+                  <c:v>0.65138271507978</c:v>
                 </c:pt>
                 <c:pt idx="73">
-                  <c:v>9.88202346178902E-7</c:v>
+                  <c:v>0.663916497749382</c:v>
                 </c:pt>
                 <c:pt idx="74">
-                  <c:v>1.01116477582975E-6</c:v>
+                  <c:v>0.67655073749878</c:v>
                 </c:pt>
                 <c:pt idx="75">
-                  <c:v>1.03686092426012E-6</c:v>
+                  <c:v>0.689287462516012</c:v>
                 </c:pt>
                 <c:pt idx="76">
-                  <c:v>1.0622877748431E-6</c:v>
+                  <c:v>0.702129633834812</c:v>
                 </c:pt>
                 <c:pt idx="77">
-                  <c:v>1.0966998655094E-6</c:v>
+                  <c:v>0.715081785907091</c:v>
                 </c:pt>
                 <c:pt idx="78">
-                  <c:v>1.12496758691383E-6</c:v>
+                  <c:v>0.728147169027444</c:v>
                 </c:pt>
                 <c:pt idx="79">
-                  <c:v>1.16308349725687E-6</c:v>
+                  <c:v>0.741329231454855</c:v>
                 </c:pt>
                 <c:pt idx="80">
-                  <c:v>1.20292720308515E-6</c:v>
+                  <c:v>0.754633148509846</c:v>
                 </c:pt>
                 <c:pt idx="81">
-                  <c:v>1.2484293197885E-6</c:v>
+                  <c:v>0.768064478446452</c:v>
                 </c:pt>
                 <c:pt idx="82">
-                  <c:v>1.29768926959111E-6</c:v>
+                  <c:v>0.781624898940262</c:v>
                 </c:pt>
                 <c:pt idx="83">
-                  <c:v>1.35212882538034E-6</c:v>
+                  <c:v>0.795323279012136</c:v>
                 </c:pt>
                 <c:pt idx="84">
-                  <c:v>1.41405414275953E-6</c:v>
+                  <c:v>0.809161980420098</c:v>
                 </c:pt>
                 <c:pt idx="85">
-                  <c:v>1.48249287113554E-6</c:v>
+                  <c:v>0.82315100125713</c:v>
                 </c:pt>
                 <c:pt idx="86">
-                  <c:v>1.56529919531051E-6</c:v>
+                  <c:v>0.837297242438799</c:v>
                 </c:pt>
                 <c:pt idx="87">
-                  <c:v>1.65780432100715E-6</c:v>
+                  <c:v>0.851612502466471</c:v>
                 </c:pt>
                 <c:pt idx="88">
-                  <c:v>1.76554139881904E-6</c:v>
+                  <c:v>0.866104706668718</c:v>
                 </c:pt>
                 <c:pt idx="89">
-                  <c:v>1.89196680357795E-6</c:v>
+                  <c:v>0.880788133741802</c:v>
                 </c:pt>
                 <c:pt idx="90">
-                  <c:v>2.0443480421659E-6</c:v>
+                  <c:v>0.895672788303241</c:v>
                 </c:pt>
                 <c:pt idx="91">
-                  <c:v>2.21823679021752E-6</c:v>
+                  <c:v>0.910778071657632</c:v>
                 </c:pt>
                 <c:pt idx="92">
-                  <c:v>2.43527347522359E-6</c:v>
+                  <c:v>0.926124580438353</c:v>
                 </c:pt>
                 <c:pt idx="93">
-                  <c:v>2.71369316005846E-6</c:v>
+                  <c:v>0.941742939159582</c:v>
                 </c:pt>
                 <c:pt idx="94">
-                  <c:v>3.07183328543636E-6</c:v>
+                  <c:v>0.95767219482098</c:v>
                 </c:pt>
                 <c:pt idx="95">
-                  <c:v>3.53872694294311E-6</c:v>
+                  <c:v>0.973965682866663</c:v>
                 </c:pt>
                 <c:pt idx="96">
-                  <c:v>4.20971982209716E-6</c:v>
+                  <c:v>0.990672650347636</c:v>
                 </c:pt>
                 <c:pt idx="97">
-                  <c:v>5.2214549583467E-6</c:v>
+                  <c:v>1.00789388886077</c:v>
                 </c:pt>
                 <c:pt idx="98">
-                  <c:v>6.86494928525612E-6</c:v>
+                  <c:v>1.02579240474486</c:v>
                 </c:pt>
                 <c:pt idx="99">
-                  <c:v>1.02310686863785E-5</c:v>
+                  <c:v>1.04472558186974</c:v>
                 </c:pt>
                 <c:pt idx="100">
-                  <c:v>2.036265895681E-5</c:v>
+                  <c:v>1.06560997912587</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -539,11 +538,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-1192144096"/>
-        <c:axId val="-1198075120"/>
+        <c:axId val="-2098952720"/>
+        <c:axId val="2062556112"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-1192144096"/>
+        <c:axId val="-2098952720"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -599,12 +598,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1198075120"/>
+        <c:crossAx val="2062556112"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-1198075120"/>
+        <c:axId val="2062556112"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -661,7 +660,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1192144096"/>
+        <c:crossAx val="-2098952720"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1119,304 +1118,304 @@
                   <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.000040205045733</c:v>
+                  <c:v>2.004347826086956</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4.000040491157743</c:v>
+                  <c:v>4.021497095231411</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>8.000054883235915</c:v>
+                  <c:v>8.074079559422598</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>16.00008343153921</c:v>
+                  <c:v>16.21898684353959</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>32.00013433355862</c:v>
+                  <c:v>32.5945463075694</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>64.00022717108108</c:v>
+                  <c:v>65.5273203338472</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>128.0003936414602</c:v>
+                  <c:v>131.7756063328385</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>256.0006954801938</c:v>
+                  <c:v>265.0728535415479</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>512.0012474022603</c:v>
+                  <c:v>533.3361043843096</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>1024.002271295615</c:v>
+                  <c:v>1073.327506476472</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>2048.00417927626</c:v>
+                  <c:v>2160.495040561708</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>4096.007733525665</c:v>
+                  <c:v>4349.667280502553</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>8192.01445878398</c:v>
+                  <c:v>8758.608362441479</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>16384.02716193879</c:v>
+                  <c:v>17639.44774825458</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>32768.05133684477</c:v>
+                  <c:v>35530.68350704803</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>65536.09739829326</c:v>
+                  <c:v>71579.1100786388</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>131072.1852005708</c:v>
+                  <c:v>144221.9484455685</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>262144.3541596302</c:v>
+                  <c:v>290626.7779203014</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>524288.6797696791</c:v>
+                  <c:v>585728.8928962857</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>1.04857730807768E6</c:v>
+                  <c:v>1.18062499026648E6</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>2.09715451901981E6</c:v>
+                  <c:v>2.38001892740234E6</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>4.1943088735332E6</c:v>
+                  <c:v>4.79843719193635E6</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>8.38861745129242E6</c:v>
+                  <c:v>9.6753766706619E6</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>1.67772343428317E7</c:v>
+                  <c:v>1.95111914929769E7</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>3.35544676721446E7</c:v>
+                  <c:v>3.93501978176389E7</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>6.71089335273737E7</c:v>
+                  <c:v>7.93698728379472E7</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>1.3421786361168E8</c:v>
+                  <c:v>1.60106462583951E8</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>2.68435721171198E8</c:v>
+                  <c:v>3.23002368898097E8</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>5.36871432207621E8</c:v>
+                  <c:v>6.51695729869384E8</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>1.07374284356616E9</c:v>
+                  <c:v>1.31500132179501E9</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>2.14748564747827E9</c:v>
+                  <c:v>2.65367878922598E9</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>4.29497122555772E9</c:v>
+                  <c:v>5.35563291644364E9</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>8.58994230892639E9</c:v>
+                  <c:v>1.0809674929447E10</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>1.71798844202832E10</c:v>
+                  <c:v>2.18199093252568E10</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>3.43597684174458E10</c:v>
+                  <c:v>4.40485678769996E10</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>6.87195360634133E10</c:v>
+                  <c:v>8.89300689341357E10</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>1.37439070582053E11</c:v>
+                  <c:v>1.79557126243295E11</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>2.74878138662876E11</c:v>
+                  <c:v>3.6257117226007E11</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>5.49756272712198E11</c:v>
+                  <c:v>7.3218440116833E11</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>1.09951253854301E12</c:v>
+                  <c:v>1.47871366028707E12</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>2.19902506197311E12</c:v>
+                  <c:v>2.98664665549617E12</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>4.39805009596729E12</c:v>
+                  <c:v>6.03280263300352E12</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>8.79610014505806E12</c:v>
+                  <c:v>1.21868044821716E13</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>1.7592200215058E13</c:v>
+                  <c:v>2.46204195192794E13</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>3.51844002715467E13</c:v>
+                  <c:v>4.97434802495069E13</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>7.03688003670682E13</c:v>
+                  <c:v>1.00510626725386E14</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>1.40737600376788E14</c:v>
+                  <c:v>2.03105834273281E14</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>2.81475200123708E14</c:v>
+                  <c:v>4.10456542165858E14</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>5.62950399549836E14</c:v>
+                  <c:v>8.29557601466858E14</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>1.1259007986742E15</c:v>
+                  <c:v>1.67672045620468E15</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>2.25180159663236E15</c:v>
+                  <c:v>3.38929498003283E15</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>4.50360319992067E15</c:v>
+                  <c:v>6.85161072404364E15</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>9.00720640543432E15</c:v>
+                  <c:v>1.38519492273832E16</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>1.80144128471333E16</c:v>
+                  <c:v>2.80068496547062E16</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>3.60288257685405E16</c:v>
+                  <c:v>5.6630784159787E16</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>7.205765183279E16</c:v>
+                  <c:v>1.14518578785034E17</c:v>
                 </c:pt>
                 <c:pt idx="57">
-                  <c:v>1.44115304180834E17</c:v>
+                  <c:v>2.31597814506409E17</c:v>
                 </c:pt>
                 <c:pt idx="58">
-                  <c:v>2.88230609946863E17</c:v>
+                  <c:v>4.68412322250462E17</c:v>
                 </c:pt>
                 <c:pt idx="59">
-                  <c:v>5.76461222111991E17</c:v>
+                  <c:v>9.47453068905051E17</c:v>
                 </c:pt>
                 <c:pt idx="60">
-                  <c:v>1.15292245150741E18</c:v>
+                  <c:v>1.91656354378366E18</c:v>
                 </c:pt>
                 <c:pt idx="61">
-                  <c:v>2.30584491744756E18</c:v>
+                  <c:v>3.87726127778319E18</c:v>
                 </c:pt>
                 <c:pt idx="62">
-                  <c:v>4.61168987256365E18</c:v>
+                  <c:v>7.84446822453773E18</c:v>
                 </c:pt>
                 <c:pt idx="63">
-                  <c:v>9.2233798171264E18</c:v>
+                  <c:v>1.58722582228439E19</c:v>
                 </c:pt>
                 <c:pt idx="64">
-                  <c:v>1.84467598245816E19</c:v>
+                  <c:v>3.21181883485983E19</c:v>
                 </c:pt>
                 <c:pt idx="65">
-                  <c:v>3.68935199823111E19</c:v>
+                  <c:v>6.49981238427468E19</c:v>
                 </c:pt>
                 <c:pt idx="66">
-                  <c:v>7.37870408189855E19</c:v>
+                  <c:v>1.31549372098733E20</c:v>
                 </c:pt>
                 <c:pt idx="67">
-                  <c:v>1.47574083431336E20</c:v>
+                  <c:v>2.66265921066272E20</c:v>
                 </c:pt>
                 <c:pt idx="68">
-                  <c:v>2.95148170997422E20</c:v>
+                  <c:v>5.38991010804166E20</c:v>
                 </c:pt>
                 <c:pt idx="69">
-                  <c:v>5.90296350411266E20</c:v>
+                  <c:v>1.09115767081886E21</c:v>
                 </c:pt>
                 <c:pt idx="70">
-                  <c:v>1.18059272150932E21</c:v>
+                  <c:v>2.2091931983375E21</c:v>
                 </c:pt>
                 <c:pt idx="71">
-                  <c:v>2.36118548211431E21</c:v>
+                  <c:v>4.47323309932845E21</c:v>
                 </c:pt>
                 <c:pt idx="72">
-                  <c:v>4.72237105343841E21</c:v>
+                  <c:v>9.05840234162556E21</c:v>
                 </c:pt>
                 <c:pt idx="73">
-                  <c:v>9.44474229905118E21</c:v>
+                  <c:v>1.83453057759661E22</c:v>
                 </c:pt>
                 <c:pt idx="74">
-                  <c:v>1.88894850318508E22</c:v>
+                  <c:v>3.71571102577271E22</c:v>
                 </c:pt>
                 <c:pt idx="75">
-                  <c:v>3.77789710344755E22</c:v>
+                  <c:v>7.52667937612768E22</c:v>
                 </c:pt>
                 <c:pt idx="76">
-                  <c:v>7.55579439901517E22</c:v>
+                  <c:v>1.52479232053157E23</c:v>
                 </c:pt>
                 <c:pt idx="77">
-                  <c:v>1.51115893180518E23</c:v>
+                  <c:v>3.08934022952949E23</c:v>
                 </c:pt>
                 <c:pt idx="78">
-                  <c:v>3.02231794904439E23</c:v>
+                  <c:v>6.25993695415549E23</c:v>
                 </c:pt>
                 <c:pt idx="79">
-                  <c:v>6.04463612848557E23</c:v>
+                  <c:v>1.26860042322505E24</c:v>
                 </c:pt>
                 <c:pt idx="80">
-                  <c:v>1.20892727386526E24</c:v>
+                  <c:v>2.57118109004354E24</c:v>
                 </c:pt>
                 <c:pt idx="81">
-                  <c:v>2.41785465774801E24</c:v>
+                  <c:v>5.21189686952062E24</c:v>
                 </c:pt>
                 <c:pt idx="82">
-                  <c:v>4.83570955370281E24</c:v>
+                  <c:v>1.05661075017417E25</c:v>
                 </c:pt>
                 <c:pt idx="83">
-                  <c:v>9.67141963391346E24</c:v>
+                  <c:v>2.14236838843926E25</c:v>
                 </c:pt>
                 <c:pt idx="84">
-                  <c:v>1.93428404656384E25</c:v>
+                  <c:v>4.34444415314626E25</c:v>
                 </c:pt>
                 <c:pt idx="85">
-                  <c:v>3.86856835788755E25</c:v>
+                  <c:v>8.81129150016346E25</c:v>
                 </c:pt>
                 <c:pt idx="86">
-                  <c:v>7.73713735645899E25</c:v>
+                  <c:v>1.78736479354241E26</c:v>
                 </c:pt>
                 <c:pt idx="87">
-                  <c:v>1.54742761443678E26</c:v>
+                  <c:v>3.62627080343183E26</c:v>
                 </c:pt>
                 <c:pt idx="88">
-                  <c:v>3.09485556230425E26</c:v>
+                  <c:v>7.35841221712629E26</c:v>
                 </c:pt>
                 <c:pt idx="89">
-                  <c:v>6.18971190714525E26</c:v>
+                  <c:v>1.49345121422091E27</c:v>
                 </c:pt>
                 <c:pt idx="90">
-                  <c:v>1.23794257006826E27</c:v>
+                  <c:v>3.03169396560521E27</c:v>
                 </c:pt>
                 <c:pt idx="91">
-                  <c:v>2.47588557066512E27</c:v>
+                  <c:v>6.15567236052428E27</c:v>
                 </c:pt>
                 <c:pt idx="92">
-                  <c:v>4.95177221604636E27</c:v>
+                  <c:v>1.25017380808988E28</c:v>
                 </c:pt>
                 <c:pt idx="93">
-                  <c:v>9.90354718943491E27</c:v>
+                  <c:v>2.53970549485657E28</c:v>
                 </c:pt>
                 <c:pt idx="94">
-                  <c:v>1.98071014725864E28</c:v>
+                  <c:v>5.16097008928399E28</c:v>
                 </c:pt>
                 <c:pt idx="95">
-                  <c:v>3.96142214407966E28</c:v>
+                  <c:v>1.04914981819865E29</c:v>
                 </c:pt>
                 <c:pt idx="96">
-                  <c:v>7.92284960433319E28</c:v>
+                  <c:v>2.13365033944943E29</c:v>
                 </c:pt>
                 <c:pt idx="97">
-                  <c:v>1.58457152403252E29</c:v>
+                  <c:v>4.34142530873657E29</c:v>
                 </c:pt>
                 <c:pt idx="98">
-                  <c:v>3.16914825653795E29</c:v>
+                  <c:v>8.83965989764336E29</c:v>
                 </c:pt>
                 <c:pt idx="99">
-                  <c:v>6.33831784857468E29</c:v>
+                  <c:v>1.80172342917706E30</c:v>
                 </c:pt>
                 <c:pt idx="100">
-                  <c:v>1.26767641322789E30</c:v>
+                  <c:v>3.67949400946432E30</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1431,11 +1430,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-1198974672"/>
-        <c:axId val="-2093676464"/>
+        <c:axId val="-2122796128"/>
+        <c:axId val="-2095378160"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-1198974672"/>
+        <c:axId val="-2122796128"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1492,12 +1491,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2093676464"/>
+        <c:crossAx val="-2095378160"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2093676464"/>
+        <c:axId val="-2095378160"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1554,7 +1553,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1198974672"/>
+        <c:crossAx val="-2122796128"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2781,7 +2780,7 @@
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="SUSWeight_function_1" connectionId="2" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="SUSWeight_function" connectionId="2" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3049,15 +3048,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E102"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="65" workbookViewId="0">
-      <selection activeCell="Q26" sqref="Q26"/>
+    <sheetView tabSelected="1" zoomScale="75" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="8.33203125" customWidth="1"/>
+    <col min="2" max="2" width="9.1640625" customWidth="1"/>
     <col min="3" max="3" width="21.1640625" customWidth="1"/>
     <col min="4" max="4" width="14.6640625" customWidth="1"/>
+    <col min="5" max="5" width="10.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
@@ -3102,19 +3102,19 @@
         <v>1</v>
       </c>
       <c r="B3" s="1">
-        <v>2.01023208135447E-5</v>
+        <v>2.1715535135079299E-3</v>
       </c>
       <c r="C3">
         <f t="shared" ref="C3:C66" si="0">EXP(B3)</f>
-        <v>1.0000201025228665</v>
-      </c>
-      <c r="D3">
-        <f t="shared" ref="D3:D66" si="1">B3+A3*LN(2/1)</f>
-        <v>0.69316728288075879</v>
+        <v>1.0021739130434784</v>
+      </c>
+      <c r="D3" s="1">
+        <f>B3+A3*LN(2/1)</f>
+        <v>0.69531873407345324</v>
       </c>
       <c r="E3">
-        <f t="shared" ref="E3:E66" si="2">EXP(D3)</f>
-        <v>2.0000402050457331</v>
+        <f t="shared" ref="E3:E66" si="1">EXP(D3)</f>
+        <v>2.0043478260869567</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
@@ -3123,19 +3123,19 @@
         <v>2</v>
       </c>
       <c r="B4" s="1">
-        <v>1.01227382007085E-5</v>
+        <v>5.3598839321026704E-3</v>
       </c>
       <c r="C4">
-        <f t="shared" si="0"/>
-        <v>1.0000101227894358</v>
+        <f>EXP(B4)</f>
+        <v>1.0053742738078528</v>
       </c>
       <c r="D4">
-        <f t="shared" si="1"/>
-        <v>1.3863044838580914</v>
+        <f t="shared" ref="D3:D66" si="2">B4+A4*LN(2/1)</f>
+        <v>1.3916542450519933</v>
       </c>
       <c r="E4">
-        <f t="shared" si="2"/>
-        <v>4.0000404911577432</v>
+        <f t="shared" si="1"/>
+        <v>4.0214970952314113</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
@@ -3144,19 +3144,19 @@
         <v>3</v>
       </c>
       <c r="B5" s="1">
-        <v>6.8603809569166001E-6</v>
+        <v>9.2173344827216099E-3</v>
       </c>
       <c r="C5">
         <f t="shared" si="0"/>
-        <v>1.0000068604044894</v>
+        <v>1.009259944927825</v>
       </c>
       <c r="D5">
-        <f t="shared" si="1"/>
-        <v>2.0794484020607928</v>
+        <f t="shared" si="2"/>
+        <v>2.0886588761625573</v>
       </c>
       <c r="E5">
-        <f t="shared" si="2"/>
-        <v>8.0000548832359151</v>
+        <f t="shared" si="1"/>
+        <v>8.0740795594225983</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
@@ -3165,19 +3165,19 @@
         <v>4</v>
       </c>
       <c r="B6" s="1">
-        <v>5.21445760507996E-6</v>
+        <v>1.3593861089636E-2</v>
       </c>
       <c r="C6">
         <f t="shared" si="0"/>
-        <v>1.0000052144712004</v>
+        <v>1.013686677721225</v>
       </c>
       <c r="D6">
-        <f t="shared" si="1"/>
-        <v>2.7725939366973864</v>
+        <f t="shared" si="2"/>
+        <v>2.7861825833294169</v>
       </c>
       <c r="E6">
-        <f t="shared" si="2"/>
-        <v>16.000083431539206</v>
+        <f t="shared" si="1"/>
+        <v>16.218986843539593</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
@@ -3186,19 +3186,19 @@
         <v>5</v>
       </c>
       <c r="B7" s="1">
-        <v>4.1979148956152597E-6</v>
+        <v>1.8409080399352601E-2</v>
       </c>
       <c r="C7">
         <f t="shared" si="0"/>
-        <v>1.0000041979237069</v>
+        <v>1.0185795721115438</v>
       </c>
       <c r="D7">
-        <f t="shared" si="1"/>
-        <v>3.4657401007146222</v>
+        <f t="shared" si="2"/>
+        <v>3.4841449831990792</v>
       </c>
       <c r="E7">
-        <f t="shared" si="2"/>
-        <v>32.00013433355862</v>
+        <f t="shared" si="1"/>
+        <v>32.594546307569402</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
@@ -3207,19 +3207,19 @@
         <v>6</v>
       </c>
       <c r="B8" s="1">
-        <v>3.5495418428918499E-6</v>
+        <v>2.35840766512481E-2</v>
       </c>
       <c r="C8">
         <f t="shared" si="0"/>
-        <v>1.0000035495481425</v>
+        <v>1.0238643802163625</v>
       </c>
       <c r="D8">
-        <f t="shared" si="1"/>
-        <v>4.1588866329015142</v>
+        <f t="shared" si="2"/>
+        <v>4.18246716001092</v>
       </c>
       <c r="E8">
-        <f t="shared" si="2"/>
-        <v>64.000227171081079</v>
+        <f t="shared" si="1"/>
+        <v>65.5273203338472</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
@@ -3228,19 +3228,19 @@
         <v>7</v>
       </c>
       <c r="B9" s="1">
-        <v>3.07531917962026E-6</v>
+        <v>2.9070260084743098E-2</v>
       </c>
       <c r="C9">
         <f t="shared" si="0"/>
-        <v>1.0000030753239084</v>
+        <v>1.0294969244753014</v>
       </c>
       <c r="D9">
-        <f t="shared" si="1"/>
-        <v>4.8520333392387966</v>
+        <f t="shared" si="2"/>
+        <v>4.8811005240043599</v>
       </c>
       <c r="E9">
-        <f t="shared" si="2"/>
-        <v>128.00039364146025</v>
+        <f t="shared" si="1"/>
+        <v>131.77560633283855</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
@@ -3249,19 +3249,19 @@
         <v>8</v>
       </c>
       <c r="B10" s="1">
-        <v>2.7167158166364499E-6</v>
+        <v>3.4827262748058398E-2</v>
       </c>
       <c r="C10">
         <f t="shared" si="0"/>
-        <v>1.0000027167195069</v>
+        <v>1.0354408341466714</v>
       </c>
       <c r="D10">
-        <f t="shared" si="1"/>
-        <v>5.545180161195379</v>
+        <f t="shared" si="2"/>
+        <v>5.5800047072276211</v>
       </c>
       <c r="E10">
-        <f t="shared" si="2"/>
-        <v>256.00069548019377</v>
+        <f t="shared" si="1"/>
+        <v>265.07285354154794</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
@@ -3270,19 +3270,19 @@
         <v>9</v>
       </c>
       <c r="B11" s="1">
-        <v>2.43632957208128E-6</v>
+        <v>4.0827190227338203E-2</v>
       </c>
       <c r="C11">
         <f t="shared" si="0"/>
-        <v>1.0000024363325399</v>
+        <v>1.0416720788756051</v>
       </c>
       <c r="D11">
-        <f t="shared" si="1"/>
-        <v>6.2383270613690796</v>
+        <f t="shared" si="2"/>
+        <v>6.2791518152668457</v>
       </c>
       <c r="E11">
-        <f t="shared" si="2"/>
-        <v>512.00124740226033</v>
+        <f t="shared" si="1"/>
+        <v>533.33610438430958</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
@@ -3291,19 +3291,19 @@
         <v>10</v>
       </c>
       <c r="B12" s="1">
-        <v>2.21805966363066E-6</v>
+        <v>4.7047115507527201E-2</v>
       </c>
       <c r="C12">
         <f t="shared" si="0"/>
-        <v>1.0000022180621235</v>
+        <v>1.04817139304343</v>
       </c>
       <c r="D12">
-        <f t="shared" si="1"/>
-        <v>6.931474023659117</v>
+        <f t="shared" si="2"/>
+        <v>6.9785189211069802</v>
       </c>
       <c r="E12">
-        <f t="shared" si="2"/>
-        <v>1024.0022712956147</v>
+        <f t="shared" si="1"/>
+        <v>1073.3275064764723</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
@@ -3312,19 +3312,19 @@
         <v>11</v>
       </c>
       <c r="B13" s="1">
-        <v>2.0406601534877999E-6</v>
+        <v>5.3473673705075102E-2</v>
       </c>
       <c r="C13">
         <f t="shared" si="0"/>
-        <v>1.0000020406622356</v>
+        <v>1.0549292190242712</v>
       </c>
       <c r="D13">
-        <f t="shared" si="1"/>
-        <v>7.6246210268195522</v>
+        <f t="shared" si="2"/>
+        <v>7.6780926598644736</v>
       </c>
       <c r="E13">
-        <f t="shared" si="2"/>
-        <v>2048.0041792762595</v>
+        <f t="shared" si="1"/>
+        <v>2160.4950405617078</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
@@ -3333,19 +3333,19 @@
         <v>12</v>
       </c>
       <c r="B14" s="1">
-        <v>1.8880660068263699E-6</v>
+        <v>6.0088467197296498E-2</v>
       </c>
       <c r="C14">
         <f t="shared" si="0"/>
-        <v>1.0000018880677892</v>
+        <v>1.0619304884039447</v>
       </c>
       <c r="D14">
-        <f t="shared" si="1"/>
-        <v>8.3177680547853505</v>
+        <f t="shared" si="2"/>
+        <v>8.3778546339166393</v>
       </c>
       <c r="E14">
-        <f t="shared" si="2"/>
-        <v>4096.0077335256647</v>
+        <f t="shared" si="1"/>
+        <v>4349.6672805025537</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
@@ -3354,19 +3354,19 @@
         <v>13</v>
       </c>
       <c r="B15" s="1">
-        <v>1.76498672282717E-6</v>
+        <v>6.6878961296137102E-2</v>
       </c>
       <c r="C15">
         <f t="shared" si="0"/>
-        <v>1.0000017649882804</v>
+        <v>1.0691660598683455</v>
       </c>
       <c r="D15">
-        <f t="shared" si="1"/>
-        <v>9.0109151122660105</v>
+        <f t="shared" si="2"/>
+        <v>9.0777923085754253</v>
       </c>
       <c r="E15">
-        <f t="shared" si="2"/>
-        <v>8192.0144587839823</v>
+        <f t="shared" si="1"/>
+        <v>8758.6083624414787</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
@@ -3375,19 +3375,19 @@
         <v>14</v>
       </c>
       <c r="B16" s="1">
-        <v>1.6578318047546E-6</v>
+        <v>7.3832494443190802E-2</v>
       </c>
       <c r="C16">
         <f t="shared" si="0"/>
-        <v>1.000001657833179</v>
+        <v>1.0766264494784286</v>
       </c>
       <c r="D16">
-        <f t="shared" si="1"/>
-        <v>9.7040621856710381</v>
+        <f t="shared" si="2"/>
+        <v>9.7778930222824254</v>
       </c>
       <c r="E16">
-        <f t="shared" si="2"/>
-        <v>16384.027161938786</v>
+        <f t="shared" si="1"/>
+        <v>17639.447748254581</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
@@ -3396,19 +3396,19 @@
         <v>15</v>
       </c>
       <c r="B17" s="1">
-        <v>1.5666749440026799E-6</v>
+        <v>8.0944217893508794E-2</v>
       </c>
       <c r="C17">
         <f t="shared" si="0"/>
-        <v>1.0000015666761712</v>
+        <v>1.0843104097609886</v>
       </c>
       <c r="D17">
-        <f t="shared" si="1"/>
-        <v>10.397209275074124</v>
+        <f t="shared" si="2"/>
+        <v>10.478151926292687</v>
       </c>
       <c r="E17">
-        <f t="shared" si="2"/>
-        <v>32768.051336844779</v>
+        <f t="shared" si="1"/>
+        <v>35530.683507048037</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
@@ -3417,19 +3417,19 @@
         <v>16</v>
       </c>
       <c r="B18" s="1">
-        <v>1.4861789078023999E-6</v>
+        <v>8.8203662741539804E-2</v>
       </c>
       <c r="C18">
         <f t="shared" si="0"/>
-        <v>1.0000014861800122</v>
+        <v>1.0922105419714174</v>
       </c>
       <c r="D18">
-        <f t="shared" si="1"/>
-        <v>11.090356375138033</v>
+        <f t="shared" si="2"/>
+        <v>11.178558551700664</v>
       </c>
       <c r="E18">
-        <f t="shared" si="2"/>
-        <v>65536.097398293263</v>
+        <f t="shared" si="1"/>
+        <v>71579.110078638798</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
@@ -3438,19 +3438,19 @@
         <v>17</v>
       </c>
       <c r="B19" s="1">
-        <v>1.41296722418643E-6</v>
+        <v>9.56066310917906E-2</v>
       </c>
       <c r="C19">
         <f t="shared" si="0"/>
-        <v>1.0000014129682224</v>
+        <v>1.1003261447568402</v>
       </c>
       <c r="D19">
-        <f t="shared" si="1"/>
-        <v>11.783503482486294</v>
+        <f t="shared" si="2"/>
+        <v>11.87910870061086</v>
       </c>
       <c r="E19">
-        <f t="shared" si="2"/>
-        <v>131072.18520057079</v>
+        <f t="shared" si="1"/>
+        <v>144221.9484455685</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
@@ -3459,19 +3459,19 @@
         <v>18</v>
       </c>
       <c r="B20" s="1">
-        <v>1.35101086006113E-6</v>
+        <v>0.10314592280126</v>
       </c>
       <c r="C20">
         <f t="shared" si="0"/>
-        <v>1.0000013510117727</v>
+        <v>1.1086531750499773</v>
       </c>
       <c r="D20">
-        <f t="shared" si="1"/>
-        <v>12.476650601089876</v>
+        <f t="shared" si="2"/>
+        <v>12.579795172880276</v>
       </c>
       <c r="E20">
-        <f t="shared" si="2"/>
-        <v>262144.35415963019</v>
+        <f t="shared" si="1"/>
+        <v>290626.77792030142</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.2">
@@ -3480,19 +3480,19 @@
         <v>19</v>
       </c>
       <c r="B21" s="1">
-        <v>1.2965569281737699E-6</v>
+        <v>0.110815890760507</v>
       </c>
       <c r="C21">
         <f t="shared" si="0"/>
-        <v>1.0000012965577687</v>
+        <v>1.1171892030645092</v>
       </c>
       <c r="D21">
-        <f t="shared" si="1"/>
-        <v>13.169797727195888</v>
+        <f t="shared" si="2"/>
+        <v>13.280612321399468</v>
       </c>
       <c r="E21">
-        <f t="shared" si="2"/>
-        <v>524288.67976967909</v>
+        <f t="shared" si="1"/>
+        <v>585728.89289628575</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.2">
@@ -3501,19 +3501,19 @@
         <v>20</v>
       </c>
       <c r="B22" s="1">
-        <v>1.24747931201368E-6</v>
+        <v>0.118610897794628</v>
       </c>
       <c r="C22">
         <f t="shared" si="0"/>
-        <v>1.0000012474800901</v>
+        <v>1.1259317305245233</v>
       </c>
       <c r="D22">
-        <f t="shared" si="1"/>
-        <v>13.862944858678219</v>
+        <f t="shared" si="2"/>
+        <v>13.981554508993534</v>
       </c>
       <c r="E22">
-        <f t="shared" si="2"/>
-        <v>1048577.3080776837</v>
+        <f t="shared" si="1"/>
+        <v>1180624.990266483</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.2">
@@ -3522,19 +3522,19 @@
         <v>21</v>
       </c>
       <c r="B23" s="1">
-        <v>1.2011615231625599E-6</v>
+        <v>0.12652820654724001</v>
       </c>
       <c r="C23">
         <f t="shared" si="0"/>
-        <v>1.0000012011622446</v>
+        <v>1.134881461812179</v>
       </c>
       <c r="D23">
-        <f t="shared" si="1"/>
-        <v>14.556091992920376</v>
+        <f t="shared" si="2"/>
+        <v>14.682618998306092</v>
       </c>
       <c r="E23">
-        <f t="shared" si="2"/>
-        <v>2097154.5190198054</v>
+        <f t="shared" si="1"/>
+        <v>2380018.9274023352</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.2">
@@ -3543,19 +3543,19 @@
         <v>22</v>
       </c>
       <c r="B24" s="1">
-        <v>1.1619401844759401E-6</v>
+        <v>0.13456286553175401</v>
       </c>
       <c r="C24">
         <f t="shared" si="0"/>
-        <v>1.0000011619408595</v>
+        <v>1.1440365772095558</v>
       </c>
       <c r="D24">
-        <f t="shared" si="1"/>
-        <v>15.249239134258982</v>
+        <f t="shared" si="2"/>
+        <v>15.383800837850551</v>
       </c>
       <c r="E24">
-        <f t="shared" si="2"/>
-        <v>4194308.8735331977</v>
+        <f t="shared" si="1"/>
+        <v>4798437.1919363476</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.2">
@@ -3564,19 +3564,19 @@
         <v>23</v>
       </c>
       <c r="B25" s="1">
-        <v>1.12668121955215E-6</v>
+        <v>0.14270957561168501</v>
       </c>
       <c r="C25">
         <f t="shared" si="0"/>
-        <v>1.0000011266818543</v>
+        <v>1.1533947790458055</v>
       </c>
       <c r="D25">
-        <f t="shared" si="1"/>
-        <v>15.942386279559962</v>
+        <f t="shared" si="2"/>
+        <v>16.085094728490429</v>
       </c>
       <c r="E25">
-        <f t="shared" si="2"/>
-        <v>8388617.4512924179</v>
+        <f t="shared" si="1"/>
+        <v>9675376.6706618909</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.2">
@@ -3585,19 +3585,19 @@
         <v>24</v>
       </c>
       <c r="B26" s="1">
-        <v>1.0933173709318001E-6</v>
+        <v>0.15096644818139901</v>
       </c>
       <c r="C26">
         <f t="shared" si="0"/>
-        <v>1.0000010933179686</v>
+        <v>1.1629576380835143</v>
       </c>
       <c r="D26">
-        <f t="shared" si="1"/>
-        <v>16.635533426756059</v>
+        <f t="shared" si="2"/>
+        <v>16.786498781620086</v>
       </c>
       <c r="E26">
-        <f t="shared" si="2"/>
-        <v>16777234.34283172</v>
+        <f t="shared" si="1"/>
+        <v>19511191.492976934</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.2">
@@ -3606,19 +3606,19 @@
         <v>25</v>
       </c>
       <c r="B27" s="1">
-        <v>1.0631121865052299E-6</v>
+        <v>0.15933204594828401</v>
       </c>
       <c r="C27">
         <f t="shared" si="0"/>
-        <v>1.0000010631127516</v>
+        <v>1.1727272813808602</v>
       </c>
       <c r="D27">
-        <f t="shared" si="1"/>
-        <v>17.32868057711082</v>
+        <f t="shared" si="2"/>
+        <v>17.488011559946916</v>
       </c>
       <c r="E27">
-        <f t="shared" si="2"/>
-        <v>33554467.672144555</v>
+        <f t="shared" si="1"/>
+        <v>39350197.817638904</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.2">
@@ -3627,19 +3627,19 @@
         <v>26</v>
       </c>
       <c r="B28" s="1">
-        <v>1.0360380662208301E-6</v>
+        <v>0.16780272436466501</v>
       </c>
       <c r="C28">
         <f t="shared" si="0"/>
-        <v>1.0000010360386029</v>
+        <v>1.1827032690934427</v>
       </c>
       <c r="D28">
-        <f t="shared" si="1"/>
-        <v>18.021827730596645</v>
+        <f t="shared" si="2"/>
+        <v>18.189629418923243</v>
       </c>
       <c r="E28">
-        <f t="shared" si="2"/>
-        <v>67108933.527373716</v>
+        <f t="shared" si="1"/>
+        <v>79369872.837947235</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.2">
@@ -3648,19 +3648,19 @@
         <v>27</v>
       </c>
       <c r="B29" s="1">
-        <v>1.0103852448452101E-6</v>
+        <v>0.17637566795473</v>
       </c>
       <c r="C29">
         <f t="shared" si="0"/>
-        <v>1.0000010103857553</v>
+        <v>1.1928861035700951</v>
       </c>
       <c r="D29">
-        <f t="shared" si="1"/>
-        <v>18.714974885503768</v>
+        <f t="shared" si="2"/>
+        <v>18.891349543073254</v>
       </c>
       <c r="E29">
-        <f t="shared" si="2"/>
-        <v>134217863.61168042</v>
+        <f t="shared" si="1"/>
+        <v>160106462.58395091</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.2">
@@ -3669,19 +3669,19 @@
         <v>28</v>
       </c>
       <c r="B30" s="1">
-        <v>9.8783920546492507E-7</v>
+        <v>0.18504915953140699</v>
       </c>
       <c r="C30">
         <f t="shared" si="0"/>
-        <v>1.0000009878396934</v>
+        <v>1.2032775912363007</v>
       </c>
       <c r="D30">
-        <f t="shared" si="1"/>
-        <v>19.408122043517672</v>
+        <f t="shared" si="2"/>
+        <v>19.593170215209874</v>
       </c>
       <c r="E30">
-        <f t="shared" si="2"/>
-        <v>268435721.17119789</v>
+        <f t="shared" si="1"/>
+        <v>323002368.89809734</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.2">
@@ -3690,19 +3690,19 @@
         <v>29</v>
       </c>
       <c r="B31" s="1">
-        <v>9.6896173325291594E-7</v>
+        <v>0.193820102747784</v>
       </c>
       <c r="C31">
         <f t="shared" si="0"/>
-        <v>1.0000009689622027</v>
+        <v>1.2138778900157374</v>
       </c>
       <c r="D31">
-        <f t="shared" si="1"/>
-        <v>20.101269205200147</v>
+        <f t="shared" si="2"/>
+        <v>20.295088338986197</v>
       </c>
       <c r="E31">
-        <f t="shared" si="2"/>
-        <v>536871432.20762134</v>
+        <f t="shared" si="1"/>
+        <v>651695729.86938417</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.2">
@@ -3711,19 +3711,19 @@
         <v>30</v>
       </c>
       <c r="B32" s="1">
-        <v>9.4954452716195199E-7</v>
+        <v>0.20268809094458601</v>
       </c>
       <c r="C32">
         <f t="shared" si="0"/>
-        <v>1.000000949544978</v>
+        <v>1.2246904166368904</v>
       </c>
       <c r="D32">
-        <f t="shared" si="1"/>
-        <v>20.794416366342887</v>
+        <f t="shared" si="2"/>
+        <v>20.997103507742946</v>
       </c>
       <c r="E32">
-        <f t="shared" si="2"/>
-        <v>1073742843.5661569</v>
+        <f t="shared" si="1"/>
+        <v>1315001321.7950149</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.2">
@@ -3732,19 +3732,19 @@
         <v>31</v>
       </c>
       <c r="B33" s="1">
-        <v>9.3107919061254603E-7</v>
+        <v>0.21165013924586401</v>
       </c>
       <c r="C33">
         <f t="shared" si="0"/>
-        <v>1.0000009310796241</v>
+        <v>1.2357154810922093</v>
       </c>
       <c r="D33">
-        <f t="shared" si="1"/>
-        <v>21.487563528437494</v>
+        <f t="shared" si="2"/>
+        <v>21.699212736604171</v>
       </c>
       <c r="E33">
-        <f t="shared" si="2"/>
-        <v>2147485647.4782658</v>
+        <f t="shared" si="1"/>
+        <v>2653678789.2259784</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.2">
@@ -3753,19 +3753,19 @@
         <v>32</v>
       </c>
       <c r="B34" s="1">
-        <v>9.1492103539130401E-7</v>
+        <v>0.220704947623271</v>
       </c>
       <c r="C34">
         <f t="shared" si="0"/>
-        <v>1.0000009149214539</v>
+        <v>1.2469554591094227</v>
       </c>
       <c r="D34">
-        <f t="shared" si="1"/>
-        <v>22.180710692839284</v>
+        <f t="shared" si="2"/>
+        <v>22.401414725541521</v>
       </c>
       <c r="E34">
-        <f t="shared" si="2"/>
-        <v>4294971225.5577183</v>
+        <f t="shared" si="1"/>
+        <v>5355632916.4436369</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.2">
@@ -3774,19 +3774,19 @@
         <v>33</v>
       </c>
       <c r="B35" s="1">
-        <v>8.9836806941306096E-7</v>
+        <v>0.229850438385688</v>
       </c>
       <c r="C35">
         <f t="shared" si="0"/>
-        <v>1.0000008983684729</v>
+        <v>1.2584117857561261</v>
       </c>
       <c r="D35">
-        <f t="shared" si="1"/>
-        <v>22.873857856846261</v>
+        <f t="shared" si="2"/>
+        <v>23.103707396863882</v>
       </c>
       <c r="E35">
-        <f t="shared" si="2"/>
-        <v>8589942308.9263878</v>
+        <f t="shared" si="1"/>
+        <v>10809674929.447031</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.2">
@@ -3795,19 +3795,19 @@
         <v>34</v>
       </c>
       <c r="B36" s="1">
-        <v>8.86868012335373E-7</v>
+        <v>0.23908452272512801</v>
       </c>
       <c r="C36">
         <f t="shared" si="0"/>
-        <v>1.0000008868684056</v>
+        <v>1.2700858831671518</v>
       </c>
       <c r="D36">
-        <f t="shared" si="1"/>
-        <v>23.567005025906152</v>
+        <f t="shared" si="2"/>
+        <v>23.806088661763269</v>
       </c>
       <c r="E36">
-        <f t="shared" si="2"/>
-        <v>17179884420.283176</v>
+        <f t="shared" si="1"/>
+        <v>21819909325.256783</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.2">
@@ -3816,19 +3816,19 @@
         <v>35</v>
       </c>
       <c r="B37" s="1">
-        <v>8.7455359503695104E-7</v>
+        <v>0.24840735789666599</v>
       </c>
       <c r="C37">
         <f t="shared" si="0"/>
-        <v>1.0000008745539775</v>
+        <v>1.2819820513541229</v>
       </c>
       <c r="D37">
-        <f t="shared" si="1"/>
-        <v>24.260152194151679</v>
+        <f t="shared" si="2"/>
+        <v>24.508558677494751</v>
       </c>
       <c r="E37">
-        <f t="shared" si="2"/>
-        <v>34359768417.445801</v>
+        <f t="shared" si="1"/>
+        <v>44048567876.999557</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.2">
@@ -3837,19 +3837,19 @@
         <v>36</v>
       </c>
       <c r="B38" s="1">
-        <v>8.6332711594243803E-7</v>
+        <v>0.25781765535015</v>
       </c>
       <c r="C38">
         <f t="shared" si="0"/>
-        <v>1.0000008633274886</v>
+        <v>1.294102824382366</v>
       </c>
       <c r="D38">
-        <f t="shared" si="1"/>
-        <v>24.953299363485147</v>
+        <f t="shared" si="2"/>
+        <v>25.211116155508179</v>
       </c>
       <c r="E38">
-        <f t="shared" si="2"/>
-        <v>68719536063.413284</v>
+        <f t="shared" si="1"/>
+        <v>88930068934.135727</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.2">
@@ -3858,19 +3858,19 @@
         <v>37</v>
       </c>
       <c r="B39" s="1">
-        <v>8.5208742241462196E-7</v>
+        <v>0.267313565577113</v>
       </c>
       <c r="C39">
         <f t="shared" si="0"/>
-        <v>1.0000008520877854</v>
+        <v>1.3064500398708023</v>
       </c>
       <c r="D39">
-        <f t="shared" si="1"/>
-        <v>25.646446532805395</v>
+        <f t="shared" si="2"/>
+        <v>25.913759246295086</v>
       </c>
       <c r="E39">
-        <f t="shared" si="2"/>
-        <v>137439070582.05304</v>
+        <f t="shared" si="1"/>
+        <v>179557126243.29517</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.2">
@@ -3879,19 +3879,19 @@
         <v>38</v>
       </c>
       <c r="B40" s="1">
-        <v>8.42988004691359E-7</v>
+        <v>0.27689376796074</v>
       </c>
       <c r="C40">
         <f t="shared" si="0"/>
-        <v>1.00000084298836</v>
+        <v>1.3190262407445357</v>
       </c>
       <c r="D40">
-        <f t="shared" si="1"/>
-        <v>26.339593704265926</v>
+        <f t="shared" si="2"/>
+        <v>26.616486629238661</v>
       </c>
       <c r="E40">
-        <f t="shared" si="2"/>
-        <v>274878138662.87592</v>
+        <f t="shared" si="1"/>
+        <v>362571172260.07043</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.2">
@@ -3900,19 +3900,19 @@
         <v>39</v>
       </c>
       <c r="B41" s="1">
-        <v>8.3459600752783995E-7</v>
+        <v>0.28655819150919598</v>
       </c>
       <c r="C41">
         <f t="shared" si="0"/>
-        <v>1.0000008345963558</v>
+        <v>1.3318356671667611</v>
       </c>
       <c r="D41">
-        <f t="shared" si="1"/>
-        <v>27.032740876433873</v>
+        <f t="shared" si="2"/>
+        <v>27.319298233347062</v>
       </c>
       <c r="E41">
-        <f t="shared" si="2"/>
-        <v>549756272712.19824</v>
+        <f t="shared" si="1"/>
+        <v>732184401168.32971</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.2">
@@ -3921,19 +3921,19 @@
         <v>40</v>
       </c>
       <c r="B42" s="1">
-        <v>8.2833742330715605E-7</v>
+        <v>0.29630645492355701</v>
       </c>
       <c r="C42">
         <f t="shared" si="0"/>
-        <v>1.0000008283377664</v>
+        <v>1.344882239470341</v>
       </c>
       <c r="D42">
-        <f t="shared" si="1"/>
-        <v>27.725888050735236</v>
+        <f t="shared" si="2"/>
+        <v>28.022193677321368</v>
       </c>
       <c r="E42">
-        <f t="shared" si="2"/>
-        <v>1099512538543.0061</v>
+        <f t="shared" si="1"/>
+        <v>1478713660287.0654</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.2">
@@ -3942,19 +3942,19 @@
         <v>41</v>
       </c>
       <c r="B43" s="1">
-        <v>8.2146487733743702E-7</v>
+        <v>0.30613795109838099</v>
       </c>
       <c r="C43">
         <f t="shared" si="0"/>
-        <v>1.0000008214652147</v>
+        <v>1.3581696546208017</v>
       </c>
       <c r="D43">
-        <f t="shared" si="1"/>
-        <v>28.419035224422633</v>
+        <f t="shared" si="2"/>
+        <v>28.725172354056138</v>
       </c>
       <c r="E43">
-        <f t="shared" si="2"/>
-        <v>2199025061973.1055</v>
+        <f t="shared" si="1"/>
+        <v>2986646655496.1689</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.2">
@@ -3963,19 +3963,19 @@
         <v>42</v>
       </c>
       <c r="B44" s="1">
-        <v>8.1510321046507502E-7</v>
+        <v>0.31605121676505199</v>
       </c>
       <c r="C44">
         <f t="shared" si="0"/>
-        <v>1.0000008151035427</v>
+        <v>1.3717005078896147</v>
       </c>
       <c r="D44">
-        <f t="shared" si="1"/>
-        <v>29.112182398620913</v>
+        <f t="shared" si="2"/>
+        <v>29.428232800282757</v>
       </c>
       <c r="E44">
-        <f t="shared" si="2"/>
-        <v>4398050095967.29</v>
+        <f t="shared" si="1"/>
+        <v>6032802633003.5166</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.2">
@@ -3984,19 +3984,19 @@
         <v>43</v>
       </c>
       <c r="B45" s="1">
-        <v>8.0977397174789799E-7</v>
+        <v>0.326046118416911</v>
       </c>
       <c r="C45">
         <f t="shared" si="0"/>
-        <v>1.0000008097742996</v>
+        <v>1.3854792635097097</v>
       </c>
       <c r="D45">
-        <f t="shared" si="1"/>
-        <v>29.805329573851619</v>
+        <f t="shared" si="2"/>
+        <v>30.131374882494558</v>
       </c>
       <c r="E45">
-        <f t="shared" si="2"/>
-        <v>8796100145058.0586</v>
+        <f t="shared" si="1"/>
+        <v>12186804482171.625</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.2">
@@ -4005,19 +4005,19 @@
         <v>44</v>
       </c>
       <c r="B46" s="1">
-        <v>8.0550741519955097E-7</v>
+        <v>0.33612133167785702</v>
       </c>
       <c r="C46">
         <f t="shared" si="0"/>
-        <v>1.0000008055077396</v>
+        <v>1.3995088192632161</v>
       </c>
       <c r="D46">
-        <f t="shared" si="1"/>
-        <v>30.498476750145009</v>
+        <f t="shared" si="2"/>
+        <v>30.834597276315449</v>
       </c>
       <c r="E46">
-        <f t="shared" si="2"/>
-        <v>17592200215058.023</v>
+        <f t="shared" si="1"/>
+        <v>24620419519279.43</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.2">
@@ -4026,19 +4026,19 @@
         <v>45</v>
       </c>
       <c r="B47" s="1">
-        <v>8.0100060989360898E-7</v>
+        <v>0.34627739548660902</v>
       </c>
       <c r="C47">
         <f t="shared" si="0"/>
-        <v>1.0000008010009307</v>
+        <v>1.4137947417085279</v>
       </c>
       <c r="D47">
-        <f t="shared" si="1"/>
-        <v>31.191623926198147</v>
+        <f t="shared" si="2"/>
+        <v>31.537900520684147</v>
       </c>
       <c r="E47">
-        <f t="shared" si="2"/>
-        <v>35184400271546.742</v>
+        <f t="shared" si="1"/>
+        <v>49743480249506.93</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.2">
@@ -4047,19 +4047,19 @@
         <v>46</v>
       </c>
       <c r="B48" s="1">
-        <v>7.9849914108589001E-7</v>
+        <v>0.35651427064131802</v>
       </c>
       <c r="C48">
         <f t="shared" si="0"/>
-        <v>1.0000007984994599</v>
+        <v>1.4283419137283551</v>
       </c>
       <c r="D48">
-        <f t="shared" si="1"/>
-        <v>31.884771104256625</v>
+        <f t="shared" si="2"/>
+        <v>32.241284576398805</v>
       </c>
       <c r="E48">
-        <f t="shared" si="2"/>
-        <v>70368800367068.219</v>
+        <f t="shared" si="1"/>
+        <v>100510626725385.88</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.2">
@@ -4068,19 +4068,19 @@
         <v>47</v>
       </c>
       <c r="B49" s="1">
-        <v>7.95960025305249E-7</v>
+        <v>0.36683082389654398</v>
       </c>
       <c r="C49">
         <f t="shared" si="0"/>
-        <v>1.0000007959603421</v>
+        <v>1.4431537513337447</v>
       </c>
       <c r="D49">
-        <f t="shared" si="1"/>
-        <v>32.577918282277459</v>
+        <f t="shared" si="2"/>
+        <v>32.944748310213974</v>
       </c>
       <c r="E49">
-        <f t="shared" si="2"/>
-        <v>140737600376787.91</v>
+        <f t="shared" si="1"/>
+        <v>203105834273280.97</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.2">
@@ -4089,19 +4089,19 @@
         <v>48</v>
       </c>
       <c r="B50" s="1">
-        <v>7.9372229175352399E-7</v>
+        <v>0.377226506726489</v>
       </c>
       <c r="C50">
         <f t="shared" si="0"/>
-        <v>1.0000007937226068</v>
+        <v>1.4582345719058065</v>
       </c>
       <c r="D50">
-        <f t="shared" si="1"/>
-        <v>33.271065460599665</v>
+        <f t="shared" si="2"/>
+        <v>33.648291173603859</v>
       </c>
       <c r="E50">
-        <f t="shared" si="2"/>
-        <v>281475200123707.88</v>
+        <f t="shared" si="1"/>
+        <v>410456542165858.25</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.2">
@@ -4110,19 +4110,19 @@
         <v>49</v>
       </c>
       <c r="B51" s="1">
-        <v>7.92483138845691E-7</v>
+        <v>0.38770181690050598</v>
       </c>
       <c r="C51">
         <f t="shared" si="0"/>
-        <v>1.0000007924834529</v>
+        <v>1.4735903190421269</v>
       </c>
       <c r="D51">
-        <f t="shared" si="1"/>
-        <v>33.964212639920461</v>
+        <f t="shared" si="2"/>
+        <v>34.351913664337822</v>
       </c>
       <c r="E51">
-        <f t="shared" si="2"/>
-        <v>562950399549836.25</v>
+        <f t="shared" si="1"/>
+        <v>829557601466858</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.2">
@@ -4131,19 +4131,19 @@
         <v>50</v>
       </c>
       <c r="B52" s="1">
-        <v>7.9210524542877504E-7</v>
+        <v>0.398257143077766</v>
       </c>
       <c r="C52">
         <f t="shared" si="0"/>
-        <v>1.0000007921055591</v>
+        <v>1.4892269250707522</v>
       </c>
       <c r="D52">
-        <f t="shared" si="1"/>
-        <v>34.657359820102513</v>
+        <f t="shared" si="2"/>
+        <v>35.05561617107503</v>
       </c>
       <c r="E52">
-        <f t="shared" si="2"/>
-        <v>1125900798674202.2</v>
+        <f t="shared" si="1"/>
+        <v>1676720456204685</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.2">
@@ -4152,19 +4152,19 @@
         <v>51</v>
       </c>
       <c r="B53" s="1">
-        <v>7.9178726581593705E-7</v>
+        <v>0.40889211562518502</v>
       </c>
       <c r="C53">
         <f t="shared" si="0"/>
-        <v>1.0000007917875793</v>
+        <v>1.5051493296315688</v>
       </c>
       <c r="D53">
-        <f t="shared" si="1"/>
-        <v>35.350507000344471</v>
+        <f t="shared" si="2"/>
+        <v>35.759398324182392</v>
       </c>
       <c r="E53">
-        <f t="shared" si="2"/>
-        <v>2251801596632360</v>
+        <f t="shared" si="1"/>
+        <v>3389294980032830</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.2">
@@ -4173,19 +4173,19 @@
         <v>52</v>
       </c>
       <c r="B54" s="1">
-        <v>7.93265178658044E-7</v>
+        <v>0.41960677262222601</v>
       </c>
       <c r="C54">
         <f t="shared" si="0"/>
-        <v>1.0000007932654933</v>
+        <v>1.5213631963203842</v>
       </c>
       <c r="D54">
-        <f t="shared" si="1"/>
-        <v>36.043654182382333</v>
+        <f t="shared" si="2"/>
+        <v>36.463260161739377</v>
       </c>
       <c r="E54">
-        <f t="shared" si="2"/>
-        <v>4503603199920670</v>
+        <f t="shared" si="1"/>
+        <v>6851610724043637</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.2">
@@ -4194,19 +4194,19 @@
         <v>53</v>
       </c>
       <c r="B55" s="1">
-        <v>7.9388612412659298E-7</v>
+        <v>0.43040178640343202</v>
       </c>
       <c r="C55">
         <f t="shared" si="0"/>
-        <v>1.0000007938864393</v>
+        <v>1.5378752968179561</v>
       </c>
       <c r="D55">
-        <f t="shared" si="1"/>
-        <v>36.736801363563224</v>
+        <f t="shared" si="2"/>
+        <v>37.16720235608053</v>
       </c>
       <c r="E55">
-        <f t="shared" si="2"/>
-        <v>9007206405434320</v>
+        <f t="shared" si="1"/>
+        <v>1.3851949227383228E+16</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.2">
@@ -4215,19 +4215,19 @@
         <v>54</v>
       </c>
       <c r="B56" s="1">
-        <v>7.9589920889067797E-7</v>
+        <v>0.44127775545689402</v>
       </c>
       <c r="C56">
         <f t="shared" si="0"/>
-        <v>1.0000007958995256</v>
+        <v>1.5546924666934938</v>
       </c>
       <c r="D56">
-        <f t="shared" si="1"/>
-        <v>37.429948546136259</v>
+        <f t="shared" si="2"/>
+        <v>37.871225505693943</v>
       </c>
       <c r="E56">
-        <f t="shared" si="2"/>
-        <v>1.801441284713328E+16</v>
+        <f t="shared" si="1"/>
+        <v>2.80068496547062E+16</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.2">
@@ -4236,19 +4236,19 @@
         <v>55</v>
       </c>
       <c r="B57" s="1">
-        <v>7.9796073153240096E-7</v>
+        <v>0.45223419121730002</v>
       </c>
       <c r="C57">
         <f t="shared" si="0"/>
-        <v>1.0000007979610499</v>
+        <v>1.5718200119193337</v>
       </c>
       <c r="D57">
-        <f t="shared" si="1"/>
-        <v>38.123095728757718</v>
+        <f t="shared" si="2"/>
+        <v>38.575329122014288</v>
       </c>
       <c r="E57">
-        <f t="shared" si="2"/>
-        <v>3.602882576854048E+16</v>
+        <f t="shared" si="1"/>
+        <v>5.6630784159786992E+16</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.2">
@@ -4257,19 +4257,19 @@
         <v>56</v>
       </c>
       <c r="B58" s="1">
-        <v>8.0206451400498197E-7</v>
+        <v>0.46327135351659898</v>
       </c>
       <c r="C58">
         <f t="shared" si="0"/>
-        <v>1.0000008020648357</v>
+        <v>1.5892645364311948</v>
       </c>
       <c r="D58">
-        <f t="shared" si="1"/>
-        <v>38.816242913421448</v>
+        <f t="shared" si="2"/>
+        <v>39.279513464873531</v>
       </c>
       <c r="E58">
-        <f t="shared" si="2"/>
-        <v>7.205765183279E+16</v>
+        <f t="shared" si="1"/>
+        <v>1.1451857878503419E+17</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.2">
@@ -4278,19 +4278,19 @@
         <v>57</v>
       </c>
       <c r="B59" s="1">
-        <v>8.0563980097294103E-7</v>
+        <v>0.47438941214729302</v>
       </c>
       <c r="C59">
         <f t="shared" si="0"/>
-        <v>1.0000008056401255</v>
+        <v>1.6070326632367569</v>
       </c>
       <c r="D59">
-        <f t="shared" si="1"/>
-        <v>39.509390097556683</v>
+        <f t="shared" si="2"/>
+        <v>39.983778704064179</v>
       </c>
       <c r="E59">
-        <f t="shared" si="2"/>
-        <v>1.4411530418083392E+17</v>
+        <f t="shared" si="1"/>
+        <v>2.3159781450640944E+17</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.2">
@@ -4299,19 +4299,19 @@
         <v>58</v>
       </c>
       <c r="B60" s="1">
-        <v>8.1113954163078197E-7</v>
+        <v>0.48558886092168602</v>
       </c>
       <c r="C60">
         <f t="shared" si="0"/>
-        <v>1.0000008111398706</v>
+        <v>1.6251317036893758</v>
       </c>
       <c r="D60">
-        <f t="shared" si="1"/>
-        <v>40.202537283616373</v>
+        <f t="shared" si="2"/>
+        <v>40.688125333398517</v>
       </c>
       <c r="E60">
-        <f t="shared" si="2"/>
-        <v>2.8823060994686266E+17</v>
+        <f t="shared" si="1"/>
+        <v>4.684123222504624E+17</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.2">
@@ -4320,19 +4320,19 @@
         <v>59</v>
       </c>
       <c r="B61" s="1">
-        <v>8.1498762235361097E-7</v>
+        <v>0.49687014610514302</v>
       </c>
       <c r="C61">
         <f t="shared" si="0"/>
-        <v>1.0000008149879545</v>
+        <v>1.6435690810158663</v>
       </c>
       <c r="D61">
-        <f t="shared" si="1"/>
-        <v>40.895684468024392</v>
+        <f t="shared" si="2"/>
+        <v>41.392553799141915</v>
       </c>
       <c r="E61">
-        <f t="shared" si="2"/>
-        <v>5.7646122211199066E+17</v>
+        <f t="shared" si="1"/>
+        <v>9.4745306890505126E+17</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.2">
@@ -4341,19 +4341,19 @@
         <v>60</v>
       </c>
       <c r="B62" s="1">
-        <v>8.2130497959605501E-7</v>
+        <v>0.50823460174650104</v>
       </c>
       <c r="C62">
         <f t="shared" si="0"/>
-        <v>1.0000008213053169</v>
+        <v>1.6623538863014127</v>
       </c>
       <c r="D62">
-        <f t="shared" si="1"/>
-        <v>41.588831654901696</v>
+        <f t="shared" si="2"/>
+        <v>42.097065435343218</v>
       </c>
       <c r="E62">
-        <f t="shared" si="2"/>
-        <v>1.1529224515074066E+18</v>
+        <f t="shared" si="1"/>
+        <v>1.9165635437836613E+18</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.2">
@@ -4362,19 +4362,19 @@
         <v>61</v>
       </c>
       <c r="B63" s="1">
-        <v>8.2756417648131005E-7</v>
+        <v>0.51968270789608495</v>
       </c>
       <c r="C63">
         <f t="shared" si="0"/>
-        <v>1.0000008275645189</v>
+        <v>1.6814940402665766</v>
       </c>
       <c r="D63">
-        <f t="shared" si="1"/>
-        <v>42.281978841720843</v>
+        <f t="shared" si="2"/>
+        <v>42.801660722052752</v>
       </c>
       <c r="E63">
-        <f t="shared" si="2"/>
-        <v>2.3058449174475602E+18</v>
+        <f t="shared" si="1"/>
+        <v>3.8772612777831869E+18</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.2">
@@ -4383,19 +4383,19 @@
         <v>62</v>
       </c>
       <c r="B64" s="1">
-        <v>8.3573223302516803E-7</v>
+        <v>0.531215077791243</v>
       </c>
       <c r="C64">
         <f t="shared" si="0"/>
-        <v>1.0000008357325822</v>
+        <v>1.7009978982074572</v>
       </c>
       <c r="D64">
-        <f t="shared" si="1"/>
-        <v>42.975126030448841</v>
+        <f t="shared" si="2"/>
+        <v>43.506340272507856</v>
       </c>
       <c r="E64">
-        <f t="shared" si="2"/>
-        <v>4.6116898725636475E+18</v>
+        <f t="shared" si="1"/>
+        <v>7.8444682245377341E+18</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.2">
@@ -4404,19 +4404,19 @@
         <v>63</v>
       </c>
       <c r="B65" s="1">
-        <v>8.4353839040831401E-7</v>
+        <v>0.54283211810683896</v>
       </c>
       <c r="C65">
         <f t="shared" si="0"/>
-        <v>1.0000008435387462</v>
+        <v>1.7208736847458395</v>
       </c>
       <c r="D65">
-        <f t="shared" si="1"/>
-        <v>43.668273218814939</v>
+        <f t="shared" si="2"/>
+        <v>44.211104493383388</v>
       </c>
       <c r="E65">
-        <f t="shared" si="2"/>
-        <v>9.223379817126402E+18</v>
+        <f t="shared" si="1"/>
+        <v>1.5872258222843933E+19</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.2">
@@ -4425,19 +4425,19 @@
         <v>64</v>
       </c>
       <c r="B66" s="1">
-        <v>8.5385612098125999E-7</v>
+        <v>0.55453460294763002</v>
       </c>
       <c r="C66">
         <f t="shared" si="0"/>
-        <v>1.0000008538564855</v>
+        <v>1.7411304791924427</v>
       </c>
       <c r="D66">
-        <f t="shared" si="1"/>
-        <v>44.36142040969262</v>
+        <f t="shared" si="2"/>
+        <v>44.915954158784132</v>
       </c>
       <c r="E66">
-        <f t="shared" si="2"/>
-        <v>1.8446759824581603E+19</v>
+        <f t="shared" si="1"/>
+        <v>3.2118188348598325E+19</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.2">
@@ -4446,19 +4446,19 @@
         <v>65</v>
       </c>
       <c r="B67" s="1">
-        <v>8.6288610376327401E-7</v>
+        <v>0.56632334301769705</v>
       </c>
       <c r="C67">
         <f t="shared" ref="C67:C102" si="4">EXP(B67)</f>
-        <v>1.000000862886476</v>
+        <v>1.7617776769446922</v>
       </c>
       <c r="D67">
         <f t="shared" ref="D67:D102" si="5">B67+A67*LN(2/1)</f>
-        <v>45.054567599282549</v>
+        <v>45.620890079414146</v>
       </c>
       <c r="E67">
-        <f t="shared" ref="E67:E130" si="6">EXP(D67)</f>
-        <v>3.6893519982311096E+19</v>
+        <f t="shared" ref="E67:E102" si="6">EXP(D67)</f>
+        <v>6.4998123842746786E+19</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.2">
@@ -4467,40 +4467,40 @@
         <v>66</v>
       </c>
       <c r="B68" s="1">
-        <v>8.7446488207761504E-7</v>
+        <v>0.57819999131163502</v>
       </c>
       <c r="C68">
         <f t="shared" si="4"/>
-        <v>1.0000008744652644</v>
+        <v>1.7828264377318859</v>
       </c>
       <c r="D68">
         <f t="shared" si="5"/>
-        <v>45.747714791421267</v>
+        <v>46.325913908268021</v>
       </c>
       <c r="E68">
         <f t="shared" si="6"/>
-        <v>7.3787040818985501E+19</v>
+        <v>1.3154937209873287E+20</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A69">
-        <f t="shared" ref="A69:A132" si="7">A68+1</f>
+        <f t="shared" ref="A69:A102" si="7">A68+1</f>
         <v>67</v>
       </c>
       <c r="B69" s="1">
-        <v>8.8661717875962101E-7</v>
+        <v>0.59016608904433698</v>
       </c>
       <c r="C69">
         <f t="shared" si="4"/>
-        <v>1.0000008866175718</v>
+        <v>1.8042880629931679</v>
       </c>
       <c r="D69">
         <f t="shared" si="5"/>
-        <v>46.440861984133512</v>
+        <v>47.031027186560671</v>
       </c>
       <c r="E69">
         <f t="shared" si="6"/>
-        <v>1.4757408343133562E+20</v>
+        <v>2.6626592106627236E+20</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.2">
@@ -4509,19 +4509,19 @@
         <v>68</v>
       </c>
       <c r="B70" s="1">
-        <v>9.0062625035577897E-7</v>
+        <v>0.60222228904317299</v>
       </c>
       <c r="C70">
         <f t="shared" si="4"/>
-        <v>1.0000009006266559</v>
+        <v>1.8261725777001043</v>
       </c>
       <c r="D70">
         <f t="shared" si="5"/>
-        <v>47.134009178702527</v>
+        <v>47.736230567119456</v>
       </c>
       <c r="E70">
         <f t="shared" si="6"/>
-        <v>2.9514817099742242E+20</v>
+        <v>5.389910108041659E+20</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.2">
@@ -4530,19 +4530,19 @@
         <v>69</v>
       </c>
       <c r="B71" s="1">
-        <v>9.1488420533047097E-7</v>
+        <v>0.61437071018838296</v>
       </c>
       <c r="C71">
         <f t="shared" si="4"/>
-        <v>1.0000009148846238</v>
+        <v>1.8484929956656715</v>
       </c>
       <c r="D71">
         <f t="shared" si="5"/>
-        <v>47.827156373520431</v>
+        <v>48.441526168824609</v>
       </c>
       <c r="E71">
         <f t="shared" si="6"/>
-        <v>5.9029635041126567E+20</v>
+        <v>1.0911576708188587E+21</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.2">
@@ -4551,19 +4551,19 @@
         <v>70</v>
       </c>
       <c r="B72" s="1">
-        <v>9.3240658334827296E-7</v>
+        <v>0.62661169392911398</v>
       </c>
       <c r="C72">
         <f t="shared" si="4"/>
-        <v>1.000000932407018</v>
+        <v>1.8712594258419737</v>
       </c>
       <c r="D72">
         <f t="shared" si="5"/>
-        <v>48.520303571602753</v>
+        <v>49.146914333125281</v>
       </c>
       <c r="E72">
         <f t="shared" si="6"/>
-        <v>1.1805927215093213E+21</v>
+        <v>2.2091931983374978E+21</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.2">
@@ -4572,19 +4572,19 @@
         <v>71</v>
       </c>
       <c r="B73" s="1">
-        <v>9.4896422923686396E-7</v>
+        <v>0.63894856873766603</v>
       </c>
       <c r="C73">
         <f t="shared" si="4"/>
-        <v>1.0000009489646795</v>
+        <v>1.8944879079398345</v>
       </c>
       <c r="D73">
         <f t="shared" si="5"/>
-        <v>49.213450768720342</v>
+        <v>49.852398388493782</v>
       </c>
       <c r="E73">
         <f t="shared" si="6"/>
-        <v>2.3611854821143117E+21</v>
+        <v>4.4732330993284494E+21</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.2">
@@ -4593,19 +4593,19 @@
         <v>72</v>
       </c>
       <c r="B74" s="1">
-        <v>9.6785511219731091E-7</v>
+        <v>0.65138271507977996</v>
       </c>
       <c r="C74">
         <f t="shared" si="4"/>
-        <v>1.0000009678555806</v>
+        <v>1.918191308210597</v>
       </c>
       <c r="D74">
         <f t="shared" si="5"/>
-        <v>49.906597968171177</v>
+        <v>50.557979715395838</v>
       </c>
       <c r="E74">
         <f t="shared" si="6"/>
-        <v>4.7223710534384096E+21</v>
+        <v>9.0584023416255629E+21</v>
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.2">
@@ -4614,19 +4614,19 @@
         <v>73</v>
       </c>
       <c r="B75" s="1">
-        <v>9.88202346178902E-7</v>
+        <v>0.663916497749382</v>
       </c>
       <c r="C75">
         <f t="shared" si="4"/>
-        <v>1.0000009882028345</v>
+        <v>1.9423848024622326</v>
       </c>
       <c r="D75">
         <f t="shared" si="5"/>
-        <v>50.599745169078354</v>
+        <v>51.263660678625392</v>
       </c>
       <c r="E75">
         <f t="shared" si="6"/>
-        <v>9.4447422990511757E+21</v>
+        <v>1.8345305775966094E+22</v>
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.2">
@@ -4635,19 +4635,19 @@
         <v>74</v>
       </c>
       <c r="B76" s="1">
-        <v>1.0111647758297501E-6</v>
+        <v>0.67655073749878003</v>
       </c>
       <c r="C76">
         <f t="shared" si="4"/>
-        <v>1.0000010111652871</v>
+        <v>1.9670810383159851</v>
       </c>
       <c r="D76">
         <f t="shared" si="5"/>
-        <v>51.292892372600726</v>
+        <v>51.969442098934728</v>
       </c>
       <c r="E76">
         <f t="shared" si="6"/>
-        <v>1.8889485031850763E+22</v>
+        <v>3.715711025772713E+22</v>
       </c>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.2">
@@ -4656,19 +4656,19 @@
         <v>75</v>
       </c>
       <c r="B77" s="1">
-        <v>1.0368609242601199E-6</v>
+        <v>0.68928746251601203</v>
       </c>
       <c r="C77">
         <f t="shared" si="4"/>
-        <v>1.0000010368614618</v>
+        <v>1.9922954421873744</v>
       </c>
       <c r="D77">
         <f t="shared" si="5"/>
-        <v>51.986039578856818</v>
+        <v>52.675326004511909</v>
       </c>
       <c r="E77">
         <f t="shared" si="6"/>
-        <v>3.7778971034475527E+22</v>
+        <v>7.5266793761276844E+22</v>
       </c>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.2">
@@ -4677,19 +4677,19 @@
         <v>76</v>
       </c>
       <c r="B78" s="1">
-        <v>1.0622877748431001E-6</v>
+        <v>0.70212963383481197</v>
       </c>
       <c r="C78">
         <f t="shared" si="4"/>
-        <v>1.0000010622883391</v>
+        <v>2.0180458331415276</v>
       </c>
       <c r="D78">
         <f t="shared" si="5"/>
-        <v>52.679186784843615</v>
+        <v>53.381315356390658</v>
       </c>
       <c r="E78">
         <f t="shared" si="6"/>
-        <v>7.5557943990151666E+22</v>
+        <v>1.5247923205315718E+23</v>
       </c>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.2">
@@ -4698,19 +4698,19 @@
         <v>77</v>
       </c>
       <c r="B79" s="1">
-        <v>1.0966998655094E-6</v>
+        <v>0.71508178590709104</v>
       </c>
       <c r="C79">
         <f t="shared" si="4"/>
-        <v>1.0000010967004669</v>
+        <v>2.0443538747575305</v>
       </c>
       <c r="D79">
         <f t="shared" si="5"/>
-        <v>53.372333999815659</v>
+        <v>54.087414689022879</v>
       </c>
       <c r="E79">
         <f t="shared" si="6"/>
-        <v>1.511158931805182E+23</v>
+        <v>3.0893402295294848E+23</v>
       </c>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.2">
@@ -4719,19 +4719,19 @@
         <v>78</v>
       </c>
       <c r="B80" s="1">
-        <v>1.1249675869138299E-6</v>
+        <v>0.72814716902744403</v>
       </c>
       <c r="C80">
         <f t="shared" si="4"/>
-        <v>1.0000011249682197</v>
+        <v>2.0712393937126756</v>
       </c>
       <c r="D80">
         <f t="shared" si="5"/>
-        <v>54.06548120864332</v>
+        <v>54.793627252703175</v>
       </c>
       <c r="E80">
         <f t="shared" si="6"/>
-        <v>3.0223179490443865E+23</v>
+        <v>6.2599369541554872E+23</v>
       </c>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.2">
@@ -4740,19 +4740,19 @@
         <v>79</v>
       </c>
       <c r="B81" s="1">
-        <v>1.16308349725687E-6</v>
+        <v>0.74132923145485496</v>
       </c>
       <c r="C81">
         <f t="shared" si="4"/>
-        <v>1.0000011630841736</v>
+        <v>2.0987233503366491</v>
       </c>
       <c r="D81">
         <f t="shared" si="5"/>
-        <v>54.758628427319174</v>
+        <v>55.499956495690533</v>
       </c>
       <c r="E81">
         <f t="shared" si="6"/>
-        <v>6.0446361284855666E+23</v>
+        <v>1.2686004232250454E+24</v>
       </c>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.2">
@@ -4761,19 +4761,19 @@
         <v>80</v>
       </c>
       <c r="B82" s="1">
-        <v>1.2029272030851499E-6</v>
+        <v>0.75463314850984597</v>
       </c>
       <c r="C82">
         <f t="shared" si="4"/>
-        <v>1.0000012029279266</v>
+        <v>2.1268311490469771</v>
       </c>
       <c r="D82">
         <f t="shared" si="5"/>
-        <v>55.451775647722826</v>
+        <v>56.206407593305471</v>
       </c>
       <c r="E82">
         <f t="shared" si="6"/>
-        <v>1.2089272738652566E+24</v>
+        <v>2.5711810900435409E+24</v>
       </c>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.2">
@@ -4782,19 +4782,19 @@
         <v>81</v>
       </c>
       <c r="B83" s="1">
-        <v>1.2484293197884999E-6</v>
+        <v>0.76806447844645198</v>
       </c>
       <c r="C83">
         <f t="shared" si="4"/>
-        <v>1.0000012484300991</v>
+        <v>2.1555900225466407</v>
       </c>
       <c r="D83">
         <f t="shared" si="5"/>
-        <v>56.144922873784886</v>
+        <v>56.912986103802019</v>
       </c>
       <c r="E83">
         <f t="shared" si="6"/>
-        <v>2.4178546577480097E+24</v>
+        <v>5.2118968695206162E+24</v>
       </c>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.2">
@@ -4803,19 +4803,19 @@
         <v>82</v>
       </c>
       <c r="B84" s="1">
-        <v>1.29768926959111E-6</v>
+        <v>0.78162489894026199</v>
       </c>
       <c r="C84">
         <f t="shared" si="4"/>
-        <v>1.0000012976901116</v>
+        <v>2.1850198188979504</v>
       </c>
       <c r="D84">
         <f t="shared" si="5"/>
-        <v>56.838070103604778</v>
+        <v>57.619693704855777</v>
       </c>
       <c r="E84">
         <f t="shared" si="6"/>
-        <v>4.8357095537028105E+24</v>
+        <v>1.0566107501741651E+25</v>
       </c>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.2">
@@ -4824,19 +4824,19 @@
         <v>83</v>
       </c>
       <c r="B85" s="1">
-        <v>1.35212882538034E-6</v>
+        <v>0.79532327901213595</v>
       </c>
       <c r="C85">
         <f t="shared" si="4"/>
-        <v>1.0000013521297395</v>
+        <v>2.215156994829286</v>
       </c>
       <c r="D85">
         <f t="shared" si="5"/>
-        <v>57.531217338604286</v>
+        <v>58.326539265487597</v>
       </c>
       <c r="E85">
         <f t="shared" si="6"/>
-        <v>9.6714196339134597E+24</v>
+        <v>2.1423683884392587E+25</v>
       </c>
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.2">
@@ -4845,19 +4845,19 @@
         <v>84</v>
       </c>
       <c r="B86" s="1">
-        <v>1.41405414275953E-6</v>
+        <v>0.80916198042009801</v>
       </c>
       <c r="C86">
         <f t="shared" si="4"/>
-        <v>1.0000014140551425</v>
+        <v>2.2460249848762062</v>
       </c>
       <c r="D86">
         <f t="shared" si="5"/>
-        <v>58.224364581089546</v>
+        <v>59.033525147455506</v>
       </c>
       <c r="E86">
         <f t="shared" si="6"/>
-        <v>1.9342840465638366E+25</v>
+        <v>4.3444441531462554E+25</v>
       </c>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.2">
@@ -4866,19 +4866,19 @@
         <v>85</v>
       </c>
       <c r="B87" s="1">
-        <v>1.48249287113554E-6</v>
+        <v>0.82315100125713003</v>
       </c>
       <c r="C87">
         <f t="shared" si="4"/>
-        <v>1.00000148249397</v>
+        <v>2.2776654689026641</v>
       </c>
       <c r="D87">
         <f t="shared" si="5"/>
-        <v>58.917511830088216</v>
+        <v>59.740661348852477</v>
       </c>
       <c r="E87">
         <f t="shared" si="6"/>
-        <v>3.8685683578875502E+25</v>
+        <v>8.8112915001634544E+25</v>
       </c>
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.2">
@@ -4887,19 +4887,19 @@
         <v>86</v>
       </c>
       <c r="B88" s="1">
-        <v>1.56529919531051E-6</v>
+        <v>0.83729724243879899</v>
       </c>
       <c r="C88">
         <f t="shared" si="4"/>
-        <v>1.0000015653004204</v>
+        <v>2.3101148512158307</v>
       </c>
       <c r="D88">
         <f t="shared" si="5"/>
-        <v>59.610659093454487</v>
+        <v>60.447954770594094</v>
       </c>
       <c r="E88">
         <f t="shared" si="6"/>
-        <v>7.7371373564589867E+25</v>
+        <v>1.7873647935424145E+26</v>
       </c>
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.2">
@@ -4908,19 +4908,19 @@
         <v>87</v>
       </c>
       <c r="B89" s="1">
-        <v>1.65780432100715E-6</v>
+        <v>0.85161250246647102</v>
       </c>
       <c r="C89">
         <f t="shared" si="4"/>
-        <v>1.0000016578056952</v>
+        <v>2.3434225816139835</v>
       </c>
       <c r="D89">
         <f t="shared" si="5"/>
-        <v>60.303806366519559</v>
+        <v>61.155417211181714</v>
       </c>
       <c r="E89">
         <f t="shared" si="6"/>
-        <v>1.5474276144367791E+26</v>
+        <v>3.626270803431831E+26</v>
       </c>
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.2">
@@ -4929,19 +4929,19 @@
         <v>88</v>
       </c>
       <c r="B90" s="1">
-        <v>1.7655413988190401E-6</v>
+        <v>0.86610470666871797</v>
       </c>
       <c r="C90">
         <f t="shared" si="4"/>
-        <v>1.0000017655429574</v>
+        <v>2.3776312207735235</v>
       </c>
       <c r="D90">
         <f t="shared" si="5"/>
-        <v>60.996953654816586</v>
+        <v>61.863056595943902</v>
       </c>
       <c r="E90">
         <f t="shared" si="6"/>
-        <v>3.0948555623042464E+26</v>
+        <v>7.3584122171262853E+26</v>
       </c>
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.2">
@@ -4950,19 +4950,19 @@
         <v>89</v>
       </c>
       <c r="B91" s="1">
-        <v>1.8919668035779501E-6</v>
+        <v>0.88078813374180198</v>
       </c>
       <c r="C91">
         <f t="shared" si="4"/>
-        <v>1.0000018919685933</v>
+        <v>2.4128005667916437</v>
       </c>
       <c r="D91">
         <f t="shared" si="5"/>
-        <v>61.690100961801932</v>
+        <v>62.57088720357693</v>
       </c>
       <c r="E91">
         <f t="shared" si="6"/>
-        <v>6.1897119071452478E+26</v>
+        <v>1.4934512142209113E+27</v>
       </c>
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.2">
@@ -4971,19 +4971,19 @@
         <v>90</v>
       </c>
       <c r="B92" s="1">
-        <v>2.0443480421658999E-6</v>
+        <v>0.89567278830324104</v>
       </c>
       <c r="C92">
         <f t="shared" si="4"/>
-        <v>1.0000020443501318</v>
+        <v>2.4489828823658555</v>
       </c>
       <c r="D92">
         <f t="shared" si="5"/>
-        <v>62.383248294743119</v>
+        <v>63.278919038698319</v>
       </c>
       <c r="E92">
         <f t="shared" si="6"/>
-        <v>1.2379425700682614E+27</v>
+        <v>3.0316939656052126E+27</v>
       </c>
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.2">
@@ -4992,19 +4992,19 @@
         <v>91</v>
       </c>
       <c r="B93" s="1">
-        <v>2.2182367902175198E-6</v>
+        <v>0.91077807165763203</v>
       </c>
       <c r="C93">
         <f t="shared" si="4"/>
-        <v>1.0000022182392505</v>
+        <v>2.4862562665303809</v>
       </c>
       <c r="D93">
         <f t="shared" si="5"/>
-        <v>63.076395649191809</v>
+        <v>63.987171502612654</v>
       </c>
       <c r="E93">
         <f t="shared" si="6"/>
-        <v>2.4758855706651205E+27</v>
+        <v>6.1556723605242764E+27</v>
       </c>
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.2">
@@ -5013,19 +5013,19 @@
         <v>92</v>
       </c>
       <c r="B94" s="1">
-        <v>2.4352734752235898E-6</v>
+        <v>0.926124580438353</v>
       </c>
       <c r="C94">
         <f t="shared" si="4"/>
-        <v>1.0000024352764405</v>
+        <v>2.5247058993494416</v>
       </c>
       <c r="D94">
         <f t="shared" si="5"/>
-        <v>63.769543046788442</v>
+        <v>64.695665191953324</v>
       </c>
       <c r="E94">
         <f t="shared" si="6"/>
-        <v>4.9517722160463631E+27</v>
+        <v>1.2501738080898751E+28</v>
       </c>
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.2">
@@ -5034,19 +5034,19 @@
         <v>93</v>
       </c>
       <c r="B95" s="1">
-        <v>2.7136931600584598E-6</v>
+        <v>0.94174293915958196</v>
       </c>
       <c r="C95">
         <f t="shared" si="4"/>
-        <v>1.0000027136968421</v>
+        <v>2.5644472008541737</v>
       </c>
       <c r="D95">
         <f t="shared" si="5"/>
-        <v>64.46269050576808</v>
+        <v>65.404430731234498</v>
       </c>
       <c r="E95">
         <f t="shared" si="6"/>
-        <v>9.9035471894349066E+27</v>
+        <v>2.539705494856566E+28</v>
       </c>
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.2">
@@ -5055,19 +5055,19 @@
         <v>94</v>
       </c>
       <c r="B96" s="1">
-        <v>3.0718332854363599E-6</v>
+        <v>0.95767219482097998</v>
       </c>
       <c r="C96">
         <f t="shared" si="4"/>
-        <v>1.0000030718380035</v>
+        <v>2.6056240233286982</v>
       </c>
       <c r="D96">
         <f t="shared" si="5"/>
-        <v>65.155838044468155</v>
+        <v>66.11350716745585</v>
       </c>
       <c r="E96">
         <f t="shared" si="6"/>
-        <v>1.9807101472586427E+28</v>
+        <v>5.160970089283993E+28</v>
       </c>
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.2">
@@ -5076,19 +5076,19 @@
         <v>95</v>
       </c>
       <c r="B97" s="1">
-        <v>3.53872694294311E-6</v>
+        <v>0.97396568286666296</v>
       </c>
       <c r="C97">
         <f t="shared" si="4"/>
-        <v>1.0000035387332042</v>
+        <v>2.6484264809493006</v>
       </c>
       <c r="D97">
         <f t="shared" si="5"/>
-        <v>65.84898569192174</v>
+        <v>66.822947836061459</v>
       </c>
       <c r="E97">
         <f t="shared" si="6"/>
-        <v>3.9614221440796588E+28</v>
+        <v>1.0491498181986535E+29</v>
       </c>
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.2">
@@ -5097,19 +5097,19 @@
         <v>96</v>
       </c>
       <c r="B98" s="1">
-        <v>4.2097198220971604E-6</v>
+        <v>0.99067265034763596</v>
       </c>
       <c r="C98">
         <f t="shared" si="4"/>
-        <v>1.000004209728683</v>
+        <v>2.6930453411251349</v>
       </c>
       <c r="D98">
         <f t="shared" si="5"/>
-        <v>66.542133543474563</v>
+        <v>67.532801984102377</v>
       </c>
       <c r="E98">
         <f t="shared" si="6"/>
-        <v>7.922849604333187E+28</v>
+        <v>2.1336503394494291E+29</v>
       </c>
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.2">
@@ -5118,19 +5118,19 @@
         <v>97</v>
       </c>
       <c r="B99" s="1">
-        <v>5.2214549583467001E-6</v>
+        <v>1.00789388886077</v>
       </c>
       <c r="C99">
         <f t="shared" si="4"/>
-        <v>1.0000052214685902</v>
+        <v>2.7398245591995001</v>
       </c>
       <c r="D99">
         <f t="shared" si="5"/>
-        <v>67.235281735769647</v>
+        <v>68.243170403175455</v>
       </c>
       <c r="E99">
         <f t="shared" si="6"/>
-        <v>1.5845715240325167E+29</v>
+        <v>4.3414253087365686E+29</v>
       </c>
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.2">
@@ -5139,19 +5139,19 @@
         <v>98</v>
       </c>
       <c r="B100" s="1">
-        <v>6.86494928525612E-6</v>
+        <v>1.0257924047448601</v>
       </c>
       <c r="C100">
         <f t="shared" si="4"/>
-        <v>1.0000068649728491</v>
+        <v>2.7893048434803265</v>
       </c>
       <c r="D100">
         <f t="shared" si="5"/>
-        <v>67.928430559823923</v>
+        <v>68.954216099619501</v>
       </c>
       <c r="E100">
         <f t="shared" si="6"/>
-        <v>3.1691482565379468E+29</v>
+        <v>8.8396598976433625E+29</v>
       </c>
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.2">
@@ -5160,19 +5160,19 @@
         <v>99</v>
       </c>
       <c r="B101" s="1">
-        <v>1.02310686863785E-5</v>
+        <v>1.0447255818697401</v>
       </c>
       <c r="C101">
         <f t="shared" si="4"/>
-        <v>1.0000102311210239</v>
+        <v>2.8426183505970362</v>
       </c>
       <c r="D101">
         <f t="shared" si="5"/>
-        <v>68.621581106503271</v>
+        <v>69.666296457304327</v>
       </c>
       <c r="E101">
         <f t="shared" si="6"/>
-        <v>6.3383178485746764E+29</v>
+        <v>1.8017234291770581E+30</v>
       </c>
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.2">
@@ -5181,19 +5181,19 @@
         <v>100</v>
       </c>
       <c r="B102" s="1">
-        <v>2.0362658956809999E-5</v>
+        <v>1.06560997912587</v>
       </c>
       <c r="C102">
         <f t="shared" si="4"/>
-        <v>1.0000203628662772</v>
+        <v>2.9026089750613213</v>
       </c>
       <c r="D102">
         <f t="shared" si="5"/>
-        <v>69.314738418653491</v>
+        <v>70.380328035120399</v>
       </c>
       <c r="E102">
         <f t="shared" si="6"/>
-        <v>1.2676764132278917E+30</v>
+        <v>3.6794940094643246E+30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
SUS works for LG
</commit_message>
<xml_diff>
--- a/Data/Lgas_10_10/analysis.xlsx
+++ b/Data/Lgas_10_10/analysis.xlsx
@@ -70,7 +70,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>idx</t>
   </si>
@@ -79,6 +79,30 @@
   </si>
   <si>
     <t>P(N)</t>
+  </si>
+  <si>
+    <t>F(N=2)</t>
+  </si>
+  <si>
+    <t>P(n=2)</t>
+  </si>
+  <si>
+    <t>F(N=3)</t>
+  </si>
+  <si>
+    <t>P(n=3)</t>
+  </si>
+  <si>
+    <t>F(N=4)</t>
+  </si>
+  <si>
+    <t>F(N=5)</t>
+  </si>
+  <si>
+    <t>P(N=5</t>
+  </si>
+  <si>
+    <t>P(N=4)</t>
   </si>
 </sst>
 </file>
@@ -539,11 +563,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2145867872"/>
-        <c:axId val="-2130533712"/>
+        <c:axId val="-2117160800"/>
+        <c:axId val="-2119546688"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2145867872"/>
+        <c:axId val="-2117160800"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -599,12 +623,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2130533712"/>
+        <c:crossAx val="-2119546688"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2130533712"/>
+        <c:axId val="-2119546688"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -661,7 +685,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2145867872"/>
+        <c:crossAx val="-2117160800"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1119,11 +1143,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2122125008"/>
-        <c:axId val="-2122082080"/>
+        <c:axId val="-2118896432"/>
+        <c:axId val="-2121846032"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2122125008"/>
+        <c:axId val="-2118896432"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1179,12 +1203,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2122082080"/>
+        <c:crossAx val="-2121846032"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2122082080"/>
+        <c:axId val="-2121846032"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1241,7 +1265,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2122125008"/>
+        <c:crossAx val="-2118896432"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2406,16 +2430,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>547806</xdr:colOff>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>339299</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>2653</xdr:rowOff>
+      <xdr:rowOff>97429</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>115626</xdr:colOff>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>741149</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>35256</xdr:rowOff>
+      <xdr:rowOff>130032</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2436,16 +2460,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>94776</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>97429</xdr:rowOff>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>170597</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>2653</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>94776</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>130032</xdr:rowOff>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>170597</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>35256</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2734,18 +2758,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C102"/>
+  <dimension ref="A1:O102"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="67" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" topLeftCell="B73" zoomScale="50" workbookViewId="0">
+      <selection activeCell="Q96" sqref="Q96"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="26" customWidth="1"/>
+    <col min="8" max="8" width="12" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.33203125" customWidth="1"/>
+    <col min="12" max="12" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2755,8 +2785,32 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" t="s">
+        <v>6</v>
+      </c>
+      <c r="K1" t="s">
+        <v>7</v>
+      </c>
+      <c r="L1" t="s">
+        <v>10</v>
+      </c>
+      <c r="N1" t="s">
+        <v>8</v>
+      </c>
+      <c r="O1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>0</v>
       </c>
@@ -2767,8 +2821,40 @@
         <f>EXP(B2)</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D2">
+        <f>C2*(2/1)^A2</f>
+        <v>1</v>
+      </c>
+      <c r="E2">
+        <f>D2/SUM(D:D)</f>
+        <v>2.0222545530781852E-48</v>
+      </c>
+      <c r="G2">
+        <f>C2*(3/1)^A2</f>
+        <v>1</v>
+      </c>
+      <c r="H2">
+        <f>G2/SUM(G:G)</f>
+        <v>6.5559469072894327E-61</v>
+      </c>
+      <c r="K2">
+        <f>G2*(4/1)^E2</f>
+        <v>1</v>
+      </c>
+      <c r="L2">
+        <f>K2/SUM(K:K)</f>
+        <v>6.3124394740968741E-61</v>
+      </c>
+      <c r="N2">
+        <f>C2*(5)^A2</f>
+        <v>1</v>
+      </c>
+      <c r="O2">
+        <f>N2/SUM(N:N)</f>
+        <v>1.6175696187198019E-78</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>1</v>
       </c>
@@ -2779,8 +2865,40 @@
         <f t="shared" ref="C3:C66" si="0">EXP(B3)</f>
         <v>101.35619242579274</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D3">
+        <f t="shared" ref="D3:D66" si="1">C3*(2/1)^A3</f>
+        <v>202.71238485158548</v>
+      </c>
+      <c r="E3">
+        <f t="shared" ref="E3:E66" si="2">D3/SUM(D:D)</f>
+        <v>4.0993604323145605E-46</v>
+      </c>
+      <c r="G3">
+        <f t="shared" ref="G3:G66" si="3">C3*(3/1)^A3</f>
+        <v>304.06857727737821</v>
+      </c>
+      <c r="H3">
+        <f t="shared" ref="H3:H66" si="4">G3/SUM(G:G)</f>
+        <v>1.9934574488055257E-58</v>
+      </c>
+      <c r="K3">
+        <f t="shared" ref="K3:K66" si="5">G3*(4/1)^E3</f>
+        <v>304.06857727737821</v>
+      </c>
+      <c r="L3">
+        <f t="shared" ref="L3:L66" si="6">K3/SUM(K:K)</f>
+        <v>1.9194144900381983E-58</v>
+      </c>
+      <c r="N3">
+        <f t="shared" ref="N3:N66" si="7">C3*(5)^A3</f>
+        <v>506.78096212896372</v>
+      </c>
+      <c r="O3">
+        <f t="shared" ref="O3:O66" si="8">N3/SUM(N:N)</f>
+        <v>8.1975348768540226E-76</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A4">
         <f>A3+1</f>
         <v>2</v>
@@ -2792,10 +2910,42 @@
         <f t="shared" si="0"/>
         <v>4969.0900081565514</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D4">
+        <f t="shared" si="1"/>
+        <v>19876.360032626206</v>
+      </c>
+      <c r="E4">
+        <f t="shared" si="2"/>
+        <v>4.0195059574599613E-44</v>
+      </c>
+      <c r="G4">
+        <f t="shared" si="3"/>
+        <v>44721.81007340896</v>
+      </c>
+      <c r="H4">
+        <f t="shared" si="4"/>
+        <v>2.9319381243915086E-56</v>
+      </c>
+      <c r="K4">
+        <f t="shared" si="5"/>
+        <v>44721.81007340896</v>
+      </c>
+      <c r="L4">
+        <f t="shared" si="6"/>
+        <v>2.8230371926044995E-56</v>
+      </c>
+      <c r="N4">
+        <f t="shared" si="7"/>
+        <v>124227.25020391379</v>
+      </c>
+      <c r="O4">
+        <f t="shared" si="8"/>
+        <v>2.0094622574695426E-73</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A5">
-        <f t="shared" ref="A5:A68" si="1">A4+1</f>
+        <f t="shared" ref="A5:A68" si="9">A4+1</f>
         <v>3</v>
       </c>
       <c r="B5">
@@ -2805,10 +2955,42 @@
         <f t="shared" si="0"/>
         <v>164223.60287425737</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D5">
+        <f t="shared" si="1"/>
+        <v>1313788.822994059</v>
+      </c>
+      <c r="E5">
+        <f t="shared" si="2"/>
+        <v>2.6568154290829656E-42</v>
+      </c>
+      <c r="G5">
+        <f t="shared" si="3"/>
+        <v>4434037.2776049487</v>
+      </c>
+      <c r="H5">
+        <f t="shared" si="4"/>
+        <v>2.9069312976920218E-54</v>
+      </c>
+      <c r="K5">
+        <f t="shared" si="5"/>
+        <v>4434037.2776049487</v>
+      </c>
+      <c r="L5">
+        <f t="shared" si="6"/>
+        <v>2.7989591940770517E-54</v>
+      </c>
+      <c r="N5">
+        <f t="shared" si="7"/>
+        <v>20527950.359282169</v>
+      </c>
+      <c r="O5">
+        <f t="shared" si="8"/>
+        <v>3.3205388835763079E-71</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="9"/>
         <v>4</v>
       </c>
       <c r="B6">
@@ -2818,10 +3000,42 @@
         <f t="shared" si="0"/>
         <v>3954835.5229426823</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D6">
+        <f t="shared" si="1"/>
+        <v>63277368.367082916</v>
+      </c>
+      <c r="E6">
+        <f t="shared" si="2"/>
+        <v>1.2796294628713895E-40</v>
+      </c>
+      <c r="G6">
+        <f t="shared" si="3"/>
+        <v>320341677.35835725</v>
+      </c>
+      <c r="H6">
+        <f t="shared" si="4"/>
+        <v>2.1001430289534317E-52</v>
+      </c>
+      <c r="K6">
+        <f t="shared" si="5"/>
+        <v>320341677.35835725</v>
+      </c>
+      <c r="L6">
+        <f t="shared" si="6"/>
+        <v>2.0221374493552994E-52</v>
+      </c>
+      <c r="N6">
+        <f t="shared" si="7"/>
+        <v>2471772201.8391762</v>
+      </c>
+      <c r="O6">
+        <f t="shared" si="8"/>
+        <v>3.9982636180912015E-69</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="9"/>
         <v>5</v>
       </c>
       <c r="B7">
@@ -2831,10 +3045,42 @@
         <f t="shared" si="0"/>
         <v>76495014.347945377</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D7">
+        <f t="shared" si="1"/>
+        <v>2447840459.1342521</v>
+      </c>
+      <c r="E7">
+        <f t="shared" si="2"/>
+        <v>4.950156513693237E-39</v>
+      </c>
+      <c r="G7">
+        <f t="shared" si="3"/>
+        <v>18588288486.550728</v>
+      </c>
+      <c r="H7">
+        <f t="shared" si="4"/>
+        <v>1.2186383241520602E-50</v>
+      </c>
+      <c r="K7">
+        <f t="shared" si="5"/>
+        <v>18588288486.550728</v>
+      </c>
+      <c r="L7">
+        <f t="shared" si="6"/>
+        <v>1.1733744599840326E-50</v>
+      </c>
+      <c r="N7">
+        <f t="shared" si="7"/>
+        <v>239046919837.32932</v>
+      </c>
+      <c r="O7">
+        <f t="shared" si="8"/>
+        <v>3.8667503497741182E-67</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="9"/>
         <v>6</v>
       </c>
       <c r="B8">
@@ -2844,10 +3090,42 @@
         <f t="shared" si="0"/>
         <v>1227793890.1402495</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D8">
+        <f t="shared" si="1"/>
+        <v>78578808968.975967</v>
+      </c>
+      <c r="E8">
+        <f t="shared" si="2"/>
+        <v>1.5890635421297258E-37</v>
+      </c>
+      <c r="G8">
+        <f t="shared" si="3"/>
+        <v>895061745912.24182</v>
+      </c>
+      <c r="H8">
+        <f t="shared" si="4"/>
+        <v>5.867977284946442E-49</v>
+      </c>
+      <c r="K8">
+        <f t="shared" si="5"/>
+        <v>895061745912.24182</v>
+      </c>
+      <c r="L8">
+        <f t="shared" si="6"/>
+        <v>5.6500230966505018E-49</v>
+      </c>
+      <c r="N8">
+        <f t="shared" si="7"/>
+        <v>19184279533441.398</v>
+      </c>
+      <c r="O8">
+        <f t="shared" si="8"/>
+        <v>3.1031907730322903E-65</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="9"/>
         <v>7</v>
       </c>
       <c r="B9">
@@ -2857,10 +3135,42 @@
         <f t="shared" si="0"/>
         <v>17024301338.313831</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D9">
+        <f t="shared" si="1"/>
+        <v>2179110571304.1704</v>
+      </c>
+      <c r="E9">
+        <f t="shared" si="2"/>
+        <v>4.4067162744806643E-36</v>
+      </c>
+      <c r="G9">
+        <f t="shared" si="3"/>
+        <v>37232147026892.352</v>
+      </c>
+      <c r="H9">
+        <f t="shared" si="4"/>
+        <v>2.4409197915270037E-47</v>
+      </c>
+      <c r="K9">
+        <f t="shared" si="5"/>
+        <v>37232147026892.352</v>
+      </c>
+      <c r="L9">
+        <f t="shared" si="6"/>
+        <v>2.3502567459793385E-47</v>
+      </c>
+      <c r="N9">
+        <f t="shared" si="7"/>
+        <v>1330023542055768</v>
+      </c>
+      <c r="O9">
+        <f t="shared" si="8"/>
+        <v>2.151405673811509E-63</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="9"/>
         <v>8</v>
       </c>
       <c r="B10">
@@ -2870,10 +3180,42 @@
         <f t="shared" si="0"/>
         <v>194356898367.92535</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D10">
+        <f t="shared" si="1"/>
+        <v>49755365982188.891</v>
+      </c>
+      <c r="E10">
+        <f t="shared" si="2"/>
+        <v>1.0061801539755294E-34</v>
+      </c>
+      <c r="G10">
+        <f t="shared" si="3"/>
+        <v>1275175610191958.2</v>
+      </c>
+      <c r="H10">
+        <f t="shared" si="4"/>
+        <v>8.3599835978888839E-46</v>
+      </c>
+      <c r="K10">
+        <f t="shared" si="5"/>
+        <v>1275175610191958.2</v>
+      </c>
+      <c r="L10">
+        <f t="shared" si="6"/>
+        <v>8.0494688581812855E-46</v>
+      </c>
+      <c r="N10">
+        <f t="shared" si="7"/>
+        <v>7.5920663424970848E+16</v>
+      </c>
+      <c r="O10">
+        <f t="shared" si="8"/>
+        <v>1.228069585892845E-61</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A11">
-        <f t="shared" si="1"/>
+        <f t="shared" si="9"/>
         <v>9</v>
       </c>
       <c r="B11">
@@ -2883,10 +3225,42 @@
         <f t="shared" si="0"/>
         <v>1973396676312.9722</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D11">
+        <f t="shared" si="1"/>
+        <v>1010379098272241.8</v>
+      </c>
+      <c r="E11">
+        <f t="shared" si="2"/>
+        <v>2.043243731816072E-33</v>
+      </c>
+      <c r="G11">
+        <f t="shared" si="3"/>
+        <v>3.8842366779868232E+16</v>
+      </c>
+      <c r="H11">
+        <f t="shared" si="4"/>
+        <v>2.5464849436227895E-44</v>
+      </c>
+      <c r="K11">
+        <f t="shared" si="5"/>
+        <v>3.8842366779868232E+16</v>
+      </c>
+      <c r="L11">
+        <f t="shared" si="6"/>
+        <v>2.4519008932858934E-44</v>
+      </c>
+      <c r="N11">
+        <f t="shared" si="7"/>
+        <v>3.8542903834237737E+18</v>
+      </c>
+      <c r="O11">
+        <f t="shared" si="8"/>
+        <v>6.2345830259501932E-60</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A12">
-        <f t="shared" si="1"/>
+        <f t="shared" si="9"/>
         <v>10</v>
       </c>
       <c r="B12">
@@ -2896,10 +3270,42 @@
         <f t="shared" si="0"/>
         <v>18041168681156.16</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D12">
+        <f t="shared" si="1"/>
+        <v>1.8474156729503908E+16</v>
+      </c>
+      <c r="E12">
+        <f t="shared" si="2"/>
+        <v>3.7359447560519276E-32</v>
+      </c>
+      <c r="G12">
+        <f t="shared" si="3"/>
+        <v>1.0653129694535901E+18</v>
+      </c>
+      <c r="H12">
+        <f t="shared" si="4"/>
+        <v>6.9841352673845861E-43</v>
+      </c>
+      <c r="K12">
+        <f t="shared" si="5"/>
+        <v>1.0653129694535901E+18</v>
+      </c>
+      <c r="L12">
+        <f t="shared" si="6"/>
+        <v>6.7247236406462E-43</v>
+      </c>
+      <c r="N12">
+        <f t="shared" si="7"/>
+        <v>1.7618328790191561E+20</v>
+      </c>
+      <c r="O12">
+        <f t="shared" si="8"/>
+        <v>2.8498873383630272E-58</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A13">
-        <f t="shared" si="1"/>
+        <f t="shared" si="9"/>
         <v>11</v>
       </c>
       <c r="B13">
@@ -2909,10 +3315,42 @@
         <f t="shared" si="0"/>
         <v>149056446439066.12</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D13">
+        <f t="shared" si="1"/>
+        <v>3.0526760230720742E+17</v>
+      </c>
+      <c r="E13">
+        <f t="shared" si="2"/>
+        <v>6.1732879867301093E-31</v>
+      </c>
+      <c r="G13">
+        <f t="shared" si="3"/>
+        <v>2.6404902317341245E+19</v>
+      </c>
+      <c r="H13">
+        <f t="shared" si="4"/>
+        <v>1.7310913768465292E-41</v>
+      </c>
+      <c r="K13">
+        <f t="shared" si="5"/>
+        <v>2.6404902317341245E+19</v>
+      </c>
+      <c r="L13">
+        <f t="shared" si="6"/>
+        <v>1.666793476976569E-41</v>
+      </c>
+      <c r="N13">
+        <f t="shared" si="7"/>
+        <v>7.2781467987825257E+21</v>
+      </c>
+      <c r="O13">
+        <f t="shared" si="8"/>
+        <v>1.1772909142293398E-56</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A14">
-        <f t="shared" si="1"/>
+        <f t="shared" si="9"/>
         <v>12</v>
       </c>
       <c r="B14">
@@ -2922,10 +3360,42 @@
         <f t="shared" si="0"/>
         <v>1069545806405926.4</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D14">
+        <f t="shared" si="1"/>
+        <v>4.3808596230386744E+18</v>
+      </c>
+      <c r="E14">
+        <f t="shared" si="2"/>
+        <v>8.8592133190863418E-30</v>
+      </c>
+      <c r="G14">
+        <f t="shared" si="3"/>
+        <v>5.6840049290217193E+20</v>
+      </c>
+      <c r="H14">
+        <f t="shared" si="4"/>
+        <v>3.7264034535437832E-40</v>
+      </c>
+      <c r="K14">
+        <f t="shared" si="5"/>
+        <v>5.6840049290217193E+20</v>
+      </c>
+      <c r="L14">
+        <f t="shared" si="6"/>
+        <v>3.5879937084917903E-40</v>
+      </c>
+      <c r="N14">
+        <f t="shared" si="7"/>
+        <v>2.6111958164207186E+23</v>
+      </c>
+      <c r="O14">
+        <f t="shared" si="8"/>
+        <v>4.2237910211704039E-55</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A15">
-        <f t="shared" si="1"/>
+        <f t="shared" si="9"/>
         <v>13</v>
       </c>
       <c r="B15">
@@ -2935,10 +3405,42 @@
         <f t="shared" si="0"/>
         <v>7207556788563748</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D15">
+        <f t="shared" si="1"/>
+        <v>5.9044305211914224E+19</v>
+      </c>
+      <c r="E15">
+        <f t="shared" si="2"/>
+        <v>1.1940261504813157E-28</v>
+      </c>
+      <c r="G15">
+        <f t="shared" si="3"/>
+        <v>1.1491173561813321E+22</v>
+      </c>
+      <c r="H15">
+        <f t="shared" si="4"/>
+        <v>7.5335523773696144E-39</v>
+      </c>
+      <c r="K15">
+        <f t="shared" si="5"/>
+        <v>1.1491173561813321E+22</v>
+      </c>
+      <c r="L15">
+        <f t="shared" si="6"/>
+        <v>7.2537337595288785E-39</v>
+      </c>
+      <c r="N15">
+        <f t="shared" si="7"/>
+        <v>8.7982870954147315E+24</v>
+      </c>
+      <c r="O15">
+        <f t="shared" si="8"/>
+        <v>1.4231841902317361E-53</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A16">
-        <f t="shared" si="1"/>
+        <f t="shared" si="9"/>
         <v>14</v>
       </c>
       <c r="B16">
@@ -2948,10 +3450,42 @@
         <f t="shared" si="0"/>
         <v>4.4078204842997968E+16</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D16">
+        <f t="shared" si="1"/>
+        <v>7.2217730814767871E+20</v>
+      </c>
+      <c r="E16">
+        <f t="shared" si="2"/>
+        <v>1.4604263495313909E-27</v>
+      </c>
+      <c r="G16">
+        <f t="shared" si="3"/>
+        <v>2.1082468733970913E+23</v>
+      </c>
+      <c r="H16">
+        <f t="shared" si="4"/>
+        <v>1.3821554569450278E-37</v>
+      </c>
+      <c r="K16">
+        <f t="shared" si="5"/>
+        <v>2.1082468733970913E+23</v>
+      </c>
+      <c r="L16">
+        <f t="shared" si="6"/>
+        <v>1.3308180784773115E-37</v>
+      </c>
+      <c r="N16">
+        <f t="shared" si="7"/>
+        <v>2.6903201198118876E+26</v>
+      </c>
+      <c r="O16">
+        <f t="shared" si="8"/>
+        <v>4.3517800904383269E-52</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A17">
-        <f t="shared" si="1"/>
+        <f t="shared" si="9"/>
         <v>15</v>
       </c>
       <c r="B17">
@@ -2961,10 +3495,42 @@
         <f t="shared" si="0"/>
         <v>2.5165535038743846E+17</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D17">
+        <f t="shared" si="1"/>
+        <v>8.2462425214955836E+21</v>
+      </c>
+      <c r="E17">
+        <f t="shared" si="2"/>
+        <v>1.6676001484881377E-26</v>
+      </c>
+      <c r="G17">
+        <f t="shared" si="3"/>
+        <v>3.6109792187617685E+24</v>
+      </c>
+      <c r="H17">
+        <f t="shared" si="4"/>
+        <v>2.3673388041527629E-36</v>
+      </c>
+      <c r="K17">
+        <f t="shared" si="5"/>
+        <v>3.6109792187617685E+24</v>
+      </c>
+      <c r="L17">
+        <f t="shared" si="6"/>
+        <v>2.2794087760655281E-36</v>
+      </c>
+      <c r="N17">
+        <f t="shared" si="7"/>
+        <v>7.679911816022902E+27</v>
+      </c>
+      <c r="O17">
+        <f t="shared" si="8"/>
+        <v>1.2422792028045868E-50</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A18">
-        <f t="shared" si="1"/>
+        <f t="shared" si="9"/>
         <v>16</v>
       </c>
       <c r="B18">
@@ -2974,10 +3540,42 @@
         <f t="shared" si="0"/>
         <v>1.3188662640311519E+18</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D18">
+        <f t="shared" si="1"/>
+        <v>8.6433219479545569E+22</v>
+      </c>
+      <c r="E18">
+        <f t="shared" si="2"/>
+        <v>1.7478997162971713E-25</v>
+      </c>
+      <c r="G18">
+        <f t="shared" si="3"/>
+        <v>5.6772868104061328E+25</v>
+      </c>
+      <c r="H18">
+        <f t="shared" si="4"/>
+        <v>3.7219990906477171E-35</v>
+      </c>
+      <c r="K18">
+        <f t="shared" si="5"/>
+        <v>5.6772868104061328E+25</v>
+      </c>
+      <c r="L18">
+        <f t="shared" si="6"/>
+        <v>3.583752936777721E-35</v>
+      </c>
+      <c r="N18">
+        <f t="shared" si="7"/>
+        <v>2.0124302124498777E+29</v>
+      </c>
+      <c r="O18">
+        <f t="shared" si="8"/>
+        <v>3.2552459714527588E-49</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A19">
-        <f t="shared" si="1"/>
+        <f t="shared" si="9"/>
         <v>17</v>
       </c>
       <c r="B19">
@@ -2987,10 +3585,42 @@
         <f t="shared" si="0"/>
         <v>6.5037472671463025E+18</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D19">
+        <f t="shared" si="1"/>
+        <v>8.5245916179940016E+23</v>
+      </c>
+      <c r="E19">
+        <f t="shared" si="2"/>
+        <v>1.7238894212620503E-24</v>
+      </c>
+      <c r="G19">
+        <f t="shared" si="3"/>
+        <v>8.3989498219007801E+26</v>
+      </c>
+      <c r="H19">
+        <f t="shared" si="4"/>
+        <v>5.5063069109369552E-34</v>
+      </c>
+      <c r="K19">
+        <f t="shared" si="5"/>
+        <v>8.3989498219007801E+26</v>
+      </c>
+      <c r="L19">
+        <f t="shared" si="6"/>
+        <v>5.3017862396725396E-34</v>
+      </c>
+      <c r="N19">
+        <f t="shared" si="7"/>
+        <v>4.9619653832598131E+30</v>
+      </c>
+      <c r="O19">
+        <f t="shared" si="8"/>
+        <v>8.0263244531004311E-48</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A20">
-        <f t="shared" si="1"/>
+        <f t="shared" si="9"/>
         <v>18</v>
       </c>
       <c r="B20">
@@ -3000,10 +3630,42 @@
         <f t="shared" si="0"/>
         <v>2.9881580520778539E+19</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D20">
+        <f t="shared" si="1"/>
+        <v>7.8332770440389693E+24</v>
+      </c>
+      <c r="E20">
+        <f t="shared" si="2"/>
+        <v>1.5840880167830634E-23</v>
+      </c>
+      <c r="G20">
+        <f t="shared" si="3"/>
+        <v>1.1576736537452897E+28</v>
+      </c>
+      <c r="H20">
+        <f t="shared" si="4"/>
+        <v>7.5896470099218888E-33</v>
+      </c>
+      <c r="K20">
+        <f t="shared" si="5"/>
+        <v>1.1576736537452897E+28</v>
+      </c>
+      <c r="L20">
+        <f t="shared" si="6"/>
+        <v>7.3077448700237233E-33</v>
+      </c>
+      <c r="N20">
+        <f t="shared" si="7"/>
+        <v>1.1398918350516715E+32</v>
+      </c>
+      <c r="O20">
+        <f t="shared" si="8"/>
+        <v>1.8438544010063478E-46</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A21">
-        <f t="shared" si="1"/>
+        <f t="shared" si="9"/>
         <v>19</v>
       </c>
       <c r="B21">
@@ -3013,10 +3675,42 @@
         <f t="shared" si="0"/>
         <v>1.2853531049543156E+20</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D21">
+        <f t="shared" si="1"/>
+        <v>6.738952086902882E+25</v>
+      </c>
+      <c r="E21">
+        <f t="shared" si="2"/>
+        <v>1.3627876540715092E-22</v>
+      </c>
+      <c r="G21">
+        <f t="shared" si="3"/>
+        <v>1.4939163853772078E+29</v>
+      </c>
+      <c r="H21">
+        <f t="shared" si="4"/>
+        <v>9.794036506462714E-32</v>
+      </c>
+      <c r="K21">
+        <f t="shared" si="5"/>
+        <v>1.4939163853772078E+29</v>
+      </c>
+      <c r="L21">
+        <f t="shared" si="6"/>
+        <v>9.4302567620552048E-32</v>
+      </c>
+      <c r="N21">
+        <f t="shared" si="7"/>
+        <v>2.4516164874159157E+33</v>
+      </c>
+      <c r="O21">
+        <f t="shared" si="8"/>
+        <v>3.965660346796543E-45</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A22">
-        <f t="shared" si="1"/>
+        <f t="shared" si="9"/>
         <v>20</v>
       </c>
       <c r="B22">
@@ -3026,10 +3720,42 @@
         <f t="shared" si="0"/>
         <v>5.21992961186553E+20</v>
       </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D22">
+        <f t="shared" si="1"/>
+        <v>5.47349291269151E+26</v>
+      </c>
+      <c r="E22">
+        <f t="shared" si="2"/>
+        <v>1.1068795963931584E-21</v>
+      </c>
+      <c r="G22">
+        <f t="shared" si="3"/>
+        <v>1.8200769144970716E+30</v>
+      </c>
+      <c r="H22">
+        <f t="shared" si="4"/>
+        <v>1.1932327618625969E-30</v>
+      </c>
+      <c r="K22">
+        <f t="shared" si="5"/>
+        <v>1.8200769144970716E+30</v>
+      </c>
+      <c r="L22">
+        <f t="shared" si="6"/>
+        <v>1.1489125360963757E-30</v>
+      </c>
+      <c r="N22">
+        <f t="shared" si="7"/>
+        <v>4.9781128042846009E+34</v>
+      </c>
+      <c r="O22">
+        <f t="shared" si="8"/>
+        <v>8.0524440307708058E-44</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A23">
-        <f t="shared" si="1"/>
+        <f t="shared" si="9"/>
         <v>21</v>
       </c>
       <c r="B23">
@@ -3039,10 +3765,42 @@
         <f t="shared" si="0"/>
         <v>1.9434271542706831E+21</v>
       </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D23">
+        <f t="shared" si="1"/>
+        <v>4.0756621434330717E+27</v>
+      </c>
+      <c r="E23">
+        <f t="shared" si="2"/>
+        <v>8.2420263263659254E-21</v>
+      </c>
+      <c r="G23">
+        <f t="shared" si="3"/>
+        <v>2.0328934457972517E+31</v>
+      </c>
+      <c r="H23">
+        <f t="shared" si="4"/>
+        <v>1.332754149882345E-29</v>
+      </c>
+      <c r="K23">
+        <f t="shared" si="5"/>
+        <v>2.0328934457972517E+31</v>
+      </c>
+      <c r="L23">
+        <f t="shared" si="6"/>
+        <v>1.2832516833883386E-29</v>
+      </c>
+      <c r="N23">
+        <f t="shared" si="7"/>
+        <v>9.2669828141721881E+35</v>
+      </c>
+      <c r="O23">
+        <f t="shared" si="8"/>
+        <v>1.4989989857403463E-42</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A24">
-        <f t="shared" si="1"/>
+        <f t="shared" si="9"/>
         <v>22</v>
       </c>
       <c r="B24">
@@ -3052,10 +3810,42 @@
         <f t="shared" si="0"/>
         <v>6.9243681679312631E+21</v>
       </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D24">
+        <f t="shared" si="1"/>
+        <v>2.9042905104226768E+28</v>
+      </c>
+      <c r="E24">
+        <f t="shared" si="2"/>
+        <v>5.8732147081640252E-20</v>
+      </c>
+      <c r="G24">
+        <f t="shared" si="3"/>
+        <v>2.1729401023251309E+32</v>
+      </c>
+      <c r="H24">
+        <f t="shared" si="4"/>
+        <v>1.4245679943563625E-28</v>
+      </c>
+      <c r="K24">
+        <f t="shared" si="5"/>
+        <v>2.1729401023251309E+32</v>
+      </c>
+      <c r="L24">
+        <f t="shared" si="6"/>
+        <v>1.3716552876765259E-28</v>
+      </c>
+      <c r="N24">
+        <f t="shared" si="7"/>
+        <v>1.6508980197742614E+37</v>
+      </c>
+      <c r="O24">
+        <f t="shared" si="8"/>
+        <v>2.6704424803915278E-41</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A25">
-        <f t="shared" si="1"/>
+        <f t="shared" si="9"/>
         <v>23</v>
       </c>
       <c r="B25">
@@ -3065,10 +3855,42 @@
         <f t="shared" si="0"/>
         <v>2.3332149595306705E+22</v>
       </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D25">
+        <f t="shared" si="1"/>
+        <v>1.9572425675238658E+29</v>
+      </c>
+      <c r="E25">
+        <f t="shared" si="2"/>
+        <v>3.9580426936535751E-19</v>
+      </c>
+      <c r="G25">
+        <f t="shared" si="3"/>
+        <v>2.1965627317692749E+33</v>
+      </c>
+      <c r="H25">
+        <f t="shared" si="4"/>
+        <v>1.4400548648010006E-27</v>
+      </c>
+      <c r="K25">
+        <f t="shared" si="5"/>
+        <v>2.1965627317692749E+33</v>
+      </c>
+      <c r="L25">
+        <f t="shared" si="6"/>
+        <v>1.3865669295350436E-27</v>
+      </c>
+      <c r="N25">
+        <f t="shared" si="7"/>
+        <v>2.7814089769490603E+38</v>
+      </c>
+      <c r="O25">
+        <f t="shared" si="8"/>
+        <v>4.4991226583473261E-40</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A26">
-        <f t="shared" si="1"/>
+        <f t="shared" si="9"/>
         <v>24</v>
       </c>
       <c r="B26">
@@ -3078,10 +3900,42 @@
         <f t="shared" si="0"/>
         <v>7.4798885599626941E+22</v>
       </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D26">
+        <f t="shared" si="1"/>
+        <v>1.2549170602642307E+30</v>
+      </c>
+      <c r="E26">
+        <f t="shared" si="2"/>
+        <v>2.537761738854832E-18</v>
+      </c>
+      <c r="G26">
+        <f t="shared" si="3"/>
+        <v>2.1125414589197985E+34</v>
+      </c>
+      <c r="H26">
+        <f t="shared" si="4"/>
+        <v>1.3849709644125959E-26</v>
+      </c>
+      <c r="K26">
+        <f t="shared" si="5"/>
+        <v>2.1125414589197985E+34</v>
+      </c>
+      <c r="L26">
+        <f t="shared" si="6"/>
+        <v>1.3335290095951536E-26</v>
+      </c>
+      <c r="N26">
+        <f t="shared" si="7"/>
+        <v>4.4583610057608452E+39</v>
+      </c>
+      <c r="O26">
+        <f t="shared" si="8"/>
+        <v>7.2117093122038027E-39</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A27">
-        <f t="shared" si="1"/>
+        <f t="shared" si="9"/>
         <v>25</v>
       </c>
       <c r="B27">
@@ -3091,10 +3945,42 @@
         <f t="shared" si="0"/>
         <v>2.2841722197399101E+23</v>
       </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D27">
+        <f t="shared" si="1"/>
+        <v>7.6644101423551872E+30</v>
+      </c>
+      <c r="E27">
+        <f t="shared" si="2"/>
+        <v>1.5499388307036398E-17</v>
+      </c>
+      <c r="G27">
+        <f t="shared" si="3"/>
+        <v>1.9353531037917591E+35</v>
+      </c>
+      <c r="H27">
+        <f t="shared" si="4"/>
+        <v>1.2688072195316588E-25</v>
+      </c>
+      <c r="K27">
+        <f t="shared" si="5"/>
+        <v>1.9353531037917591E+35</v>
+      </c>
+      <c r="L27">
+        <f t="shared" si="6"/>
+        <v>1.2216799328691007E-25</v>
+      </c>
+      <c r="N27">
+        <f t="shared" si="7"/>
+        <v>6.8073636881706423E+40</v>
+      </c>
+      <c r="O27">
+        <f t="shared" si="8"/>
+        <v>1.1011384685561209E-37</v>
+      </c>
+    </row>
+    <row r="28" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A28">
-        <f t="shared" si="1"/>
+        <f t="shared" si="9"/>
         <v>26</v>
       </c>
       <c r="B28">
@@ -3104,10 +3990,42 @@
         <f t="shared" si="0"/>
         <v>6.6535665727017133E+23</v>
       </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D28">
+        <f t="shared" si="1"/>
+        <v>4.4651329424238539E+31</v>
+      </c>
+      <c r="E28">
+        <f t="shared" si="2"/>
+        <v>9.0296354229160325E-17</v>
+      </c>
+      <c r="G28">
+        <f t="shared" si="3"/>
+        <v>1.6912473507662586E+36</v>
+      </c>
+      <c r="H28">
+        <f t="shared" si="4"/>
+        <v>1.1087727838717499E-24</v>
+      </c>
+      <c r="K28">
+        <f t="shared" si="5"/>
+        <v>1.6912473507662589E+36</v>
+      </c>
+      <c r="L28">
+        <f t="shared" si="6"/>
+        <v>1.0675896537438695E-24</v>
+      </c>
+      <c r="N28">
+        <f t="shared" si="7"/>
+        <v>9.914586801382472E+41</v>
+      </c>
+      <c r="O28">
+        <f t="shared" si="8"/>
+        <v>1.6037534392076625E-36</v>
+      </c>
+    </row>
+    <row r="29" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A29">
-        <f t="shared" si="1"/>
+        <f t="shared" si="9"/>
         <v>27</v>
       </c>
       <c r="B29">
@@ -3117,10 +4035,42 @@
         <f t="shared" si="0"/>
         <v>1.8440529765346631E+24</v>
       </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D29">
+        <f t="shared" si="1"/>
+        <v>2.4750460082211979E+32</v>
+      </c>
+      <c r="E29">
+        <f t="shared" si="2"/>
+        <v>5.0051730592033048E-16</v>
+      </c>
+      <c r="G29">
+        <f t="shared" si="3"/>
+        <v>1.4062005740045518E+37</v>
+      </c>
+      <c r="H29">
+        <f t="shared" si="4"/>
+        <v>9.2189763041737671E-24</v>
+      </c>
+      <c r="K29">
+        <f t="shared" si="5"/>
+        <v>1.4062005740045528E+37</v>
+      </c>
+      <c r="L29">
+        <f t="shared" si="6"/>
+        <v>8.8765560118440215E-24</v>
+      </c>
+      <c r="N29">
+        <f t="shared" si="7"/>
+        <v>1.3739265326668792E+43</v>
+      </c>
+      <c r="O29">
+        <f t="shared" si="8"/>
+        <v>2.2224218175949831E-35</v>
+      </c>
+    </row>
+    <row r="30" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A30">
-        <f t="shared" si="1"/>
+        <f t="shared" si="9"/>
         <v>28</v>
       </c>
       <c r="B30">
@@ -3130,10 +4080,42 @@
         <f t="shared" si="0"/>
         <v>4.8962878897037741E+24</v>
       </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D30">
+        <f t="shared" si="1"/>
+        <v>1.3143372723799103E+33</v>
+      </c>
+      <c r="E30">
+        <f t="shared" si="2"/>
+        <v>2.6579245333506366E-15</v>
+      </c>
+      <c r="G30">
+        <f t="shared" si="3"/>
+        <v>1.1201136185249221E+38</v>
+      </c>
+      <c r="H30">
+        <f t="shared" si="4"/>
+        <v>7.3434054131812387E-23</v>
+      </c>
+      <c r="K30">
+        <f t="shared" si="5"/>
+        <v>1.1201136185249263E+38</v>
+      </c>
+      <c r="L30">
+        <f t="shared" si="6"/>
+        <v>7.0706494210502327E-23</v>
+      </c>
+      <c r="N30">
+        <f t="shared" si="7"/>
+        <v>1.8240093773990029E+44</v>
+      </c>
+      <c r="O30">
+        <f t="shared" si="8"/>
+        <v>2.9504621531406483E-34</v>
+      </c>
+    </row>
+    <row r="31" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A31">
-        <f t="shared" si="1"/>
+        <f t="shared" si="9"/>
         <v>29</v>
       </c>
       <c r="B31">
@@ -3143,10 +4125,42 @@
         <f t="shared" si="0"/>
         <v>1.2159535627996638E+25</v>
       </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D31">
+        <f t="shared" si="1"/>
+        <v>6.5281009820990476E+33</v>
+      </c>
+      <c r="E31">
+        <f t="shared" si="2"/>
+        <v>1.3201481934003972E-14</v>
+      </c>
+      <c r="G31">
+        <f t="shared" si="3"/>
+        <v>8.3451351873114886E+38</v>
+      </c>
+      <c r="H31">
+        <f t="shared" si="4"/>
+        <v>5.4710263222166974E-22</v>
+      </c>
+      <c r="K31">
+        <f t="shared" si="5"/>
+        <v>8.3451351873116412E+38</v>
+      </c>
+      <c r="L31">
+        <f t="shared" si="6"/>
+        <v>5.2678160773060814E-22</v>
+      </c>
+      <c r="N31">
+        <f t="shared" si="7"/>
+        <v>2.2648900054388933E+45</v>
+      </c>
+      <c r="O31">
+        <f t="shared" si="8"/>
+        <v>3.6636172625400805E-33</v>
+      </c>
+    </row>
+    <row r="32" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A32">
-        <f t="shared" si="1"/>
+        <f t="shared" si="9"/>
         <v>30</v>
       </c>
       <c r="B32">
@@ -3156,10 +4170,42 @@
         <f t="shared" si="0"/>
         <v>2.8636877237565846E+25</v>
       </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D32">
+        <f t="shared" si="1"/>
+        <v>3.0748612798728033E+34</v>
+      </c>
+      <c r="E32">
+        <f t="shared" si="2"/>
+        <v>6.2181522233065922E-14</v>
+      </c>
+      <c r="G32">
+        <f t="shared" si="3"/>
+        <v>5.8960790740979167E+39</v>
+      </c>
+      <c r="H32">
+        <f t="shared" si="4"/>
+        <v>3.8654381370966177E-21</v>
+      </c>
+      <c r="K32">
+        <f t="shared" si="5"/>
+        <v>5.8960790740984245E+39</v>
+      </c>
+      <c r="L32">
+        <f t="shared" si="6"/>
+        <v>3.7218642289735447E-21</v>
+      </c>
+      <c r="N32">
+        <f t="shared" si="7"/>
+        <v>2.6670170237837219E+46</v>
+      </c>
+      <c r="O32">
+        <f t="shared" si="8"/>
+        <v>4.3140857102810558E-32</v>
+      </c>
+    </row>
+    <row r="33" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A33">
-        <f t="shared" si="1"/>
+        <f t="shared" si="9"/>
         <v>31</v>
       </c>
       <c r="B33">
@@ -3169,10 +4215,42 @@
         <f t="shared" si="0"/>
         <v>6.4947688898268716E+25</v>
       </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D33">
+        <f t="shared" si="1"/>
+        <v>1.394740998844232E+35</v>
+      </c>
+      <c r="E33">
+        <f t="shared" si="2"/>
+        <v>2.8205213352775644E-13</v>
+      </c>
+      <c r="G33">
+        <f t="shared" si="3"/>
+        <v>4.0116459582586836E+40</v>
+      </c>
+      <c r="H33">
+        <f t="shared" si="4"/>
+        <v>2.630013791318617E-20</v>
+      </c>
+      <c r="K33">
+        <f t="shared" si="5"/>
+        <v>4.0116459582602523E+40</v>
+      </c>
+      <c r="L33">
+        <f t="shared" si="6"/>
+        <v>2.5323272303023198E-20</v>
+      </c>
+      <c r="N33">
+        <f t="shared" si="7"/>
+        <v>3.0243624420030374E+47</v>
+      </c>
+      <c r="O33">
+        <f t="shared" si="8"/>
+        <v>4.8921168021813426E-31</v>
+      </c>
+    </row>
+    <row r="34" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A34">
-        <f t="shared" si="1"/>
+        <f t="shared" si="9"/>
         <v>32</v>
       </c>
       <c r="B34">
@@ -3182,10 +4260,42 @@
         <f t="shared" si="0"/>
         <v>1.400615843318863E+26</v>
       </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D34">
+        <f t="shared" si="1"/>
+        <v>6.0155992413139765E+35</v>
+      </c>
+      <c r="E34">
+        <f t="shared" si="2"/>
+        <v>1.2165072955240866E-12</v>
+      </c>
+      <c r="G34">
+        <f t="shared" si="3"/>
+        <v>2.5953694344956001E+41</v>
+      </c>
+      <c r="H34">
+        <f t="shared" si="4"/>
+        <v>1.7015104217354954E-19</v>
+      </c>
+      <c r="K34">
+        <f t="shared" si="5"/>
+        <v>2.595369434499977E+41</v>
+      </c>
+      <c r="L34">
+        <f t="shared" si="6"/>
+        <v>1.6383112468202138E-19</v>
+      </c>
+      <c r="N34">
+        <f t="shared" si="7"/>
+        <v>3.2610628831173828E+48</v>
+      </c>
+      <c r="O34">
+        <f t="shared" si="8"/>
+        <v>5.2749962444654829E-30</v>
+      </c>
+    </row>
+    <row r="35" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A35">
-        <f t="shared" si="1"/>
+        <f t="shared" si="9"/>
         <v>33</v>
       </c>
       <c r="B35">
@@ -3195,10 +4305,42 @@
         <f t="shared" si="0"/>
         <v>2.8088084989176123E+26</v>
       </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D35">
+        <f t="shared" si="1"/>
+        <v>2.4127481287155992E+36</v>
+      </c>
+      <c r="E35">
+        <f t="shared" si="2"/>
+        <v>4.879190888725992E-12</v>
+      </c>
+      <c r="G35">
+        <f t="shared" si="3"/>
+        <v>1.5614336565338909E+42</v>
+      </c>
+      <c r="H35">
+        <f t="shared" si="4"/>
+        <v>1.0236676151490993E-18</v>
+      </c>
+      <c r="K35">
+        <f t="shared" si="5"/>
+        <v>1.5614336565444524E+42</v>
+      </c>
+      <c r="L35">
+        <f t="shared" si="6"/>
+        <v>9.8564554497546229E-19</v>
+      </c>
+      <c r="N35">
+        <f t="shared" si="7"/>
+        <v>3.2698834535172355E+49</v>
+      </c>
+      <c r="O35">
+        <f t="shared" si="8"/>
+        <v>5.2892641311640641E-29</v>
+      </c>
+    </row>
+    <row r="36" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A36">
-        <f t="shared" si="1"/>
+        <f t="shared" si="9"/>
         <v>34</v>
       </c>
       <c r="B36">
@@ -3208,10 +4350,42 @@
         <f t="shared" si="0"/>
         <v>5.5919113093353678E+26</v>
       </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D36">
+        <f t="shared" si="1"/>
+        <v>9.6068304782911777E+36</v>
+      </c>
+      <c r="E36">
+        <f t="shared" si="2"/>
+        <v>1.9427456675374613E-11</v>
+      </c>
+      <c r="G36">
+        <f t="shared" si="3"/>
+        <v>9.3257320954206309E+42</v>
+      </c>
+      <c r="H36">
+        <f t="shared" si="4"/>
+        <v>6.1139004489182689E-18</v>
+      </c>
+      <c r="K36">
+        <f t="shared" si="5"/>
+        <v>9.325732095671794E+42</v>
+      </c>
+      <c r="L36">
+        <f t="shared" si="6"/>
+        <v>5.8868119405570802E-18</v>
+      </c>
+      <c r="N36">
+        <f t="shared" si="7"/>
+        <v>3.2549207735197664E+50</v>
+      </c>
+      <c r="O36">
+        <f t="shared" si="8"/>
+        <v>5.265060954585531E-28</v>
+      </c>
+    </row>
+    <row r="37" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A37">
-        <f t="shared" si="1"/>
+        <f t="shared" si="9"/>
         <v>35</v>
       </c>
       <c r="B37">
@@ -3221,10 +4395,42 @@
         <f t="shared" si="0"/>
         <v>1.0638963063177336E+27</v>
       </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D37">
+        <f t="shared" si="1"/>
+        <v>3.6555198735758911E+37</v>
+      </c>
+      <c r="E37">
+        <f t="shared" si="2"/>
+        <v>7.392391708206638E-11</v>
+      </c>
+      <c r="G37">
+        <f t="shared" si="3"/>
+        <v>5.3228376030194887E+43</v>
+      </c>
+      <c r="H37">
+        <f t="shared" si="4"/>
+        <v>3.4896240721519513E-17</v>
+      </c>
+      <c r="K37">
+        <f t="shared" si="5"/>
+        <v>5.3228376035649746E+43</v>
+      </c>
+      <c r="L37">
+        <f t="shared" si="6"/>
+        <v>3.3600090202950753E-17</v>
+      </c>
+      <c r="N37">
+        <f t="shared" si="7"/>
+        <v>3.0963457722616542E+51</v>
+      </c>
+      <c r="O37">
+        <f t="shared" si="8"/>
+        <v>5.0085548502619544E-27</v>
+      </c>
+    </row>
+    <row r="38" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A38">
-        <f t="shared" si="1"/>
+        <f t="shared" si="9"/>
         <v>36</v>
       </c>
       <c r="B38">
@@ -3234,10 +4440,42 @@
         <f t="shared" si="0"/>
         <v>1.9606287826087545E+27</v>
       </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D38">
+        <f t="shared" si="1"/>
+        <v>1.347333840144143E+38</v>
+      </c>
+      <c r="E38">
+        <f t="shared" si="2"/>
+        <v>2.7246519927478089E-10</v>
+      </c>
+      <c r="G38">
+        <f t="shared" si="3"/>
+        <v>2.9427986207846041E+44</v>
+      </c>
+      <c r="H38">
+        <f t="shared" si="4"/>
+        <v>1.9292831516708433E-16</v>
+      </c>
+      <c r="K38">
+        <f t="shared" si="5"/>
+        <v>2.942798621896149E+44</v>
+      </c>
+      <c r="L38">
+        <f t="shared" si="6"/>
+        <v>1.8576238185175133E-16</v>
+      </c>
+      <c r="N38">
+        <f t="shared" si="7"/>
+        <v>2.8530903838818696E+52</v>
+      </c>
+      <c r="O38">
+        <f t="shared" si="8"/>
+        <v>4.615072324428929E-26</v>
+      </c>
+    </row>
+    <row r="39" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A39">
-        <f t="shared" si="1"/>
+        <f t="shared" si="9"/>
         <v>37</v>
       </c>
       <c r="B39">
@@ -3247,10 +4485,42 @@
         <f t="shared" si="0"/>
         <v>3.4573771729134435E+27</v>
       </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D39">
+        <f t="shared" si="1"/>
+        <v>4.7517830040320565E+38</v>
+      </c>
+      <c r="E39">
+        <f t="shared" si="2"/>
+        <v>9.6093148151433639E-10</v>
+      </c>
+      <c r="G39">
+        <f t="shared" si="3"/>
+        <v>1.5568012975578395E+45</v>
+      </c>
+      <c r="H39">
+        <f t="shared" si="4"/>
+        <v>1.0206306651988494E-15</v>
+      </c>
+      <c r="K39">
+        <f t="shared" si="5"/>
+        <v>1.5568012996317073E+45</v>
+      </c>
+      <c r="L39">
+        <f t="shared" si="6"/>
+        <v>9.8272139771205041E-16</v>
+      </c>
+      <c r="N39">
+        <f t="shared" si="7"/>
+        <v>2.5155729766363537E+53</v>
+      </c>
+      <c r="O39">
+        <f t="shared" si="8"/>
+        <v>4.0691144206795037E-25</v>
+      </c>
+    </row>
+    <row r="40" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A40">
-        <f t="shared" si="1"/>
+        <f t="shared" si="9"/>
         <v>38</v>
       </c>
       <c r="B40">
@@ -3260,10 +4530,42 @@
         <f t="shared" si="0"/>
         <v>5.8039705192995229E+27</v>
       </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D40">
+        <f t="shared" si="1"/>
+        <v>1.5953832683097336E+39</v>
+      </c>
+      <c r="E40">
+        <f t="shared" si="2"/>
+        <v>3.2262710782441149E-9</v>
+      </c>
+      <c r="G40">
+        <f t="shared" si="3"/>
+        <v>7.840303545319168E+45</v>
+      </c>
+      <c r="H40">
+        <f t="shared" si="4"/>
+        <v>5.1400613780145577E-15</v>
+      </c>
+      <c r="K40">
+        <f t="shared" si="5"/>
+        <v>7.8403035803854069E+45</v>
+      </c>
+      <c r="L40">
+        <f t="shared" si="6"/>
+        <v>4.94914418097279E-15</v>
+      </c>
+      <c r="N40">
+        <f t="shared" si="7"/>
+        <v>2.1114721746196749E+54</v>
+      </c>
+      <c r="O40">
+        <f t="shared" si="8"/>
+        <v>3.4154532404370184E-24</v>
+      </c>
+    </row>
+    <row r="41" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A41">
-        <f t="shared" si="1"/>
+        <f t="shared" si="9"/>
         <v>39</v>
       </c>
       <c r="B41">
@@ -3273,10 +4575,42 @@
         <f t="shared" si="0"/>
         <v>9.1423035226493579E+27</v>
       </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D41">
+        <f t="shared" si="1"/>
+        <v>5.0260345139052272E+39</v>
+      </c>
+      <c r="E41">
+        <f t="shared" si="2"/>
+        <v>1.0163921179672949E-8</v>
+      </c>
+      <c r="G41">
+        <f t="shared" si="3"/>
+        <v>3.7049689251176195E+46</v>
+      </c>
+      <c r="H41">
+        <f t="shared" si="4"/>
+        <v>2.4289579566228312E-14</v>
+      </c>
+      <c r="K41">
+        <f t="shared" si="5"/>
+        <v>3.7049689773213235E+46</v>
+      </c>
+      <c r="L41">
+        <f t="shared" si="6"/>
+        <v>2.3387392422747449E-14</v>
+      </c>
+      <c r="N41">
+        <f t="shared" si="7"/>
+        <v>1.6629753231699139E+55</v>
+      </c>
+      <c r="O41">
+        <f t="shared" si="8"/>
+        <v>2.6899783594403968E-23</v>
+      </c>
+    </row>
+    <row r="42" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A42">
-        <f t="shared" si="1"/>
+        <f t="shared" si="9"/>
         <v>40</v>
       </c>
       <c r="B42">
@@ -3286,10 +4620,42 @@
         <f t="shared" si="0"/>
         <v>1.3959951414227392E+28</v>
       </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D42">
+        <f t="shared" si="1"/>
+        <v>1.5349128903131033E+40</v>
+      </c>
+      <c r="E42">
+        <f t="shared" si="2"/>
+        <v>3.1039845810140704E-8</v>
+      </c>
+      <c r="G42">
+        <f t="shared" si="3"/>
+        <v>1.697204191188653E+47</v>
+      </c>
+      <c r="H42">
+        <f t="shared" si="4"/>
+        <v>1.1126780568261912E-13</v>
+      </c>
+      <c r="K42">
+        <f t="shared" si="5"/>
+        <v>1.6972042642199674E+47</v>
+      </c>
+      <c r="L42">
+        <f t="shared" si="6"/>
+        <v>1.0713499193067664E-13</v>
+      </c>
+      <c r="N42">
+        <f t="shared" si="7"/>
+        <v>1.269650184824731E+56</v>
+      </c>
+      <c r="O42">
+        <f t="shared" si="8"/>
+        <v>2.0537475653744662E-22</v>
+      </c>
+    </row>
+    <row r="43" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A43">
-        <f t="shared" si="1"/>
+        <f t="shared" si="9"/>
         <v>41</v>
       </c>
       <c r="B43">
@@ -3299,10 +4665,42 @@
         <f t="shared" si="0"/>
         <v>2.0320155189386453E+28</v>
       </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D43">
+        <f t="shared" si="1"/>
+        <v>4.4684493817886465E+40</v>
+      </c>
+      <c r="E43">
+        <f t="shared" si="2"/>
+        <v>9.0363421075214929E-8</v>
+      </c>
+      <c r="G43">
+        <f t="shared" si="3"/>
+        <v>7.4113694660604024E+47</v>
+      </c>
+      <c r="H43">
+        <f t="shared" si="4"/>
+        <v>4.8588544729798026E-13</v>
+      </c>
+      <c r="K43">
+        <f t="shared" si="5"/>
+        <v>7.4113703944849453E+47</v>
+      </c>
+      <c r="L43">
+        <f t="shared" si="6"/>
+        <v>4.6783827035299693E-13</v>
+      </c>
+      <c r="N43">
+        <f t="shared" si="7"/>
+        <v>9.240536741975326E+56</v>
+      </c>
+      <c r="O43">
+        <f t="shared" si="8"/>
+        <v>1.4947211494483348E-21</v>
+      </c>
+    </row>
+    <row r="44" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A44">
-        <f t="shared" si="1"/>
+        <f t="shared" si="9"/>
         <v>42</v>
       </c>
       <c r="B44">
@@ -3312,10 +4710,42 @@
         <f t="shared" si="0"/>
         <v>2.795656712509026E+28</v>
       </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D44">
+        <f t="shared" si="1"/>
+        <v>1.22954282506948E+41</v>
+      </c>
+      <c r="E44">
+        <f t="shared" si="2"/>
+        <v>2.4864485762013704E-7</v>
+      </c>
+      <c r="G44">
+        <f t="shared" si="3"/>
+        <v>3.0589793144146472E+48</v>
+      </c>
+      <c r="H44">
+        <f t="shared" si="4"/>
+        <v>2.0054505975799054E-12</v>
+      </c>
+      <c r="K44">
+        <f t="shared" si="5"/>
+        <v>3.0589803688295934E+48</v>
+      </c>
+      <c r="L44">
+        <f t="shared" si="6"/>
+        <v>1.9309628430687343E-12</v>
+      </c>
+      <c r="N44">
+        <f t="shared" si="7"/>
+        <v>6.3565874200072047E+57</v>
+      </c>
+      <c r="O44">
+        <f t="shared" si="8"/>
+        <v>1.0282222689340143E-20</v>
+      </c>
+    </row>
+    <row r="45" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A45">
-        <f t="shared" si="1"/>
+        <f t="shared" si="9"/>
         <v>43</v>
       </c>
       <c r="B45">
@@ -3325,10 +4755,42 @@
         <f t="shared" si="0"/>
         <v>3.7837291145720289E+28</v>
       </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D45">
+        <f t="shared" si="1"/>
+        <v>3.3282033262612277E+41</v>
+      </c>
+      <c r="E45">
+        <f t="shared" si="2"/>
+        <v>6.7304743301017283E-7</v>
+      </c>
+      <c r="G45">
+        <f t="shared" si="3"/>
+        <v>1.2420354445918311E+49</v>
+      </c>
+      <c r="H45">
+        <f t="shared" si="4"/>
+        <v>8.1427184317156711E-12</v>
+      </c>
+      <c r="K45">
+        <f t="shared" si="5"/>
+        <v>1.2420366034634346E+49</v>
+      </c>
+      <c r="L45">
+        <f t="shared" si="6"/>
+        <v>7.8402808839757921E-12</v>
+      </c>
+      <c r="N45">
+        <f t="shared" si="7"/>
+        <v>4.3016019783090413E+58</v>
+      </c>
+      <c r="O45">
+        <f t="shared" si="8"/>
+        <v>6.9581406719377018E-20</v>
+      </c>
+    </row>
+    <row r="46" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A46">
-        <f t="shared" si="1"/>
+        <f t="shared" si="9"/>
         <v>44</v>
       </c>
       <c r="B46">
@@ -3338,10 +4800,42 @@
         <f t="shared" si="0"/>
         <v>4.9278295557501226E+28</v>
       </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D46">
+        <f t="shared" si="1"/>
+        <v>8.6691294339928004E+41</v>
+      </c>
+      <c r="E46">
+        <f t="shared" si="2"/>
+        <v>1.7531186469116051E-6</v>
+      </c>
+      <c r="G46">
+        <f t="shared" si="3"/>
+        <v>4.8527831574231126E+49</v>
+      </c>
+      <c r="H46">
+        <f t="shared" si="4"/>
+        <v>3.1814588732654306E-11</v>
+      </c>
+      <c r="K46">
+        <f t="shared" si="5"/>
+        <v>4.8527949513431574E+49</v>
+      </c>
+      <c r="L46">
+        <f t="shared" si="6"/>
+        <v>3.0632974410556569E-11</v>
+      </c>
+      <c r="N46">
+        <f t="shared" si="7"/>
+        <v>2.8011467951217371E+59</v>
+      </c>
+      <c r="O46">
+        <f t="shared" si="8"/>
+        <v>4.5310499533632634E-19</v>
+      </c>
+    </row>
+    <row r="47" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A47">
-        <f t="shared" si="1"/>
+        <f t="shared" si="9"/>
         <v>45</v>
       </c>
       <c r="B47">
@@ -3351,10 +4845,42 @@
         <f t="shared" si="0"/>
         <v>6.1297365063915331E+28</v>
       </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D47">
+        <f t="shared" si="1"/>
+        <v>2.1567093004737683E+42</v>
+      </c>
+      <c r="E47">
+        <f t="shared" si="2"/>
+        <v>4.361415202549146E-6</v>
+      </c>
+      <c r="G47">
+        <f t="shared" si="3"/>
+        <v>1.8109158448641021E+50</v>
+      </c>
+      <c r="H47">
+        <f t="shared" si="4"/>
+        <v>1.187226813249824E-10</v>
+      </c>
+      <c r="K47">
+        <f t="shared" si="5"/>
+        <v>1.8109267940661847E+50</v>
+      </c>
+      <c r="L47">
+        <f t="shared" si="6"/>
+        <v>1.1431365779563086E-10</v>
+      </c>
+      <c r="N47">
+        <f t="shared" si="7"/>
+        <v>1.7421758986959997E+60</v>
+      </c>
+      <c r="O47">
+        <f t="shared" si="8"/>
+        <v>2.8180908041965164E-18</v>
+      </c>
+    </row>
+    <row r="48" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A48">
-        <f t="shared" si="1"/>
+        <f t="shared" si="9"/>
         <v>46</v>
       </c>
       <c r="B48">
@@ -3364,10 +4890,42 @@
         <f t="shared" si="0"/>
         <v>7.3442580887674299E+28</v>
       </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D48">
+        <f t="shared" si="1"/>
+        <v>5.1680621862321482E+42</v>
+      </c>
+      <c r="E48">
+        <f t="shared" si="2"/>
+        <v>1.0451137286699162E-5</v>
+      </c>
+      <c r="G48">
+        <f t="shared" si="3"/>
+        <v>6.5091704975503079E+50</v>
+      </c>
+      <c r="H48">
+        <f t="shared" si="4"/>
+        <v>4.267377619243456E-10</v>
+      </c>
+      <c r="K48">
+        <f t="shared" si="5"/>
+        <v>6.5092648053913629E+50</v>
+      </c>
+      <c r="L48">
+        <f t="shared" si="6"/>
+        <v>4.1089340104901951E-10</v>
+      </c>
+      <c r="N48">
+        <f t="shared" si="7"/>
+        <v>1.0436818469042109E+61</v>
+      </c>
+      <c r="O48">
+        <f t="shared" si="8"/>
+        <v>1.6882280471616232E-17</v>
+      </c>
+    </row>
+    <row r="49" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A49">
-        <f t="shared" si="1"/>
+        <f t="shared" si="9"/>
         <v>47</v>
       </c>
       <c r="B49">
@@ -3377,10 +4935,42 @@
         <f t="shared" si="0"/>
         <v>8.4956152162922545E+28</v>
       </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D49">
+        <f t="shared" si="1"/>
+        <v>1.1956515475742785E+43</v>
+      </c>
+      <c r="E49">
+        <f t="shared" si="2"/>
+        <v>2.4179117859770632E-5</v>
+      </c>
+      <c r="G49">
+        <f t="shared" si="3"/>
+        <v>2.2588833585112932E+51</v>
+      </c>
+      <c r="H49">
+        <f t="shared" si="4"/>
+        <v>1.480911936815968E-9</v>
+      </c>
+      <c r="K49">
+        <f t="shared" si="5"/>
+        <v>2.2589590761380911E+51</v>
+      </c>
+      <c r="L49">
+        <f t="shared" si="6"/>
+        <v>1.4259542442583493E-9</v>
+      </c>
+      <c r="N49">
+        <f t="shared" si="7"/>
+        <v>6.036497677749434E+61</v>
+      </c>
+      <c r="O49">
+        <f t="shared" si="8"/>
+        <v>9.7644552470001211E-17</v>
+      </c>
+    </row>
+    <row r="50" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A50">
-        <f t="shared" si="1"/>
+        <f t="shared" si="9"/>
         <v>48</v>
       </c>
       <c r="B50">
@@ -3390,10 +4980,42 @@
         <f t="shared" si="0"/>
         <v>9.2794812951238229E+28</v>
       </c>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D50">
+        <f t="shared" si="1"/>
+        <v>2.611941781431946E+43</v>
+      </c>
+      <c r="E50">
+        <f t="shared" si="2"/>
+        <v>5.2820111598758987E-5</v>
+      </c>
+      <c r="G50">
+        <f t="shared" si="3"/>
+        <v>7.4019121651039771E+51</v>
+      </c>
+      <c r="H50">
+        <f t="shared" si="4"/>
+        <v>4.8526543166841448E-9</v>
+      </c>
+      <c r="K50">
+        <f t="shared" si="5"/>
+        <v>7.4024541842141894E+51</v>
+      </c>
+      <c r="L50">
+        <f t="shared" si="6"/>
+        <v>4.6727543997627226E-9</v>
+      </c>
+      <c r="N50">
+        <f t="shared" si="7"/>
+        <v>3.2967340129359796E+62</v>
+      </c>
+      <c r="O50">
+        <f t="shared" si="8"/>
+        <v>5.3326967803254555E-16</v>
+      </c>
+    </row>
+    <row r="51" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A51">
-        <f t="shared" si="1"/>
+        <f t="shared" si="9"/>
         <v>49</v>
       </c>
       <c r="B51">
@@ -3403,10 +5025,42 @@
         <f t="shared" si="0"/>
         <v>9.7729288489031328E+28</v>
       </c>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D51">
+        <f t="shared" si="1"/>
+        <v>5.5016698402798149E+43</v>
+      </c>
+      <c r="E51">
+        <f t="shared" si="2"/>
+        <v>1.1125776884038788E-4</v>
+      </c>
+      <c r="G51">
+        <f t="shared" si="3"/>
+        <v>2.3386553181610708E+52</v>
+      </c>
+      <c r="H51">
+        <f t="shared" si="4"/>
+        <v>1.5332100100314056E-8</v>
+      </c>
+      <c r="K51">
+        <f t="shared" si="5"/>
+        <v>2.3390160508620951E+52</v>
+      </c>
+      <c r="L51">
+        <f t="shared" si="6"/>
+        <v>1.4764897250008071E-8</v>
+      </c>
+      <c r="N51">
+        <f t="shared" si="7"/>
+        <v>1.7360209001721099E+63</v>
+      </c>
+      <c r="O51">
+        <f t="shared" si="8"/>
+        <v>2.8081346655810072E-15</v>
+      </c>
+    </row>
+    <row r="52" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A52">
-        <f t="shared" si="1"/>
+        <f t="shared" si="9"/>
         <v>50</v>
       </c>
       <c r="B52">
@@ -3416,10 +5070,42 @@
         <f t="shared" si="0"/>
         <v>9.8068014435835635E+28</v>
       </c>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D52">
+        <f t="shared" si="1"/>
+        <v>1.1041476831754845E+44</v>
+      </c>
+      <c r="E52">
+        <f t="shared" si="2"/>
+        <v>2.232867679572353E-4</v>
+      </c>
+      <c r="G52">
+        <f t="shared" si="3"/>
+        <v>7.040283022042195E+52</v>
+      </c>
+      <c r="H52">
+        <f t="shared" si="4"/>
+        <v>4.615572170479983E-8</v>
+      </c>
+      <c r="K52">
+        <f t="shared" si="5"/>
+        <v>7.04246261692778E+52</v>
+      </c>
+      <c r="L52">
+        <f t="shared" si="6"/>
+        <v>4.4455119017946496E-8</v>
+      </c>
+      <c r="N52">
+        <f t="shared" si="7"/>
+        <v>8.7101894084749563E+63</v>
+      </c>
+      <c r="O52">
+        <f t="shared" si="8"/>
+        <v>1.4089337760444092E-14</v>
+      </c>
+    </row>
+    <row r="53" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A53">
-        <f t="shared" si="1"/>
+        <f t="shared" si="9"/>
         <v>51</v>
       </c>
       <c r="B53">
@@ -3429,10 +5115,42 @@
         <f t="shared" si="0"/>
         <v>9.4626558197722141E+28</v>
       </c>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D53">
+        <f t="shared" si="1"/>
+        <v>2.1308006611930699E+44</v>
+      </c>
+      <c r="E53">
+        <f t="shared" si="2"/>
+        <v>4.3090213387996933E-4</v>
+      </c>
+      <c r="G53">
+        <f t="shared" si="3"/>
+        <v>2.0379664713705209E+53</v>
+      </c>
+      <c r="H53">
+        <f t="shared" si="4"/>
+        <v>1.3360799985141124E-7</v>
+      </c>
+      <c r="K53">
+        <f t="shared" si="5"/>
+        <v>2.039184228994206E+53</v>
+      </c>
+      <c r="L53">
+        <f t="shared" si="6"/>
+        <v>1.2872227022058824E-7</v>
+      </c>
+      <c r="N53">
+        <f t="shared" si="7"/>
+        <v>4.2022633460857393E+64</v>
+      </c>
+      <c r="O53">
+        <f t="shared" si="8"/>
+        <v>6.7974535184881087E-14</v>
+      </c>
+    </row>
+    <row r="54" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A54">
-        <f t="shared" si="1"/>
+        <f t="shared" si="9"/>
         <v>52</v>
       </c>
       <c r="B54">
@@ -3442,10 +5160,42 @@
         <f t="shared" si="0"/>
         <v>8.9486231904590015E+28</v>
       </c>
-    </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D54">
+        <f t="shared" si="1"/>
+        <v>4.0301016066030138E+44</v>
+      </c>
+      <c r="E54">
+        <f t="shared" si="2"/>
+        <v>8.1498913233206546E-4</v>
+      </c>
+      <c r="G54">
+        <f t="shared" si="3"/>
+        <v>5.7817787229388466E+53</v>
+      </c>
+      <c r="H54">
+        <f t="shared" si="4"/>
+        <v>3.7905034337282777E-7</v>
+      </c>
+      <c r="K54">
+        <f t="shared" si="5"/>
+        <v>5.7883147538902132E+53</v>
+      </c>
+      <c r="L54">
+        <f t="shared" si="6"/>
+        <v>3.6538386540953916E-7</v>
+      </c>
+      <c r="N54">
+        <f t="shared" si="7"/>
+        <v>1.9869935009484422E+65</v>
+      </c>
+      <c r="O54">
+        <f t="shared" si="8"/>
+        <v>3.2141003197278961E-13</v>
+      </c>
+    </row>
+    <row r="55" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A55">
-        <f t="shared" si="1"/>
+        <f t="shared" si="9"/>
         <v>53</v>
       </c>
       <c r="B55">
@@ -3455,10 +5205,42 @@
         <f t="shared" si="0"/>
         <v>7.983927540532119E+28</v>
       </c>
-    </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D55">
+        <f t="shared" si="1"/>
+        <v>7.1912826192986983E+44</v>
+      </c>
+      <c r="E55">
+        <f t="shared" si="2"/>
+        <v>1.454260401934881E-3</v>
+      </c>
+      <c r="G55">
+        <f t="shared" si="3"/>
+        <v>1.5475442891109039E+54</v>
+      </c>
+      <c r="H55">
+        <f t="shared" si="4"/>
+        <v>1.0145618196090053E-6</v>
+      </c>
+      <c r="K55">
+        <f t="shared" si="5"/>
+        <v>1.5506673364841704E+54</v>
+      </c>
+      <c r="L55">
+        <f t="shared" si="6"/>
+        <v>9.7884937060153379E-7</v>
+      </c>
+      <c r="N55">
+        <f t="shared" si="7"/>
+        <v>8.8639401824376558E+65</v>
+      </c>
+      <c r="O55">
+        <f t="shared" si="8"/>
+        <v>1.4338040341260811E-12</v>
+      </c>
+    </row>
+    <row r="56" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A56">
-        <f t="shared" si="1"/>
+        <f t="shared" si="9"/>
         <v>54</v>
       </c>
       <c r="B56">
@@ -3468,10 +5250,42 @@
         <f t="shared" si="0"/>
         <v>7.0449425189183648E+28</v>
       </c>
-    </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D56">
+        <f t="shared" si="1"/>
+        <v>1.2691040201218924E+45</v>
+      </c>
+      <c r="E56">
+        <f t="shared" si="2"/>
+        <v>2.566451383021326E-3</v>
+      </c>
+      <c r="G56">
+        <f t="shared" si="3"/>
+        <v>4.096615546766375E+54</v>
+      </c>
+      <c r="H56">
+        <f t="shared" si="4"/>
+        <v>2.6857194024176824E-6</v>
+      </c>
+      <c r="K56">
+        <f t="shared" si="5"/>
+        <v>4.1112166783625312E+54</v>
+      </c>
+      <c r="L56">
+        <f t="shared" si="6"/>
+        <v>2.5951806447061077E-6</v>
+      </c>
+      <c r="N56">
+        <f t="shared" si="7"/>
+        <v>3.9107286958319582E+66</v>
+      </c>
+      <c r="O56">
+        <f t="shared" si="8"/>
+        <v>6.3258759254334885E-12</v>
+      </c>
+    </row>
+    <row r="57" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A57">
-        <f t="shared" si="1"/>
+        <f t="shared" si="9"/>
         <v>55</v>
       </c>
       <c r="B57">
@@ -3481,10 +5295,42 @@
         <f t="shared" si="0"/>
         <v>5.8640513752982505E+28</v>
       </c>
-    </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D57">
+        <f t="shared" si="1"/>
+        <v>2.1127471670939716E+45</v>
+      </c>
+      <c r="E57">
+        <f t="shared" si="2"/>
+        <v>4.2725125781588212E-3</v>
+      </c>
+      <c r="G57">
+        <f t="shared" si="3"/>
+        <v>1.0229791357377258E+55</v>
+      </c>
+      <c r="H57">
+        <f t="shared" si="4"/>
+        <v>6.7065969011613606E-6</v>
+      </c>
+      <c r="K57">
+        <f t="shared" si="5"/>
+        <v>1.029056179614869E+55</v>
+      </c>
+      <c r="L57">
+        <f t="shared" si="6"/>
+        <v>6.4958548492642217E-6</v>
+      </c>
+      <c r="N57">
+        <f t="shared" si="7"/>
+        <v>1.6276012136102332E+67</v>
+      </c>
+      <c r="O57">
+        <f t="shared" si="8"/>
+        <v>2.632758274527392E-11</v>
+      </c>
+    </row>
+    <row r="58" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A58">
-        <f t="shared" si="1"/>
+        <f t="shared" si="9"/>
         <v>56</v>
       </c>
       <c r="B58">
@@ -3494,10 +5340,42 @@
         <f t="shared" si="0"/>
         <v>4.804154520574811E+28</v>
       </c>
-    </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D58">
+        <f t="shared" si="1"/>
+        <v>3.4617581613905605E+45</v>
+      </c>
+      <c r="E58">
+        <f t="shared" si="2"/>
+        <v>7.0005562035276277E-3</v>
+      </c>
+      <c r="G58">
+        <f t="shared" si="3"/>
+        <v>2.5142428970405214E+55</v>
+      </c>
+      <c r="H58">
+        <f t="shared" si="4"/>
+        <v>1.6483242945027229E-5</v>
+      </c>
+      <c r="K58">
+        <f t="shared" si="5"/>
+        <v>2.5387619853015839E+55</v>
+      </c>
+      <c r="L58">
+        <f t="shared" si="6"/>
+        <v>1.6025781371354267E-5</v>
+      </c>
+      <c r="N58">
+        <f t="shared" si="7"/>
+        <v>6.6671037032489824E+67</v>
+      </c>
+      <c r="O58">
+        <f t="shared" si="8"/>
+        <v>1.0784504395229836E-10</v>
+      </c>
+    </row>
+    <row r="59" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A59">
-        <f t="shared" si="1"/>
+        <f t="shared" si="9"/>
         <v>57</v>
       </c>
       <c r="B59">
@@ -3507,10 +5385,42 @@
         <f t="shared" si="0"/>
         <v>3.7018043039237399E+28</v>
       </c>
-    </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D59">
+        <f t="shared" si="1"/>
+        <v>5.334862234799825E+45</v>
+      </c>
+      <c r="E59">
+        <f t="shared" si="2"/>
+        <v>1.0788449444368809E-2</v>
+      </c>
+      <c r="G59">
+        <f t="shared" si="3"/>
+        <v>5.8119915611669557E+55</v>
+      </c>
+      <c r="H59">
+        <f t="shared" si="4"/>
+        <v>3.8103108100624783E-5</v>
+      </c>
+      <c r="K59">
+        <f t="shared" si="5"/>
+        <v>5.899568781562091E+55</v>
+      </c>
+      <c r="L59">
+        <f t="shared" si="6"/>
+        <v>3.7240670856882147E-5</v>
+      </c>
+      <c r="N59">
+        <f t="shared" si="7"/>
+        <v>2.5686427317953986E+68</v>
+      </c>
+      <c r="O59">
+        <f t="shared" si="8"/>
+        <v>4.1549584442976734E-10</v>
+      </c>
+    </row>
+    <row r="60" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A60">
-        <f t="shared" si="1"/>
+        <f t="shared" si="9"/>
         <v>58</v>
       </c>
       <c r="B60">
@@ -3520,10 +5430,42 @@
         <f t="shared" si="0"/>
         <v>2.713929387601292E+28</v>
       </c>
-    </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D60">
+        <f t="shared" si="1"/>
+        <v>7.8223688823750508E+45</v>
+      </c>
+      <c r="E60">
+        <f t="shared" si="2"/>
+        <v>1.5818821088240061E-2</v>
+      </c>
+      <c r="G60">
+        <f t="shared" si="3"/>
+        <v>1.2782956690840772E+56</v>
+      </c>
+      <c r="H60">
+        <f t="shared" si="4"/>
+        <v>8.3804385383332328E-5</v>
+      </c>
+      <c r="K60">
+        <f t="shared" si="5"/>
+        <v>1.3066377367312975E+56</v>
+      </c>
+      <c r="L60">
+        <f t="shared" si="6"/>
+        <v>8.2480716276872419E-5</v>
+      </c>
+      <c r="N60">
+        <f t="shared" si="7"/>
+        <v>9.4158340416306426E+68</v>
+      </c>
+      <c r="O60">
+        <f t="shared" si="8"/>
+        <v>1.5230767080649409E-9</v>
+      </c>
+    </row>
+    <row r="61" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A61">
-        <f t="shared" si="1"/>
+        <f t="shared" si="9"/>
         <v>59</v>
       </c>
       <c r="B61">
@@ -3533,10 +5475,42 @@
         <f t="shared" si="0"/>
         <v>1.9349746124482949E+28</v>
       </c>
-    </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D61">
+        <f t="shared" si="1"/>
+        <v>1.1154369207799694E+46</v>
+      </c>
+      <c r="E61">
+        <f t="shared" si="2"/>
+        <v>2.2556973917188042E-2</v>
+      </c>
+      <c r="G61">
+        <f t="shared" si="3"/>
+        <v>2.7341938351606935E+56</v>
+      </c>
+      <c r="H61">
+        <f t="shared" si="4"/>
+        <v>1.792522961755158E-4</v>
+      </c>
+      <c r="K61">
+        <f t="shared" si="5"/>
+        <v>2.8210445933792797E+56</v>
+      </c>
+      <c r="L61">
+        <f t="shared" si="6"/>
+        <v>1.7807673249434932E-4</v>
+      </c>
+      <c r="N61">
+        <f t="shared" si="7"/>
+        <v>3.3566458856331817E+69</v>
+      </c>
+      <c r="O61">
+        <f t="shared" si="8"/>
+        <v>5.4296084054010573E-9</v>
+      </c>
+    </row>
+    <row r="62" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A62">
-        <f t="shared" si="1"/>
+        <f t="shared" si="9"/>
         <v>60</v>
       </c>
       <c r="B62">
@@ -3546,10 +5520,42 @@
         <f t="shared" si="0"/>
         <v>1.3403233985887997E+28</v>
       </c>
-    </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D62">
+        <f t="shared" si="1"/>
+        <v>1.5452876693607616E+46</v>
+      </c>
+      <c r="E62">
+        <f t="shared" si="2"/>
+        <v>3.1249650251803776E-2</v>
+      </c>
+      <c r="G62">
+        <f t="shared" si="3"/>
+        <v>5.6817861329553501E+56</v>
+      </c>
+      <c r="H62">
+        <f t="shared" si="4"/>
+        <v>3.7249488226228614E-4</v>
+      </c>
+      <c r="K62">
+        <f t="shared" si="5"/>
+        <v>5.9333374192021171E+56</v>
+      </c>
+      <c r="L62">
+        <f t="shared" si="6"/>
+        <v>3.7453833338107519E-4</v>
+      </c>
+      <c r="N62">
+        <f t="shared" si="7"/>
+        <v>1.1625452324665049E+70</v>
+      </c>
+      <c r="O62">
+        <f t="shared" si="8"/>
+        <v>1.8804978484253677E-8</v>
+      </c>
+    </row>
+    <row r="63" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A63">
-        <f t="shared" si="1"/>
+        <f t="shared" si="9"/>
         <v>61</v>
       </c>
       <c r="B63">
@@ -3559,10 +5565,42 @@
         <f t="shared" si="0"/>
         <v>8.6586912380763998E+27</v>
       </c>
-    </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D63">
+        <f t="shared" si="1"/>
+        <v>1.9965582660258331E+46</v>
+      </c>
+      <c r="E63">
+        <f t="shared" si="2"/>
+        <v>4.0375490439566279E-2</v>
+      </c>
+      <c r="G63">
+        <f t="shared" si="3"/>
+        <v>1.1011558521885732E+57</v>
+      </c>
+      <c r="H63">
+        <f t="shared" si="4"/>
+        <v>7.2191193035993362E-4</v>
+      </c>
+      <c r="K63">
+        <f t="shared" si="5"/>
+        <v>1.1645476374383808E+57</v>
+      </c>
+      <c r="L63">
+        <f t="shared" si="6"/>
+        <v>7.3511364760322898E-4</v>
+      </c>
+      <c r="N63">
+        <f t="shared" si="7"/>
+        <v>3.7551087404814534E+70</v>
+      </c>
+      <c r="O63">
+        <f t="shared" si="8"/>
+        <v>6.0741498135919798E-8</v>
+      </c>
+    </row>
+    <row r="64" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A64">
-        <f t="shared" si="1"/>
+        <f t="shared" si="9"/>
         <v>62</v>
       </c>
       <c r="B64">
@@ -3572,10 +5610,42 @@
         <f t="shared" si="0"/>
         <v>5.4999594452600973E+27</v>
       </c>
-    </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D64">
+        <f t="shared" si="1"/>
+        <v>2.5364086075623643E+46</v>
+      </c>
+      <c r="E64">
+        <f t="shared" si="2"/>
+        <v>5.1292638551096913E-2</v>
+      </c>
+      <c r="G64">
+        <f t="shared" si="3"/>
+        <v>2.0983468621616198E+57</v>
+      </c>
+      <c r="H64">
+        <f t="shared" si="4"/>
+        <v>1.3756650621408956E-3</v>
+      </c>
+      <c r="K64">
+        <f t="shared" si="5"/>
+        <v>2.2529861674421864E+57</v>
+      </c>
+      <c r="L64">
+        <f t="shared" si="6"/>
+        <v>1.4221838817956287E-3</v>
+      </c>
+      <c r="N64">
+        <f t="shared" si="7"/>
+        <v>1.1926135958266336E+71</v>
+      </c>
+      <c r="O64">
+        <f t="shared" si="8"/>
+        <v>1.9291355194813397E-7</v>
+      </c>
+    </row>
+    <row r="65" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A65">
-        <f t="shared" si="1"/>
+        <f t="shared" si="9"/>
         <v>63</v>
       </c>
       <c r="B65">
@@ -3585,10 +5655,42 @@
         <f t="shared" si="0"/>
         <v>3.3229859086390569E+27</v>
       </c>
-    </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D65">
+        <f t="shared" si="1"/>
+        <v>3.0649135308603936E+46</v>
+      </c>
+      <c r="E65">
+        <f t="shared" si="2"/>
+        <v>6.1980353425733679E-2</v>
+      </c>
+      <c r="G65">
+        <f t="shared" si="3"/>
+        <v>3.8033609831846477E+57</v>
+      </c>
+      <c r="H65">
+        <f t="shared" si="4"/>
+        <v>2.4934632675014689E-3</v>
+      </c>
+      <c r="K65">
+        <f t="shared" si="5"/>
+        <v>4.1446077811293614E+57</v>
+      </c>
+      <c r="L65">
+        <f t="shared" si="6"/>
+        <v>2.6162585762250041E-3</v>
+      </c>
+      <c r="N65">
+        <f t="shared" si="7"/>
+        <v>3.6027885412851837E+71</v>
+      </c>
+      <c r="O65">
+        <f t="shared" si="8"/>
+        <v>5.8277612870547454E-7</v>
+      </c>
+    </row>
+    <row r="66" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A66">
-        <f t="shared" si="1"/>
+        <f t="shared" si="9"/>
         <v>64</v>
       </c>
       <c r="B66">
@@ -3598,477 +5700,1662 @@
         <f t="shared" si="0"/>
         <v>1.9092610538670513E+27</v>
       </c>
-    </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D66">
+        <f t="shared" si="1"/>
+        <v>3.5219650030586482E+46</v>
+      </c>
+      <c r="E66">
+        <f t="shared" si="2"/>
+        <v>7.1223097632173757E-2</v>
+      </c>
+      <c r="G66">
+        <f t="shared" si="3"/>
+        <v>6.5557987893779251E+57</v>
+      </c>
+      <c r="H66">
+        <f t="shared" si="4"/>
+        <v>4.2979468798034015E-3</v>
+      </c>
+      <c r="K66">
+        <f t="shared" si="5"/>
+        <v>7.236127213193198E+57</v>
+      </c>
+      <c r="L66">
+        <f t="shared" si="6"/>
+        <v>4.5677615060147354E-3</v>
+      </c>
+      <c r="N66">
+        <f t="shared" si="7"/>
+        <v>1.0350124912223106E+72</v>
+      </c>
+      <c r="O66">
+        <f t="shared" si="8"/>
+        <v>1.6742047607967053E-6</v>
+      </c>
+    </row>
+    <row r="67" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A67">
-        <f t="shared" si="1"/>
+        <f t="shared" si="9"/>
         <v>65</v>
       </c>
       <c r="B67">
         <v>62.208283296825201</v>
       </c>
       <c r="C67">
-        <f t="shared" ref="C67:C102" si="2">EXP(B67)</f>
+        <f t="shared" ref="C67:C102" si="10">EXP(B67)</f>
         <v>1.0392359565385312E+27</v>
       </c>
-    </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D67">
+        <f t="shared" ref="D67:D102" si="11">C67*(2/1)^A67</f>
+        <v>3.8341039444926055E+46</v>
+      </c>
+      <c r="E67">
+        <f t="shared" ref="E67:E102" si="12">D67/SUM(D:D)</f>
+        <v>7.7535341587252005E-2</v>
+      </c>
+      <c r="G67">
+        <f t="shared" ref="G67:G102" si="13">C67*(3/1)^A67</f>
+        <v>1.0705223068297702E+58</v>
+      </c>
+      <c r="H67">
+        <f t="shared" ref="H67:H102" si="14">G67/SUM(G:G)</f>
+        <v>7.0182874066449805E-3</v>
+      </c>
+      <c r="K67">
+        <f t="shared" ref="K67:K102" si="15">G67*(4/1)^E67</f>
+        <v>1.1920010785035343E+58</v>
+      </c>
+      <c r="L67">
+        <f t="shared" ref="L67:L102" si="16">K67/SUM(K:K)</f>
+        <v>7.5244346611117573E-3</v>
+      </c>
+      <c r="N67">
+        <f t="shared" ref="N67:N102" si="17">C67*(5)^A67</f>
+        <v>2.8168547045103178E+72</v>
+      </c>
+      <c r="O67">
+        <f t="shared" ref="O67:O102" si="18">N67/SUM(N:N)</f>
+        <v>4.5564585903638348E-6</v>
+      </c>
+    </row>
+    <row r="68" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A68">
-        <f t="shared" si="1"/>
+        <f t="shared" si="9"/>
         <v>66</v>
       </c>
       <c r="B68">
         <v>61.575294912925301</v>
       </c>
       <c r="C68">
-        <f t="shared" si="2"/>
+        <f t="shared" si="10"/>
         <v>5.5183698248072935E+26</v>
       </c>
-    </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D68">
+        <f t="shared" si="11"/>
+        <v>4.0718382344920623E+46</v>
+      </c>
+      <c r="E68">
+        <f t="shared" si="12"/>
+        <v>8.2342934090994122E-2</v>
+      </c>
+      <c r="G68">
+        <f t="shared" si="13"/>
+        <v>1.7053503463648105E+58</v>
+      </c>
+      <c r="H68">
+        <f t="shared" si="14"/>
+        <v>1.1180186329095343E-2</v>
+      </c>
+      <c r="K68">
+        <f t="shared" si="15"/>
+        <v>1.9115646908804191E+58</v>
+      </c>
+      <c r="L68">
+        <f t="shared" si="16"/>
+        <v>1.2066636412003347E-2</v>
+      </c>
+      <c r="N68">
+        <f t="shared" si="17"/>
+        <v>7.4787856907931505E+72</v>
+      </c>
+      <c r="O68">
+        <f t="shared" si="18"/>
+        <v>1.2097456518343386E-5</v>
+      </c>
+    </row>
+    <row r="69" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A69">
-        <f t="shared" ref="A69:A102" si="3">A68+1</f>
+        <f t="shared" ref="A69:A102" si="19">A68+1</f>
         <v>67</v>
       </c>
       <c r="B69">
         <v>60.896020527712103</v>
       </c>
       <c r="C69">
-        <f t="shared" si="2"/>
+        <f t="shared" si="10"/>
         <v>2.7977292607783441E+26</v>
       </c>
-    </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D69">
+        <f t="shared" si="11"/>
+        <v>4.1287196528885378E+46</v>
+      </c>
+      <c r="E69">
+        <f t="shared" si="12"/>
+        <v>8.34932211643723E-2</v>
+      </c>
+      <c r="G69">
+        <f t="shared" si="13"/>
+        <v>2.5937597779992533E+58</v>
+      </c>
+      <c r="H69">
+        <f t="shared" si="14"/>
+        <v>1.7004551394825929E-2</v>
+      </c>
+      <c r="K69">
+        <f t="shared" si="15"/>
+        <v>2.9120423005383503E+58</v>
+      </c>
+      <c r="L69">
+        <f t="shared" si="16"/>
+        <v>1.8382090768158155E-2</v>
+      </c>
+      <c r="N69">
+        <f t="shared" si="17"/>
+        <v>1.8958150891013409E+73</v>
+      </c>
+      <c r="O69">
+        <f t="shared" si="18"/>
+        <v>3.0666128908409034E-5</v>
+      </c>
+    </row>
+    <row r="70" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A70">
-        <f t="shared" si="3"/>
+        <f t="shared" si="19"/>
         <v>68</v>
       </c>
       <c r="B70">
         <v>60.181164454213601</v>
       </c>
       <c r="C70">
-        <f t="shared" si="2"/>
+        <f t="shared" si="10"/>
         <v>1.3688240811989158E+26</v>
       </c>
-    </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D70">
+        <f t="shared" si="11"/>
+        <v>4.0400556012491237E+46</v>
+      </c>
+      <c r="E70">
+        <f t="shared" si="12"/>
+        <v>8.1700208343150657E-2</v>
+      </c>
+      <c r="G70">
+        <f t="shared" si="13"/>
+        <v>3.8070883713559802E+58</v>
+      </c>
+      <c r="H70">
+        <f t="shared" si="14"/>
+        <v>2.4959069233968803E-2</v>
+      </c>
+      <c r="K70">
+        <f t="shared" si="15"/>
+        <v>4.2636484104086035E+58</v>
+      </c>
+      <c r="L70">
+        <f t="shared" si="16"/>
+        <v>2.6914022529533659E-2</v>
+      </c>
+      <c r="N70">
+        <f t="shared" si="17"/>
+        <v>4.6377563830823108E+73</v>
+      </c>
+      <c r="O70">
+        <f t="shared" si="18"/>
+        <v>7.5018938242977809E-5</v>
+      </c>
+    </row>
+    <row r="71" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A71">
-        <f t="shared" si="3"/>
+        <f t="shared" si="19"/>
         <v>69</v>
       </c>
       <c r="B71">
         <v>59.4248952297974</v>
       </c>
       <c r="C71">
-        <f t="shared" si="2"/>
+        <f t="shared" si="10"/>
         <v>6.4254579528298695E+25</v>
       </c>
-    </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D71">
+        <f t="shared" si="11"/>
+        <v>3.7929209091914977E+46</v>
+      </c>
+      <c r="E71">
+        <f t="shared" si="12"/>
+        <v>7.6702515780779565E-2</v>
+      </c>
+      <c r="G71">
+        <f t="shared" si="13"/>
+        <v>5.3613068155762304E+58</v>
+      </c>
+      <c r="H71">
+        <f t="shared" si="14"/>
+        <v>3.5148442836606744E-2</v>
+      </c>
+      <c r="K71">
+        <f t="shared" si="15"/>
+        <v>5.962799105215054E+58</v>
+      </c>
+      <c r="L71">
+        <f t="shared" si="16"/>
+        <v>3.763980844786903E-2</v>
+      </c>
+      <c r="N71">
+        <f t="shared" si="17"/>
+        <v>1.0885149174488136E+74</v>
+      </c>
+      <c r="O71">
+        <f t="shared" si="18"/>
+        <v>1.7607486599884939E-4</v>
+      </c>
+    </row>
+    <row r="72" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A72">
-        <f t="shared" si="3"/>
+        <f t="shared" si="19"/>
         <v>70</v>
       </c>
       <c r="B72">
         <v>58.601871602189199</v>
       </c>
       <c r="C72">
-        <f t="shared" si="2"/>
+        <f t="shared" si="10"/>
         <v>2.8214312095959801E+25</v>
       </c>
-    </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D72">
+        <f t="shared" si="11"/>
+        <v>3.3309580444796044E+46</v>
+      </c>
+      <c r="E72">
+        <f t="shared" si="12"/>
+        <v>6.7360450715612877E-2</v>
+      </c>
+      <c r="G72">
+        <f t="shared" si="13"/>
+        <v>7.0624810642599185E+58</v>
+      </c>
+      <c r="H72">
+        <f t="shared" si="14"/>
+        <v>4.6301250891024992E-2</v>
+      </c>
+      <c r="K72">
+        <f t="shared" si="15"/>
+        <v>7.7537595447681156E+58</v>
+      </c>
+      <c r="L72">
+        <f t="shared" si="16"/>
+        <v>4.8945137823049663E-2</v>
+      </c>
+      <c r="N72">
+        <f t="shared" si="17"/>
+        <v>2.3898451929393492E+74</v>
+      </c>
+      <c r="O72">
+        <f t="shared" si="18"/>
+        <v>3.8657409775422544E-4</v>
+      </c>
+    </row>
+    <row r="73" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A73">
-        <f t="shared" si="3"/>
+        <f t="shared" si="19"/>
         <v>71</v>
       </c>
       <c r="B73">
         <v>57.746054608202897</v>
       </c>
       <c r="C73">
-        <f t="shared" si="2"/>
+        <f t="shared" si="10"/>
         <v>1.1989273515613513E+25</v>
       </c>
-    </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D73">
+        <f t="shared" si="11"/>
+        <v>2.8308871702044985E+46</v>
+      </c>
+      <c r="E73">
+        <f t="shared" si="12"/>
+        <v>5.7247744691966668E-2</v>
+      </c>
+      <c r="G73">
+        <f t="shared" si="13"/>
+        <v>9.0033048004432923E+58</v>
+      </c>
+      <c r="H73">
+        <f t="shared" si="14"/>
+        <v>5.9025188261850305E-2</v>
+      </c>
+      <c r="K73">
+        <f t="shared" si="15"/>
+        <v>9.7469453222346193E+58</v>
+      </c>
+      <c r="L73">
+        <f t="shared" si="16"/>
+        <v>6.1527002403937686E-2</v>
+      </c>
+      <c r="N73">
+        <f t="shared" si="17"/>
+        <v>5.0776548406840209E+74</v>
+      </c>
+      <c r="O73">
+        <f t="shared" si="18"/>
+        <v>8.2134602046360079E-4</v>
+      </c>
+    </row>
+    <row r="74" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A74">
-        <f t="shared" si="3"/>
+        <f t="shared" si="19"/>
         <v>72</v>
       </c>
       <c r="B74">
         <v>56.834756439823501</v>
       </c>
       <c r="C74">
-        <f t="shared" si="2"/>
+        <f t="shared" si="10"/>
         <v>4.8197121577318454E+24</v>
       </c>
-    </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D74">
+        <f t="shared" si="11"/>
+        <v>2.2760447150752203E+46</v>
+      </c>
+      <c r="E74">
+        <f t="shared" si="12"/>
+        <v>4.6027417880704052E-2</v>
+      </c>
+      <c r="G74">
+        <f t="shared" si="13"/>
+        <v>1.0858040118098389E+59</v>
+      </c>
+      <c r="H74">
+        <f t="shared" si="14"/>
+        <v>7.1184734531471727E-2</v>
+      </c>
+      <c r="K74">
+        <f t="shared" si="15"/>
+        <v>1.157344650967121E+59</v>
+      </c>
+      <c r="L74">
+        <f t="shared" si="16"/>
+        <v>7.305668059899724E-2</v>
+      </c>
+      <c r="N74">
+        <f t="shared" si="17"/>
+        <v>1.0206137484702471E+75</v>
+      </c>
+      <c r="O74">
+        <f t="shared" si="18"/>
+        <v>1.6509137919732055E-3</v>
+      </c>
+    </row>
+    <row r="75" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A75">
-        <f t="shared" si="3"/>
+        <f t="shared" si="19"/>
         <v>73</v>
       </c>
       <c r="B75">
         <v>55.867584188291303</v>
       </c>
       <c r="C75">
-        <f t="shared" si="2"/>
+        <f t="shared" si="10"/>
         <v>1.8322449367863726E+24</v>
       </c>
-    </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D75">
+        <f t="shared" si="11"/>
+        <v>1.7305064155775156E+46</v>
+      </c>
+      <c r="E75">
+        <f t="shared" si="12"/>
+        <v>3.4995244780326409E-2</v>
+      </c>
+      <c r="G75">
+        <f t="shared" si="13"/>
+        <v>1.2383263800034567E+59</v>
+      </c>
+      <c r="H75">
+        <f t="shared" si="14"/>
+        <v>8.1184020011985811E-2</v>
+      </c>
+      <c r="K75">
+        <f t="shared" si="15"/>
+        <v>1.2998832918268133E+59</v>
+      </c>
+      <c r="L75">
+        <f t="shared" si="16"/>
+        <v>8.205434603046563E-2</v>
+      </c>
+      <c r="N75">
+        <f t="shared" si="17"/>
+        <v>1.9399647861224133E+75</v>
+      </c>
+      <c r="O75">
+        <f t="shared" si="18"/>
+        <v>3.1380280994178743E-3</v>
+      </c>
+    </row>
+    <row r="76" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A76">
-        <f t="shared" si="3"/>
+        <f t="shared" si="19"/>
         <v>74</v>
       </c>
       <c r="B76">
         <v>54.854339431282398</v>
       </c>
       <c r="C76">
-        <f t="shared" si="2"/>
+        <f t="shared" si="10"/>
         <v>6.6517653953389543E+23</v>
       </c>
-    </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D76">
+        <f t="shared" si="11"/>
+        <v>1.2564829581944333E+46</v>
+      </c>
+      <c r="E76">
+        <f t="shared" si="12"/>
+        <v>2.5409283830738399E-2</v>
+      </c>
+      <c r="G76">
+        <f t="shared" si="13"/>
+        <v>1.3486826565485663E+59</v>
+      </c>
+      <c r="H76">
+        <f t="shared" si="14"/>
+        <v>8.8418918911144687E-2</v>
+      </c>
+      <c r="K76">
+        <f t="shared" si="15"/>
+        <v>1.3970362843242172E+59</v>
+      </c>
+      <c r="L76">
+        <f t="shared" si="16"/>
+        <v>8.818706987913813E-2</v>
+      </c>
+      <c r="N76">
+        <f t="shared" si="17"/>
+        <v>3.521415279536326E+75</v>
+      </c>
+      <c r="O76">
+        <f t="shared" si="18"/>
+        <v>5.6961343710736599E-3</v>
+      </c>
+    </row>
+    <row r="77" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A77">
-        <f t="shared" si="3"/>
+        <f t="shared" si="19"/>
         <v>75</v>
       </c>
       <c r="B77">
         <v>53.7883395192775</v>
       </c>
       <c r="C77">
-        <f t="shared" si="2"/>
+        <f t="shared" si="10"/>
         <v>2.2907571140526035E+23</v>
       </c>
-    </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D77">
+        <f t="shared" si="11"/>
+        <v>8.6542356926377696E+45</v>
+      </c>
+      <c r="E77">
+        <f t="shared" si="12"/>
+        <v>1.7501067532848472E-2</v>
+      </c>
+      <c r="G77">
+        <f t="shared" si="13"/>
+        <v>1.3933914711962989E+59</v>
+      </c>
+      <c r="H77">
+        <f t="shared" si="14"/>
+        <v>9.1350005062328488E-2</v>
+      </c>
+      <c r="K77">
+        <f t="shared" si="15"/>
+        <v>1.4276108517107007E+59</v>
+      </c>
+      <c r="L77">
+        <f t="shared" si="16"/>
+        <v>9.0117070939876864E-2</v>
+      </c>
+      <c r="N77">
+        <f t="shared" si="17"/>
+        <v>6.0635835929991636E+75</v>
+      </c>
+      <c r="O77">
+        <f t="shared" si="18"/>
+        <v>9.8082686006033034E-3</v>
+      </c>
+    </row>
+    <row r="78" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A78">
-        <f t="shared" si="3"/>
+        <f t="shared" si="19"/>
         <v>76</v>
       </c>
       <c r="B78">
         <v>52.665878574276199</v>
       </c>
       <c r="C78">
-        <f t="shared" si="2"/>
+        <f t="shared" si="10"/>
         <v>7.4559064354213004E+22</v>
       </c>
-    </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D78">
+        <f t="shared" si="11"/>
+        <v>5.6335236240073024E+45</v>
+      </c>
+      <c r="E78">
+        <f t="shared" si="12"/>
+        <v>1.1392418798522286E-2</v>
+      </c>
+      <c r="G78">
+        <f t="shared" si="13"/>
+        <v>1.3605540770895198E+59</v>
+      </c>
+      <c r="H78">
+        <f t="shared" si="14"/>
+        <v>8.9197202938950657E-2</v>
+      </c>
+      <c r="K78">
+        <f t="shared" si="15"/>
+        <v>1.3822122182439294E+59</v>
+      </c>
+      <c r="L78">
+        <f t="shared" si="16"/>
+        <v>8.7251309680219838E-2</v>
+      </c>
+      <c r="N78">
+        <f t="shared" si="17"/>
+        <v>9.8678100038237665E+75</v>
+      </c>
+      <c r="O78">
+        <f t="shared" si="18"/>
+        <v>1.5961869665484657E-2</v>
+      </c>
+    </row>
+    <row r="79" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A79">
-        <f t="shared" si="3"/>
+        <f t="shared" si="19"/>
         <v>77</v>
       </c>
       <c r="B79">
         <v>51.508698307164401</v>
       </c>
       <c r="C79">
-        <f t="shared" si="2"/>
+        <f t="shared" si="10"/>
         <v>2.3439235624233343E+22</v>
       </c>
-    </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D79">
+        <f t="shared" si="11"/>
+        <v>3.5420371422708386E+45</v>
+      </c>
+      <c r="E79">
+        <f t="shared" si="12"/>
+        <v>7.1629007381292468E-3</v>
+      </c>
+      <c r="G79">
+        <f t="shared" si="13"/>
+        <v>1.2831577703648023E+59</v>
+      </c>
+      <c r="H79">
+        <f t="shared" si="14"/>
+        <v>8.4123142161875303E-2</v>
+      </c>
+      <c r="K79">
+        <f t="shared" si="15"/>
+        <v>1.2959628557889475E+59</v>
+      </c>
+      <c r="L79">
+        <f t="shared" si="16"/>
+        <v>8.1806870878454674E-2</v>
+      </c>
+      <c r="N79">
+        <f t="shared" si="17"/>
+        <v>1.5510785025142469E+76</v>
+      </c>
+      <c r="O79">
+        <f t="shared" si="18"/>
+        <v>2.5089774619164517E-2</v>
+      </c>
+    </row>
+    <row r="80" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A80">
-        <f t="shared" si="3"/>
+        <f t="shared" si="19"/>
         <v>78</v>
       </c>
       <c r="B80">
         <v>50.2743823984855</v>
       </c>
       <c r="C80">
-        <f t="shared" si="2"/>
+        <f t="shared" si="10"/>
         <v>6.8216095309063153E+21</v>
       </c>
-    </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D80">
+        <f t="shared" si="11"/>
+        <v>2.0617049733104708E+45</v>
+      </c>
+      <c r="E80">
+        <f t="shared" si="12"/>
+        <v>4.1692922693810381E-3</v>
+      </c>
+      <c r="G80">
+        <f t="shared" si="13"/>
+        <v>1.1203267994277864E+59</v>
+      </c>
+      <c r="H80">
+        <f t="shared" si="14"/>
+        <v>7.3448030158620642E-2</v>
+      </c>
+      <c r="K80">
+        <f t="shared" si="15"/>
+        <v>1.1268208880144354E+59</v>
+      </c>
+      <c r="L80">
+        <f t="shared" si="16"/>
+        <v>7.1129886537392162E-2</v>
+      </c>
+      <c r="N80">
+        <f t="shared" si="17"/>
+        <v>2.2570812601490635E+76</v>
+      </c>
+      <c r="O80">
+        <f t="shared" si="18"/>
+        <v>3.6509860733989305E-2</v>
+      </c>
+    </row>
+    <row r="81" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A81">
-        <f t="shared" si="3"/>
+        <f t="shared" si="19"/>
         <v>79</v>
       </c>
       <c r="B81">
         <v>49.015719479861801</v>
       </c>
       <c r="C81">
-        <f t="shared" si="2"/>
+        <f t="shared" si="10"/>
         <v>1.9375659628094475E+21</v>
       </c>
-    </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D81">
+        <f t="shared" si="11"/>
+        <v>1.1711867598234097E+45</v>
+      </c>
+      <c r="E81">
+        <f t="shared" si="12"/>
+        <v>2.3684377575577775E-3</v>
+      </c>
+      <c r="G81">
+        <f t="shared" si="13"/>
+        <v>9.5463118958648185E+58</v>
+      </c>
+      <c r="H81">
+        <f t="shared" si="14"/>
+        <v>6.2585113949715276E-2</v>
+      </c>
+      <c r="K81">
+        <f t="shared" si="15"/>
+        <v>9.5777073101342262E+58</v>
+      </c>
+      <c r="L81">
+        <f t="shared" si="16"/>
+        <v>6.0458697695837484E-2</v>
+      </c>
+      <c r="N81">
+        <f t="shared" si="17"/>
+        <v>3.2054339999572318E+76</v>
+      </c>
+      <c r="O81">
+        <f t="shared" si="18"/>
+        <v>5.1850126531423089E-2</v>
+      </c>
+    </row>
+    <row r="82" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A82">
-        <f t="shared" si="3"/>
+        <f t="shared" si="19"/>
         <v>80</v>
       </c>
       <c r="B82">
         <v>47.678460587848299</v>
       </c>
       <c r="C82">
-        <f t="shared" si="2"/>
+        <f t="shared" si="10"/>
         <v>5.0873584534673641E+20</v>
       </c>
-    </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D82">
+        <f t="shared" si="11"/>
+        <v>6.1502389880314454E+44</v>
+      </c>
+      <c r="E82">
+        <f t="shared" si="12"/>
+        <v>1.243734879606556E-3</v>
+      </c>
+      <c r="G82">
+        <f t="shared" si="13"/>
+        <v>7.5195649781818835E+58</v>
+      </c>
+      <c r="H82">
+        <f t="shared" si="14"/>
+        <v>4.9297868762873447E-2</v>
+      </c>
+      <c r="K82">
+        <f t="shared" si="15"/>
+        <v>7.5325412651850621E+58</v>
+      </c>
+      <c r="L82">
+        <f t="shared" si="16"/>
+        <v>4.7548710822617801E-2</v>
+      </c>
+      <c r="N82">
+        <f t="shared" si="17"/>
+        <v>4.2081642818159584E+76</v>
+      </c>
+      <c r="O82">
+        <f t="shared" si="18"/>
+        <v>6.8069986928473283E-2</v>
+      </c>
+    </row>
+    <row r="83" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A83">
-        <f t="shared" si="3"/>
+        <f t="shared" si="19"/>
         <v>81</v>
       </c>
       <c r="B83">
         <v>46.274610002273597</v>
       </c>
       <c r="C83">
-        <f t="shared" si="2"/>
+        <f t="shared" si="10"/>
         <v>1.2497057734812249E+20</v>
       </c>
-    </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D83">
+        <f t="shared" si="11"/>
+        <v>3.0216031529658479E+44</v>
+      </c>
+      <c r="E83">
+        <f t="shared" si="12"/>
+        <v>6.1104507336805865E-4</v>
+      </c>
+      <c r="G83">
+        <f t="shared" si="13"/>
+        <v>5.5415264247182871E+58</v>
+      </c>
+      <c r="H83">
+        <f t="shared" si="14"/>
+        <v>3.6329953025794524E-2</v>
+      </c>
+      <c r="K83">
+        <f t="shared" si="15"/>
+        <v>5.5462225758828844E+58</v>
+      </c>
+      <c r="L83">
+        <f t="shared" si="16"/>
+        <v>3.5010194320130368E-2</v>
+      </c>
+      <c r="N83">
+        <f t="shared" si="17"/>
+        <v>5.1686619360962751E+76</v>
+      </c>
+      <c r="O83">
+        <f t="shared" si="18"/>
+        <v>8.3606705172628054E-2</v>
+      </c>
+    </row>
+    <row r="84" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A84">
-        <f t="shared" si="3"/>
+        <f t="shared" si="19"/>
         <v>82</v>
       </c>
       <c r="B84">
         <v>44.805943897744498</v>
       </c>
       <c r="C84">
-        <f t="shared" si="2"/>
+        <f t="shared" si="10"/>
         <v>2.8772274251596464E+19</v>
       </c>
-    </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D84">
+        <f t="shared" si="11"/>
+        <v>1.3913418092715259E+44</v>
+      </c>
+      <c r="E84">
+        <f t="shared" si="12"/>
+        <v>2.8136473086873834E-4</v>
+      </c>
+      <c r="G84">
+        <f t="shared" si="13"/>
+        <v>3.8275165590452993E+58</v>
+      </c>
+      <c r="H84">
+        <f t="shared" si="14"/>
+        <v>2.509299534787212E-2</v>
+      </c>
+      <c r="K84">
+        <f t="shared" si="15"/>
+        <v>3.8290097896915073E+58</v>
+      </c>
+      <c r="L84">
+        <f t="shared" si="16"/>
+        <v>2.4170392543152043E-2</v>
+      </c>
+      <c r="N84">
+        <f t="shared" si="17"/>
+        <v>5.9499668599948185E+76</v>
+      </c>
+      <c r="O84">
+        <f t="shared" si="18"/>
+        <v>9.6244856251172753E-2</v>
+      </c>
+    </row>
+    <row r="85" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A85">
-        <f t="shared" si="3"/>
+        <f t="shared" si="19"/>
         <v>83</v>
       </c>
       <c r="B85">
         <v>43.280780965470498</v>
       </c>
       <c r="C85">
-        <f t="shared" si="2"/>
+        <f t="shared" si="10"/>
         <v>6.2604326214233836E+18</v>
       </c>
-    </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D85">
+        <f t="shared" si="11"/>
+        <v>6.0547189103971404E+43</v>
+      </c>
+      <c r="E85">
+        <f t="shared" si="12"/>
+        <v>1.2244182884159206E-4</v>
+      </c>
+      <c r="G85">
+        <f t="shared" si="13"/>
+        <v>2.4984374869799335E+58</v>
+      </c>
+      <c r="H85">
+        <f t="shared" si="14"/>
+        <v>1.6379623515822075E-2</v>
+      </c>
+      <c r="K85">
+        <f t="shared" si="15"/>
+        <v>2.4988616087948311E+58</v>
+      </c>
+      <c r="L85">
+        <f t="shared" si="16"/>
+        <v>1.5773912659661712E-2</v>
+      </c>
+      <c r="N85">
+        <f t="shared" si="17"/>
+        <v>6.4731356132949402E+76</v>
+      </c>
+      <c r="O85">
+        <f t="shared" si="18"/>
+        <v>0.10470747505919067</v>
+      </c>
+    </row>
+    <row r="86" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A86">
-        <f t="shared" si="3"/>
+        <f t="shared" si="19"/>
         <v>84</v>
       </c>
       <c r="B86">
         <v>41.696149769648599</v>
       </c>
       <c r="C86">
-        <f t="shared" si="2"/>
+        <f t="shared" si="10"/>
         <v>1.2835351355575992E+18</v>
       </c>
-    </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D86">
+        <f t="shared" si="11"/>
+        <v>2.4827180252130317E+43</v>
+      </c>
+      <c r="E86">
+        <f t="shared" si="12"/>
+        <v>5.0206878304963339E-5</v>
+      </c>
+      <c r="G86">
+        <f t="shared" si="13"/>
+        <v>1.5367143897815157E+58</v>
+      </c>
+      <c r="H86">
+        <f t="shared" si="14"/>
+        <v>1.0074617951075296E-2</v>
+      </c>
+      <c r="K86">
+        <f t="shared" si="15"/>
+        <v>1.5368213511492859E+58</v>
+      </c>
+      <c r="L86">
+        <f t="shared" si="16"/>
+        <v>9.7010917616296467E-3</v>
+      </c>
+      <c r="N86">
+        <f t="shared" si="17"/>
+        <v>6.6357211228991787E+76</v>
+      </c>
+      <c r="O86">
+        <f t="shared" si="18"/>
+        <v>0.1073374088669896</v>
+      </c>
+    </row>
+    <row r="87" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A87">
-        <f t="shared" si="3"/>
+        <f t="shared" si="19"/>
         <v>85</v>
       </c>
       <c r="B87">
         <v>40.025455722904702</v>
       </c>
       <c r="C87">
-        <f t="shared" si="2"/>
+        <f t="shared" si="10"/>
         <v>2.4145408432414432E+17</v>
       </c>
-    </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D87">
+        <f t="shared" si="11"/>
+        <v>9.3408024573077107E+42</v>
+      </c>
+      <c r="E87">
+        <f t="shared" si="12"/>
+        <v>1.888948029869442E-5</v>
+      </c>
+      <c r="G87">
+        <f t="shared" si="13"/>
+        <v>8.6724380713872845E+57</v>
+      </c>
+      <c r="H87">
+        <f t="shared" si="14"/>
+        <v>5.6856043552770599E-3</v>
+      </c>
+      <c r="K87">
+        <f t="shared" si="15"/>
+        <v>8.6726651741198296E+57</v>
+      </c>
+      <c r="L87">
+        <f t="shared" si="16"/>
+        <v>5.4745673990739254E-3</v>
+      </c>
+      <c r="N87">
+        <f t="shared" si="17"/>
+        <v>6.2414417929586288E+76</v>
+      </c>
+      <c r="O87">
+        <f t="shared" si="18"/>
+        <v>0.10095966621297926</v>
+      </c>
+    </row>
+    <row r="88" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A88">
-        <f t="shared" si="3"/>
+        <f t="shared" si="19"/>
         <v>86</v>
       </c>
       <c r="B88">
         <v>38.275686343515602</v>
       </c>
       <c r="C88">
-        <f t="shared" si="2"/>
+        <f t="shared" si="10"/>
         <v>4.1968105989495216E+16</v>
       </c>
-    </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D88">
+        <f t="shared" si="11"/>
+        <v>3.2471249235855444E+42</v>
+      </c>
+      <c r="E88">
+        <f t="shared" si="12"/>
+        <v>6.5665131611345219E-6</v>
+      </c>
+      <c r="G88">
+        <f t="shared" si="13"/>
+        <v>4.5221740752834312E+57</v>
+      </c>
+      <c r="H88">
+        <f t="shared" si="14"/>
+        <v>2.964713314307886E-3</v>
+      </c>
+      <c r="K88">
+        <f t="shared" si="15"/>
+        <v>4.5222152413648259E+57</v>
+      </c>
+      <c r="L88">
+        <f t="shared" si="16"/>
+        <v>2.8546209999953851E-3</v>
+      </c>
+      <c r="N88">
+        <f t="shared" si="17"/>
+        <v>5.4242505656376636E+76</v>
+      </c>
+      <c r="O88">
+        <f t="shared" si="18"/>
+        <v>8.7741029192991857E-2</v>
+      </c>
+    </row>
+    <row r="89" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A89">
-        <f t="shared" si="3"/>
+        <f t="shared" si="19"/>
         <v>87</v>
       </c>
       <c r="B89">
         <v>36.448647304976298</v>
       </c>
       <c r="C89">
-        <f t="shared" si="2"/>
+        <f t="shared" si="10"/>
         <v>6752217099006399</v>
       </c>
-    </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D89">
+        <f t="shared" si="11"/>
+        <v>1.0448549876009248E+42</v>
+      </c>
+      <c r="E89">
+        <f t="shared" si="12"/>
+        <v>2.112962755982421E-6</v>
+      </c>
+      <c r="G89">
+        <f t="shared" si="13"/>
+        <v>2.1827075868128427E+57</v>
+      </c>
+      <c r="H89">
+        <f t="shared" si="14"/>
+        <v>1.4309715053282836E-3</v>
+      </c>
+      <c r="K89">
+        <f t="shared" si="15"/>
+        <v>2.1827139803838499E+57</v>
+      </c>
+      <c r="L89">
+        <f t="shared" si="16"/>
+        <v>1.3778249890438125E-3</v>
+      </c>
+      <c r="N89">
+        <f t="shared" si="17"/>
+        <v>4.3635180281618294E+76</v>
+      </c>
+      <c r="O89">
+        <f t="shared" si="18"/>
+        <v>7.0582941930907125E-2</v>
+      </c>
+    </row>
+    <row r="90" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A90">
-        <f t="shared" si="3"/>
+        <f t="shared" si="19"/>
         <v>88</v>
       </c>
       <c r="B90">
         <v>34.536563985290599</v>
       </c>
       <c r="C90">
-        <f t="shared" si="2"/>
+        <f t="shared" si="10"/>
         <v>997790035954207</v>
       </c>
-    </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D90">
+        <f t="shared" si="11"/>
+        <v>3.08801059076928E+41</v>
+      </c>
+      <c r="E90">
+        <f t="shared" si="12"/>
+        <v>6.2447434771368331E-7</v>
+      </c>
+      <c r="G90">
+        <f t="shared" si="13"/>
+        <v>9.676305647121387E+56</v>
+      </c>
+      <c r="H90">
+        <f t="shared" si="14"/>
+        <v>6.3437346081232735E-4</v>
+      </c>
+      <c r="K90">
+        <f t="shared" si="15"/>
+        <v>9.6763140239537765E+56</v>
+      </c>
+      <c r="L90">
+        <f t="shared" si="16"/>
+        <v>6.1081146608562989E-4</v>
+      </c>
+      <c r="N90">
+        <f t="shared" si="17"/>
+        <v>3.2240334888277676E+76</v>
+      </c>
+      <c r="O90">
+        <f t="shared" si="18"/>
+        <v>5.2150986212630049E-2</v>
+      </c>
+    </row>
+    <row r="91" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A91">
-        <f t="shared" si="3"/>
+        <f t="shared" si="19"/>
         <v>89</v>
       </c>
       <c r="B91">
         <v>32.527897785480498</v>
       </c>
       <c r="C91">
-        <f t="shared" si="2"/>
+        <f t="shared" si="10"/>
         <v>133871002657141.98</v>
       </c>
-    </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D91">
+        <f t="shared" si="11"/>
+        <v>8.2862137144277798E+40</v>
+      </c>
+      <c r="E91">
+        <f t="shared" si="12"/>
+        <v>1.6756833411780479E-7</v>
+      </c>
+      <c r="G91">
+        <f t="shared" si="13"/>
+        <v>3.8947374467163624E+56</v>
+      </c>
+      <c r="H91">
+        <f t="shared" si="14"/>
+        <v>2.5533691918504475E-4</v>
+      </c>
+      <c r="K91">
+        <f t="shared" si="15"/>
+        <v>3.894738351460225E+56</v>
+      </c>
+      <c r="L91">
+        <f t="shared" si="16"/>
+        <v>2.4585300111036509E-4</v>
+      </c>
+      <c r="N91">
+        <f t="shared" si="17"/>
+        <v>2.1628026949418502E+76</v>
+      </c>
+      <c r="O91">
+        <f t="shared" si="18"/>
+        <v>3.4984839306232487E-2</v>
+      </c>
+    </row>
+    <row r="92" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A92">
-        <f t="shared" si="3"/>
+        <f t="shared" si="19"/>
         <v>90</v>
       </c>
       <c r="B92">
         <v>30.424322291069501</v>
       </c>
       <c r="C92">
-        <f t="shared" si="2"/>
+        <f t="shared" si="10"/>
         <v>16334855110628.742</v>
       </c>
-    </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D92">
+        <f t="shared" si="11"/>
+        <v>2.022157117737274E+40</v>
+      </c>
+      <c r="E92">
+        <f t="shared" si="12"/>
+        <v>4.089316438383662E-8</v>
+      </c>
+      <c r="G92">
+        <f t="shared" si="13"/>
+        <v>1.4257002029555903E+56</v>
+      </c>
+      <c r="H92">
+        <f t="shared" si="14"/>
+        <v>9.3468148362886179E-5</v>
+      </c>
+      <c r="K92">
+        <f t="shared" si="15"/>
+        <v>1.4257002837784846E+56</v>
+      </c>
+      <c r="L92">
+        <f t="shared" si="16"/>
+        <v>8.9996467495544213E-5</v>
+      </c>
+      <c r="N92">
+        <f t="shared" si="17"/>
+        <v>1.3195190875366055E+76</v>
+      </c>
+      <c r="O92">
+        <f t="shared" si="18"/>
+        <v>2.1344139873200878E-2</v>
+      </c>
+    </row>
+    <row r="93" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A93">
-        <f t="shared" si="3"/>
+        <f t="shared" si="19"/>
         <v>91</v>
       </c>
       <c r="B93">
         <v>28.1961126957228</v>
       </c>
       <c r="C93">
-        <f t="shared" si="2"/>
+        <f t="shared" si="10"/>
         <v>1759608919966.0981</v>
       </c>
-    </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D93">
+        <f t="shared" si="11"/>
+        <v>4.3565806710194742E+39</v>
+      </c>
+      <c r="E93">
+        <f t="shared" si="12"/>
+        <v>8.8101150978215465E-9</v>
+      </c>
+      <c r="G93">
+        <f t="shared" si="13"/>
+        <v>4.6073407642638817E+55</v>
+      </c>
+      <c r="H93">
+        <f t="shared" si="14"/>
+        <v>3.0205481434304328E-5</v>
+      </c>
+      <c r="K93">
+        <f t="shared" si="15"/>
+        <v>4.6073408205352372E+55</v>
+      </c>
+      <c r="L93">
+        <f t="shared" si="16"/>
+        <v>2.9083560066164513E-5</v>
+      </c>
+      <c r="N93">
+        <f t="shared" si="17"/>
+        <v>7.1070038294498482E+75</v>
+      </c>
+      <c r="O93">
+        <f t="shared" si="18"/>
+        <v>1.1496073474643364E-2</v>
+      </c>
+    </row>
+    <row r="94" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A94">
-        <f t="shared" si="3"/>
+        <f t="shared" si="19"/>
         <v>92</v>
       </c>
       <c r="B94">
         <v>25.881421051795499</v>
       </c>
       <c r="C94">
-        <f t="shared" si="2"/>
+        <f t="shared" si="10"/>
         <v>173843455782.48331</v>
       </c>
-    </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D94">
+        <f t="shared" si="11"/>
+        <v>8.6083109792349461E+38</v>
+      </c>
+      <c r="E94">
+        <f t="shared" si="12"/>
+        <v>1.7408196072070802E-9</v>
+      </c>
+      <c r="G94">
+        <f t="shared" si="13"/>
+        <v>1.3655694137579834E+55</v>
+      </c>
+      <c r="H94">
+        <f t="shared" si="14"/>
+        <v>8.9526005748156955E-6</v>
+      </c>
+      <c r="K94">
+        <f t="shared" si="15"/>
+        <v>1.3655694170534965E+55</v>
+      </c>
+      <c r="L94">
+        <f t="shared" si="16"/>
+        <v>8.6200742928279478E-6</v>
+      </c>
+      <c r="N94">
+        <f t="shared" si="17"/>
+        <v>3.5107406309201601E+75</v>
+      </c>
+      <c r="O94">
+        <f t="shared" si="18"/>
+        <v>5.6788673837816399E-3</v>
+      </c>
+    </row>
+    <row r="95" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A95">
-        <f t="shared" si="3"/>
+        <f t="shared" si="19"/>
         <v>93</v>
       </c>
       <c r="B95">
         <v>23.467580098290099</v>
       </c>
       <c r="C95">
-        <f t="shared" si="2"/>
+        <f t="shared" si="10"/>
         <v>15553944333.436964</v>
       </c>
-    </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D95">
+        <f t="shared" si="11"/>
+        <v>1.5403880367342059E+38</v>
+      </c>
+      <c r="E95">
+        <f t="shared" si="12"/>
+        <v>3.1150567207929144E-10</v>
+      </c>
+      <c r="G95">
+        <f t="shared" si="13"/>
+        <v>3.6653650060221579E+54</v>
+      </c>
+      <c r="H95">
+        <f t="shared" si="14"/>
+        <v>2.4029938375317877E-6</v>
+      </c>
+      <c r="K95">
+        <f t="shared" si="15"/>
+        <v>3.6653650076050038E+54</v>
+      </c>
+      <c r="L95">
+        <f t="shared" si="16"/>
+        <v>2.3137394760979217E-6</v>
+      </c>
+      <c r="N95">
+        <f t="shared" si="17"/>
+        <v>1.5705470216489359E+75</v>
+      </c>
+      <c r="O95">
+        <f t="shared" si="18"/>
+        <v>2.5404691469901896E-3</v>
+      </c>
+    </row>
+    <row r="96" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A96">
-        <f t="shared" si="3"/>
+        <f t="shared" si="19"/>
         <v>94</v>
       </c>
       <c r="B96">
         <v>20.866650523199699</v>
       </c>
       <c r="C96">
-        <f t="shared" si="2"/>
+        <f t="shared" si="10"/>
         <v>1154173711.0381618</v>
       </c>
-    </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D96">
+        <f t="shared" si="11"/>
+        <v>2.2860765586955762E+37</v>
+      </c>
+      <c r="E96">
+        <f t="shared" si="12"/>
+        <v>4.6230287295074378E-11</v>
+      </c>
+      <c r="G96">
+        <f t="shared" si="13"/>
+        <v>8.1596047419603939E+53</v>
+      </c>
+      <c r="H96">
+        <f t="shared" si="14"/>
+        <v>5.349393547275943E-7</v>
+      </c>
+      <c r="K96">
+        <f t="shared" si="15"/>
+        <v>8.159604742483333E+53</v>
+      </c>
+      <c r="L96">
+        <f t="shared" si="16"/>
+        <v>5.1507011069479852E-7</v>
+      </c>
+      <c r="N96">
+        <f t="shared" si="17"/>
+        <v>5.8270881182198971E+74</v>
+      </c>
+      <c r="O96">
+        <f t="shared" si="18"/>
+        <v>9.4257207056356468E-4</v>
+      </c>
+    </row>
+    <row r="97" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A97">
-        <f t="shared" si="3"/>
+        <f t="shared" si="19"/>
         <v>95</v>
       </c>
       <c r="B97">
         <v>18.114732919158101</v>
       </c>
       <c r="C97">
-        <f t="shared" si="2"/>
+        <f t="shared" si="10"/>
         <v>73642504.158180341</v>
       </c>
-    </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D97">
+        <f t="shared" si="11"/>
+        <v>2.9172801437008497E+36</v>
+      </c>
+      <c r="E97">
+        <f t="shared" si="12"/>
+        <v>5.899483053203626E-12</v>
+      </c>
+      <c r="G97">
+        <f t="shared" si="13"/>
+        <v>1.5618802968534905E+53</v>
+      </c>
+      <c r="H97">
+        <f t="shared" si="14"/>
+        <v>1.0239604301712942E-7</v>
+      </c>
+      <c r="K97">
+        <f t="shared" si="15"/>
+        <v>1.561880296866264E+53</v>
+      </c>
+      <c r="L97">
+        <f t="shared" si="16"/>
+        <v>9.8592748397527492E-8</v>
+      </c>
+      <c r="N97">
+        <f t="shared" si="17"/>
+        <v>1.858998159774857E+74</v>
+      </c>
+      <c r="O97">
+        <f t="shared" si="18"/>
+        <v>3.0070589445078288E-4</v>
+      </c>
+    </row>
+    <row r="98" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A98">
-        <f t="shared" si="3"/>
+        <f t="shared" si="19"/>
         <v>96</v>
       </c>
       <c r="B98">
         <v>15.160365786311999</v>
       </c>
       <c r="C98">
-        <f t="shared" si="2"/>
+        <f t="shared" si="10"/>
         <v>3837630.9202127336</v>
       </c>
-    </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D98">
+        <f t="shared" si="11"/>
+        <v>3.0404844621638025E+35</v>
+      </c>
+      <c r="E98">
+        <f t="shared" si="12"/>
+        <v>6.1486335471742273E-13</v>
+      </c>
+      <c r="G98">
+        <f t="shared" si="13"/>
+        <v>2.4417638384490688E+52</v>
+      </c>
+      <c r="H98">
+        <f t="shared" si="14"/>
+        <v>1.6008074085011347E-8</v>
+      </c>
+      <c r="K98">
+        <f t="shared" si="15"/>
+        <v>2.4417638384511503E+52</v>
+      </c>
+      <c r="L98">
+        <f t="shared" si="16"/>
+        <v>1.5413486440261345E-8</v>
+      </c>
+      <c r="N98">
+        <f t="shared" si="17"/>
+        <v>4.8437712025970594E+73</v>
+      </c>
+      <c r="O98">
+        <f t="shared" si="18"/>
+        <v>7.8351371373508818E-5</v>
+      </c>
+    </row>
+    <row r="99" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A99">
-        <f t="shared" si="3"/>
+        <f t="shared" si="19"/>
         <v>97</v>
       </c>
       <c r="B99">
         <v>11.9793326504101</v>
       </c>
       <c r="C99">
-        <f t="shared" si="2"/>
+        <f t="shared" si="10"/>
         <v>159425.60250434367</v>
       </c>
-    </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D99">
+        <f t="shared" si="11"/>
+        <v>2.5261995088297295E+34</v>
+      </c>
+      <c r="E99">
+        <f t="shared" si="12"/>
+        <v>5.1086184587147959E-14</v>
+      </c>
+      <c r="G99">
+        <f t="shared" si="13"/>
+        <v>3.0431248799961399E+51</v>
+      </c>
+      <c r="H99">
+        <f t="shared" si="14"/>
+        <v>1.995056514550622E-9</v>
+      </c>
+      <c r="K99">
+        <f t="shared" si="15"/>
+        <v>3.0431248799963552E+51</v>
+      </c>
+      <c r="L99">
+        <f t="shared" si="16"/>
+        <v>1.9209541617095309E-9</v>
+      </c>
+      <c r="N99">
+        <f t="shared" si="17"/>
+        <v>1.0061170008558543E+73</v>
+      </c>
+      <c r="O99">
+        <f t="shared" si="18"/>
+        <v>1.6274642934619149E-5</v>
+      </c>
+    </row>
+    <row r="100" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A100">
-        <f t="shared" si="3"/>
+        <f t="shared" si="19"/>
         <v>98</v>
       </c>
       <c r="B100">
         <v>8.5122313337400506</v>
       </c>
       <c r="C100">
-        <f t="shared" si="2"/>
+        <f t="shared" si="10"/>
         <v>4975.2521600233076</v>
       </c>
-    </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D100">
+        <f t="shared" si="11"/>
+        <v>1.5767203467350852E+33</v>
+      </c>
+      <c r="E100">
+        <f t="shared" si="12"/>
+        <v>3.1885299001160408E-15</v>
+      </c>
+      <c r="G100">
+        <f t="shared" si="13"/>
+        <v>2.8490368036104402E+50</v>
+      </c>
+      <c r="H100">
+        <f t="shared" si="14"/>
+        <v>1.8678134021383637E-10</v>
+      </c>
+      <c r="K100">
+        <f t="shared" si="15"/>
+        <v>2.8490368036104526E+50</v>
+      </c>
+      <c r="L100">
+        <f t="shared" si="16"/>
+        <v>1.7984372382265405E-10</v>
+      </c>
+      <c r="N100">
+        <f t="shared" si="17"/>
+        <v>1.5699127690635128E+72</v>
+      </c>
+      <c r="O100">
+        <f t="shared" si="18"/>
+        <v>2.539443199277415E-6</v>
+      </c>
+    </row>
+    <row r="101" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A101">
-        <f t="shared" si="3"/>
+        <f t="shared" si="19"/>
         <v>99</v>
       </c>
       <c r="B101">
         <v>4.5925281691556501</v>
       </c>
       <c r="C101">
-        <f t="shared" si="2"/>
+        <f t="shared" si="10"/>
         <v>98.743755778151453</v>
       </c>
-    </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D101">
+        <f t="shared" si="11"/>
+        <v>6.2586290640481692E+31</v>
+      </c>
+      <c r="E101">
+        <f t="shared" si="12"/>
+        <v>1.2656541120798871E-16</v>
+      </c>
+      <c r="G101">
+        <f t="shared" si="13"/>
+        <v>1.6963437346903636E+49</v>
+      </c>
+      <c r="H101">
+        <f t="shared" si="14"/>
+        <v>1.1121139461143095E-11</v>
+      </c>
+      <c r="K101">
+        <f t="shared" si="15"/>
+        <v>1.6963437346903639E+49</v>
+      </c>
+      <c r="L101">
+        <f t="shared" si="16"/>
+        <v>1.0708067152496368E-11</v>
+      </c>
+      <c r="N101">
+        <f t="shared" si="17"/>
+        <v>1.5579017713615016E+71</v>
+      </c>
+      <c r="O101">
+        <f t="shared" si="18"/>
+        <v>2.5200145743041283E-7</v>
+      </c>
+    </row>
+    <row r="102" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A102">
-        <f t="shared" si="3"/>
+        <f t="shared" si="19"/>
         <v>100</v>
       </c>
       <c r="B102">
         <v>-4.2275663371143801E-2</v>
       </c>
       <c r="C102">
-        <f t="shared" si="2"/>
+        <f t="shared" si="10"/>
         <v>0.95860549172533494</v>
+      </c>
+      <c r="D102">
+        <f t="shared" si="11"/>
+        <v>1.2151768269676978E+30</v>
+      </c>
+      <c r="E102">
+        <f t="shared" si="12"/>
+        <v>2.4573968711305289E-18</v>
+      </c>
+      <c r="G102">
+        <f t="shared" si="13"/>
+        <v>4.940437216854938E+47</v>
+      </c>
+      <c r="H102">
+        <f t="shared" si="14"/>
+        <v>3.2389244092497741E-13</v>
+      </c>
+      <c r="K102">
+        <f t="shared" si="15"/>
+        <v>4.940437216854938E+47</v>
+      </c>
+      <c r="L102">
+        <f t="shared" si="16"/>
+        <v>3.1186210906972411E-13</v>
+      </c>
+      <c r="N102">
+        <f t="shared" si="17"/>
+        <v>7.5620639595228107E+69</v>
+      </c>
+      <c r="O102">
+        <f t="shared" si="18"/>
+        <v>1.2232164915740069E-8</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>